<commit_message>
added aux nb for metrics, fixed eq problem
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,30 +494,50 @@
           <t>Most representative docs Non-optimized Thetas</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Avg Cosine Similarity between Top Docs Optimized and Most representative docs Optimized S3</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Avg Cosine Similarity between Top Docs Optimized and Most representative docs Optimized Thetas</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Avg Cosine Similarity between Top Docs Non-optimized and Most representative docs Non-optimized S3</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Avg Cosine Similarity between Top Docs Non-optimized and Most representative docs Non-optimized Thetas</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['presente', 'suministro', 'service', 'técnicas', 'regir', 'materiales', 'prescripción', 'característica', 'ayuntamiento', 'vehículo', 'mantenimiento', 'técnicas_particulares', 'regular', 'especificación', 'adquisición']</t>
+          <t>['reparación', 'edificio', 'cubierto', 'sustitución', 'instalación', 'fachada', 'zona', 'exterior', 'colocación', 'interior', 'centro', 'pintura', 'acceso', 'revestimiento', 'planta']</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Vehicle Maintenance and Service Regulations</t>
+          <t>Building Renovation and Installation Services</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['reparación', 'edificio', 'instalación', 'sustitución', 'cubierto', 'obras', 'fachada', 'colocación', 'puerta', 'exterior', 'centro', 'suministro', 'interior', 'zona', 'obra']</t>
+          <t>['reparación', 'sustitución', 'cubierto', 'instalación', 'colocación', 'edificio', 'zona', 'puerta', 'interior', 'acceso', 'exterior', 'fachada', 'suministro', 'pintura', 'pavimento']</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -527,33 +547,45 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[{'document_id': 28959, 'sentence': 'Adecuacion Instalaciones Locales Diversos Y Rent A Car', 'score': 0.36476126313209534, 'original_document': 'Adecuacion Instalaciones Locales Diversos Y Rent A Car'}, {'document_id': 17341, 'sentence': 'Servicios de grúa portavehiculos para el rescate y traslado de automóviles en los eventos de Ciudad del Motor de Aragón, S', 'score': 0.3392905294895172, 'original_document': 'Servicios de grúa portavehiculos para el rescate y traslado de automóviles en los eventos de Ciudad del Motor de Aragón, S.A.'}, {'document_id': 4543, 'sentence': 'reforma de locales de los servicios juridicos de la carm, consistente en la división de un despacho en dos, reforma de carpinteria exterior, falso techo, iluminación y aire acondicionado', 'score': 0.33480051159858704, 'original_document': 'reforma de locales de los servicios juridicos de la carm, consistente en la división de un despacho en dos, reforma de carpinteria exterior, falso techo, iluminación y aire acondicionado'}]</t>
+          <t>['El objeto de esta licitación es la contratación de la obra de SUSTITUCIÓN DE CUBIERTA EN EL TALLER DE SUBBLOQUES II NAVANTIA SAN FERNANDO.\r\nLas actuaciones que realizar son:\r\n1. Trabajos previos Desmontaje de revestimientos, instalaciones y cubierta. Además de protección de los elementos existentes.\r\n2. Estructura metálica Limpieza de la estructura existente y aplicación de tratamiento intumescente.\r\n3. Cubierta Instalación completa de nueva cubierta de panel sándwich incluyendo toda la remataria necesaria y canalones.\r\n4. Revestimientos Renovación de falso techo y pintura.\r\n5. Instalaciones Renovación de instalaciones.\r\n', 'Trabajos de acondic. vvda. Retirada de enseres existentes, i/transporte a punto de reciclaje. Tapado de hueco existente techo. Pintura general en paramentos horizontales y verticales. Limpieza general. Equipamiento mín. cocina. Revisión instalaciones.', 'Obras de reforma de áreas higiénicas para mejora de condiciones de accesibilidad y habitabilidad en varias viviendas municipales dispersas']</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['El objeto del presente contrato es el suministro del material de oficina, que se encuentra detallado o en el anexo | del presente pliego, así como del material escolar, que se encuentra detallado en el anexo lIl del presente pliego, con destino al uso y consumo de las diferentes Áreas y Servicios del Ayuntamiento', 'El alcance del suministro regulado por el presente pliego comprende las siguientes prestaciones: Suministro de material de oficina, material de imprenta y material fungible informático (consumibles) con destino a MERCASA y Oficina Municipal de Servicios al Alumnado con las características descritas en el presente pliego y anexos.', 'El alcance del suministro regulado por el presente pliego comprende las siguientes prestaciones: Suministro de material de oficina, material de imprenta y material fungible informático (consumibles) con destino a MERCASA y Oficina Municipal de Servicios al Alumnado con las características descritas en el presente pliego y anexos.']</t>
+          <t>['el objeto del contrato son las obras de reparación de filtraciones y otros trabajos correctivos en el centro comercial opción de gijón.\nde cara a la presente licitación, en una primera fase (fase 0), se han localizado los siguientes ámbitos de intervención en el edificio:\n\uf0b7 acceso de uso público por la calle general suárez valdés.\n\uf0b7 acceso de uso público por el aparcamiento del centro comercial.\n\uf0b7 interior de locales del centro comercial.\nlas intervenciones proyectadas consisten en:\n\uf0b7 actuaciones previas de liberación de espacios de trabajo\n\uf0b7 reparaciones en cubiertas del edificio.\n\uf0b7 impermeabilización mediante tratamiento por el interior de forjado de hormigón\n\uf0b7 sistema de recogida de agua y evacuación\n\uf0b7 reposición de revestimientos a situación original\n\uf0b7 pinturas de revestimientos repuestos.\n\uf0b7 trabajos de corrección de deficiencias en pasos de instalaciones por sectores de incendios\n\uf0b7 trabajos de desmontaje de falsos techos y liberación de áreas de trabajo en forjado para tercera empresa. posterior restitución a situación original de elementos desmontados.\nen fases posteriores a la ejecución de las reparaciones reseñadas, se requiere la ejecución de unos trabajos de control técnico de las reparaciones efectuadas y de la estanquidad de la envolvente del edificio en lo relativo a sus condiciones de protección frente a la humedad e identificación de filtraciones de agua de los cerramientos del edificio, con la visita de personal técnico y operarios para su corrección inmediata. estos trabajos se contemplan de forma periódica o a demanda durante el periodo de duración del contrato.', 'el objeto del contrato viene motivado por la adecuación y puesta en uso del edificio b como centro social, dependiente de la junta municipal de distrito de san blas canillejas. hasta la fecha, este edificio lleva varios años sin funcionamiento y presenta un grado de deterioro considerable, careciendo de las medidas de accesibilidad necesarias para su uso público. ante tal situación y con el fin de evitar que el espacio sea ocupado y vandalizado, el objetivo principal de la junta municipal de san blas-canillejas es volver a ponerlo en uso, reconvirtiéndolo en un centro social. para ello los servicios técnicos de la junta municipal de distrito han llevado a cabo una reforma parcial de las instalaciones interiores, no alcanzando con ellas a cubrir el total de las necesarias para la puesta en uso del edificio b.\ncon el presente contrato, la empresa municipal de la vivienda y suelo de madrid pretende llevar a cabo las obras de instalación del ascensor de tal manera que se pueda garantizar el uso del edifico en condiciones de accesibilidad universal. para ello, se prevé la instalación de un ascensor anexo a la fachada testera orientada al oeste, para lo que será necesaria la demolición parcial de esa misma fachada. la instalación no afecta a la estructura del edificio ni a su distribución funcional. para la correcta instalación del ascensor se ha redactado por el departamento de rehabilitación de la Empresa Municipal de la Vivienda y Suelo de Madrid, proyecto de ejecución para la instalación de ascensor, de acuerdo a la normativa técnica y administrativa de aplicación\n', 'es objeto del presente contrato, por procedimiento abierto simplificado, tramitación ordinaria,\na través de varios criterios, la ejecución de las obras de renovación del pavimento e\ninstalaciones de varias viales públicas en suelo urbano consolidado del casco antiguo del\nnúcleo urbano de ibeas de juarros (burgos) dado el mal estado actual de las mismas por falta\nde mantenimiento y las adversas condiciones climatológicas de la zona.\nla actuación propuesta consistirá en un acabado uniforme de la pavimentación y de la\nurbanización de la red viaria del casco antiguo, en concreto para las calles la iglesia y san\nmiguel, zona del edificio de emiliano aguirre, incremento isleta n-120, dentro de la sobriedad\nde las soluciones empleadas, fijando las pautas globales a seguir en posteriores actuaciones\nde sustitución, conservación y reparación de la urbanización; así como en la renovación de las\nredes de abastecimiento de agua potable y saneamiento existentes, en concreto:\n\uf0b7 sustitución total de la pavimentación con nueva disposición de calzadas y aceras en\nlas calles indicadas.\n\uf0b7 sustitución, ampliación y refuerzo de las conducciones de distribución y evacuación\nanticuadas en los tramos de sustitución de pavimentación con ejecución de acometidas\ndomiciliarias y en los tramos de recuperación de firme de calzada con la conexión de\nlas acometidas existentes, además de reforma saneamiento c/soto y rejilla sumidero\nen la c/yacimientos arqueológicos.\n\uf0b7 colocación de canalizaciones para cableado de electricidad y alumbrado y\ntelecomunicaciones para sustitución de tendidos aéreos en las zonas de sustitución\ntotal de la pavimentación']</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.', 'El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.', 'El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.']</t>
+          <t>['servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales', 'realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'servicio y suministro para el mantenimiento del alumbrado público, de edificios e instalaciones en general y para fiestas y actos culturales del ayuntamiento de santoña, con el fin de conservar las instalaciones en perfecto estado, manteniendo el nivel técnico alcanzado, minimizar los posibles riesgos a las personas, cosas o animales, incluyendo el servicio de control y funcionamiento, tanto de las instalaciones existentes, como de aquellas otras que se efectúen durante la vigencia del contrato, con arreglo a las condiciones que en su caso se señalen.\n\nel ámbito de aplicación de este contrato, se extiende a todos las instalaciones eléctricas que el ayuntamiento tiene para alumbrado público, iluminación artística además del mantenimiento de las instalaciones eléctricas de los edificios, oficinas y pabellones municipales.\n']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>[{'document_id': 27948, 'sentence': 'Instalaciones Renovación de instalaciones', 'score': 0.4417335093021393, 'original_document': 'El objeto de esta licitación es la contratación de la obra de SUSTITUCIÓN DE CUBIERTA EN EL TALLER DE SUBBLOQUES II NAVANTIA SAN FERNANDO.\r\nLas actuaciones que realizar son:\r\n1. Trabajos previos Desmontaje de revestimientos, instalaciones y cubierta. Además de protección de los elementos existentes.\r\n2. Estructura metálica Limpieza de la estructura existente y aplicación de tratamiento intumescente.\r\n3. Cubierta Instalación completa de nueva cubierta de panel sándwich incluyendo toda la remataria necesaria y canalones.\r\n4. Revestimientos Renovación de falso techo y pintura.\r\n5. Instalaciones Renovación de instalaciones.\r\n'}, {'document_id': 2385, 'sentence': 'Revisión instalaciones', 'score': 0.4408396780490875, 'original_document': 'Trabajos de acondic. vvda. Retirada de enseres existentes, i/transporte a punto de reciclaje. Tapado de hueco existente techo. Pintura general en paramentos horizontales y verticales. Limpieza general. Equipamiento mín. cocina. Revisión instalaciones.'}, {'document_id': 14833, 'sentence': 'Obras de reforma de áreas higiénicas para mejora de condiciones de accesibilidad y habitabilidad en varias viviendas municipales dispersas', 'score': 0.4002198874950409, 'original_document': 'Obras de reforma de áreas higiénicas para mejora de condiciones de accesibilidad y habitabilidad en varias viviendas municipales dispersas'}]</t>
+          <t>['El objeto de esta licitación es la contratación de la obra de SUSTITUCIÓN DE CUBIERTA EN EL TALLER DE SUBBLOQUES II NAVANTIA SAN FERNANDO.\r\nLas actuaciones que realizar son:\r\n1. Trabajos previos Desmontaje de revestimientos, instalaciones y cubierta. Además de protección de los elementos existentes.\r\n2. Estructura metálica Limpieza de la estructura existente y aplicación de tratamiento intumescente.\r\n3. Cubierta Instalación completa de nueva cubierta de panel sándwich incluyendo toda la remataria necesaria y canalones.\r\n4. Revestimientos Renovación de falso techo y pintura.\r\n5. Instalaciones Renovación de instalaciones.\r\n', 'Trabajos de acondic. vvda. Retirada de enseres existentes, i/transporte a punto de reciclaje. Tapado de hueco existente techo. Pintura general en paramentos horizontales y verticales. Limpieza general. Equipamiento mín. cocina. Revisión instalaciones.', 'Obras de reforma de áreas higiénicas para mejora de condiciones de accesibilidad y habitabilidad en varias viviendas municipales dispersas']</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>['El objeto del contrato son las obras de reparación de filtraciones y otros trabajos correctivos en el Centro Comercial Opción de Gijón.\nDe cara a la presente licitación, en una primera fase (FASE 0), se han localizado los siguientes ámbitos de intervención en el edificio:\n\uf0b7 Acceso de uso público por la calle General Suárez Valdés.\n\uf0b7 Acceso de uso público por el aparcamiento del centro comercial.\n\uf0b7 Interior de locales del centro comercial.\nLas intervenciones proyectadas consisten en:\n\uf0b7 Actuaciones previas de liberación de espacios de trabajo\n\uf0b7 Reparaciones en cubiertas del edificio.\n\uf0b7 Impermeabilización mediante tratamiento por el interior de forjado de hormigón\n\uf0b7 Sistema de recogida de agua y evacuación\n\uf0b7 Reposición de revestimientos a situación original\n\uf0b7 Pinturas de revestimientos repuestos.\n\uf0b7 Trabajos de corrección de deficiencias en pasos de instalaciones por sectores de incendios\n\uf0b7 Trabajos de desmontaje de falsos techos y liberación de áreas de trabajo en forjado para tercera empresa. Posterior restitución a situación original de elementos desmontados.\nEn fases posteriores a la ejecución de las reparaciones reseñadas, se requiere la ejecución de unos trabajos de control técnico de las reparaciones efectuadas y de la estanquidad de la envolvente del edificio en lo relativo a sus condiciones de protección frente a la humedad e identificación de filtraciones de agua de los cerramientos del edificio, con la visita de personal técnico y operarios para su corrección inmediata. Estos trabajos se contemplan de forma periódica o a demanda durante el periodo de duración del contrato.', 'El objeto del contrato viene motivado por la adecuación y puesta en uso del Edificio B como Centro Social, dependiente de la Junta Municipal de Distrito de San Blas Canillejas. Hasta la fecha, este edificio lleva varios años sin funcionamiento y presenta un grado de deterioro considerable, careciendo de las medidas de accesibilidad necesarias para su uso público. Ante tal situación y con el fin de evitar que el espacio sea ocupado y vandalizado, el objetivo principal de la Junta Municipal de San Blas-Canillejas es volver a ponerlo en uso, reconvirtiéndolo en un Centro Social. Para ello los Servicios Técnicos de la Junta Municipal de Distrito han llevado a cabo una reforma parcial de las instalaciones interiores, no alcanzando con ellas a cubrir el total de las necesarias para la puesta en uso del Edificio B.\nCon el presente contrato, la Empresa Municipal de la Vivienda y Suelo de Madrid pretende llevar a cabo las obras de instalación del ascensor de tal manera que se pueda garantizar el uso del edifico en condiciones de accesibilidad universal. Para ello, se prevé la instalación de un ascensor anexo a la fachada testera orientada al Oeste, para lo que será necesaria la demolición parcial de esa misma fachada. La instalación no afecta a la estructura del edificio ni a su distribución funcional. Para la correcta instalación del ascensor se ha redactado por el Departamento de Rehabilitación de la EMVS, Proyecto de Ejecución para la Instalación de Ascensor, de acuerdo a la normativa técnica y administrativa de aplicación\n', 'Realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de Prodetur en Calle Leonardo Da Vinci nº 16 de Sevilla.El presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: Los equipos de ventilación proyectados serán de la marca ¿Soler &amp;Palau¿ modelo CHAT/4/560N o similar. La instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de CO y posibilitar la puesta en funcionamiento manualmente. La central de detección de CO se instalará en el cuarto de instalaciones de la planta baja. La entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. Todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. Se adjunta plano de la instalación propuesta. Se adjunta medición de la instalación propuesta para su presupuestación.']</t>
+          <t>['El objeto del contrato son las obras de reparación de filtraciones y otros trabajos correctivos en el Centro Comercial Opción de Gijón.\nDe cara a la presente licitación, en una primera fase (FASE 0), se han localizado los siguientes ámbitos de intervención en el edificio:\n\uf0b7 Acceso de uso público por la calle General Suárez Valdés.\n\uf0b7 Acceso de uso público por el aparcamiento del centro comercial.\n\uf0b7 Interior de locales del centro comercial.\nLas intervenciones proyectadas consisten en:\n\uf0b7 Actuaciones previas de liberación de espacios de trabajo\n\uf0b7 Reparaciones en cubiertas del edificio.\n\uf0b7 Impermeabilización mediante tratamiento por el interior de forjado de hormigón\n\uf0b7 Sistema de recogida de agua y evacuación\n\uf0b7 Reposición de revestimientos a situación original\n\uf0b7 Pinturas de revestimientos repuestos.\n\uf0b7 Trabajos de corrección de deficiencias en pasos de instalaciones por sectores de incendios\n\uf0b7 Trabajos de desmontaje de falsos techos y liberación de áreas de trabajo en forjado para tercera empresa. Posterior restitución a situación original de elementos desmontados.\nEn fases posteriores a la ejecución de las reparaciones reseñadas, se requiere la ejecución de unos trabajos de control técnico de las reparaciones efectuadas y de la estanquidad de la envolvente del edificio en lo relativo a sus condiciones de protección frente a la humedad e identificación de filtraciones de agua de los cerramientos del edificio, con la visita de personal técnico y operarios para su corrección inmediata. Estos trabajos se contemplan de forma periódica o a demanda durante el periodo de duración del contrato.', 'Es objeto del presente contrato, por procedimiento abierto simplificado, tramitación ordinaria,\na través de varios criterios, la ejecución de las obras de renovación del pavimento e\ninstalaciones de varias viales públicas en suelo urbano consolidado del Casco Antiguo del\nnúcleo urbano de Ibeas de Juarros (Burgos) dado el mal estado actual de las mismas por falta\nde mantenimiento y las adversas condiciones climatológicas de la zona.\nLa actuación propuesta consistirá en un acabado uniforme de la pavimentación y de la\nurbanización de la red viaria del Casco Antiguo, en concreto para las calles La Iglesia y San\nMiguel, zona del edificio de Emiliano Aguirre, incremento Isleta N-120, dentro de la sobriedad\nde las soluciones empleadas, fijando las pautas globales a seguir en posteriores actuaciones\nde sustitución, conservación y reparación de la urbanización; así como en la renovación de las\nredes de abastecimiento de agua potable y saneamiento existentes, en concreto:\n\uf0b7 Sustitución total de la pavimentación con nueva disposición de calzadas y aceras en\nlas calles indicadas.\n\uf0b7 Sustitución, ampliación y refuerzo de las conducciones de distribución y evacuación\nanticuadas en los tramos de sustitución de pavimentación con ejecución de acometidas\ndomiciliarias y en los tramos de recuperación de firme de calzada con la conexión de\nlas acometidas existentes, además de reforma saneamiento c/Soto y rejilla sumidero\nen la c/Yacimientos Arqueológicos.\n\uf0b7 Colocación de canalizaciones para cableado de electricidad y alumbrado y\ntelecomunicaciones para sustitución de tendidos aéreos en las zonas de sustitución\ntotal de la pavimentación', 'El objeto de este proyecto es definir las obras necesarias para la creación de una rampa de acceso restringido para vehículos de mantenimiento y/o emergencias a la pista deportiva y de una salida de emergencia contigua a la citada rampa, con su correspondiente alumbrado y señalización; la modificación del acceso a la escalera\nque comunica las dos plantas del polideportivo; la instalación de accesos a las cubiertas, de líneas de vida en los faldones inclinados, así como una barandilla de seguridad en la cubierta plana; la instalación de una cortina motorizada que divida la pista en dos zonas de forma que puedan realizarse dos actividades distintas de\nforma simultánea; la sustitución de las campanas de los focos luminosos de la pista por otras con tecnología LED; la renovación de los falsos techos de escayola y de los tubos de acero inoxidable de las chimeneas que atraviesan la planta alta, creando una protección de éstas con placas de yeso; la ampliación hasta 1,20 m de\nlos pasillos de los dos vestuarios, con la sustitución de las puertas de acceso, y el cambio del solado existente en estas dependencias por un suelo continuo vinílico de seguridad y antideslizante; la sustitución y cambio de posición de la puerta principal del edificio de forma que cumpla los requisitos exigidos como puerta en una vía de evacuación, y la renovación de la pintura en paramentos interiores, techos, elementos metálicos, así como la aplicación de pintura ignífuga en los elementos estructurales de acero laminado y/o conformado.']</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>['Contrato de obra de asfaltado viarios públicos, renovación de aceras y carril bici:\n(1) Asfaltado Calle Vicente Soriano – calle Cementerio, calle Pobla de Farnals, calle San Isidro (tramo entre calle Bobalar y Diputación Provincial), calle Mártires (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Rei en Jaume (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Camí Fondo (tramo entre la avenida Sant Pere y la calle Sagunto), av. Sant Pere este (tramo parcial entre calle Camí Fondo y José Mª Llopis), av. Sant Pere este (tramo parcial entre calle José Mª Llopis y Comunidad Valenciana) y calle Castellón (tramo entre calle José Mª Llopis y Comunidad Valenciana).\n(2) Renovación de la acera oeste de la calle Mártires y la calle Vicente Soriano lado barranco y la nueva ejecución de la acera norte y oeste del polideportivo Paco Camarasa (calle Vicente Soriano y calle del Cementerio). \n(3) Carril bici en el lado barranco de la calle Vicente Soriano.', 'El objeto del contrato al que se refiere el presente pliego, es devolver las características fundamentales como son la resistencia , seguridad y comodidad de un pavimento para tráfico rodado, las cuales se van perdiendo con el envejecimiento del firme, provocando un gran número de intervenciones de bacheo, con el consiguiente aumento del coste de mantenimiento, sin que estas operaciones consigan obtener resultados positivos cuando la superficie a bachear es superior a la del pavimento primitivo. Es por todo ello por lo que se decide actuar sobre dicho pavimento con una solución de tipo preventivo y aplicable a toda la superficie de una calle, o de forma parcial. En el Anexo al Proyecto, se detallan el listado de las calles que son objeto del presente proyecto, con su medición. Calles: Calle Santa María del Pino, Calle Nueva Jarilla, Calle Madrid, Calle Plaza el Roble, Calle Manzano, Calle Covidehur, Calle Miguel de Unamuno, Calle Sepúlveda, Calle Duero, Calle Dámaso Alonso, Calle Violeta, Calle Guadalcacín-La Rosa.', 'El presente contrato tiene por objeto establecer acometer las obras  de “Pavimentación. “Carrer Saboneria” y “Carrer Botera” del municipio de Vilanova d’Alcolea / 12183, mediando Plan de Cooperación Provincial de Obras y Servicios de la Diputación Provincial para el año 2021 (Plan Castellón 135-2021), con número de expediente municipal 140/2021, de conformidad con el Proyecto de obras suscrito por el Arquitecto Vicente Pañego, colegiado COACV 08.087, conforme al artículo 13 LCSP de 2017.\nLa actuación pretendida viene motivada por la necesidad de poner el valor el Casco Antiguo de Vilanova d’Alcolea, se pretende acometer las obras de renovación y mejora del pavimento de las calles indicadas en el párrafo anterior.\n\n\tLa intervención consiste en la renovación y mejora del pavimento de las Calle Saboneria y Botera. Todo ello, se concreta adoptando la solución que se adoptó en la Calle Mayor, para ello se adopta una sección transversal tipo en las calles en las que se distinguen:\nUna franja longitudinal de 40 cm de anchura pegada a las fachadas y en ambos lados de la calle.\nUna franja central de 30 cm de anchura en el eje de la calle\nEl resto de calle se completará con adoquines de piedra granítica con ancho variable en cada punto de las calles.\n\n\tLa solución adoptada se plantea en plataforma única con pendiente de desagüe al centro de la calle.\nSe sustituirán las tapas de agua potable y de saneamiento, así como la de los pozos de registro.']</t>
-        </is>
+          <t>['Pavimentación de los siguientes caminos municipales: 1.- Acceso a Remesar 1; 2.- Acceso a Remesar 2; 3.- Camino del límite municipal a la LU-611 por Portaxe; 4.- Camino de la LU-611 la La Reina; 5.- Camino de la LU-0903 a la LU-0905; 6.- Camino de la LU-0903 a Outeiro; 7.- Camino de Lamela a Ver; 8.- Camino de la Avda. Alfonso XIII a Camino del Canal; 9.- Camino de acceso a Ver; 10.- Camino de Ribas Pequeñas a Chorente; 11.- Camino de Acceso a Guntín y 12.- Camino de Vilaboa a Xulián', 'Obras para la reparación de los siguientes caminos: Camino de los Furtivos, Camino de la Cebadilla al Porche de Alfredo, Camino Majadales, Camino de la Raña del Quinto, Camino de Portejuelo al Morrillo, Camino de las Navas 1, Camino de las Navas 2, Camino Miraflores, Camino Rubiastro, Camino las Larguillas y Camino Posada de Aguedillo.', 'Mejora de la capa de rodaje de los caminos: Lote 1: camino en Señorín (Camanzo), camino en Cirela (Gres), camino en Lareo (Salgueiros), caminos en Pastoriza (Carbia), caminos en Fondevila y Los Maestros (Bascuas) y camino en Obra (Santomé de Obra). Lote 2: camino en Oirós, camino en Castro (Besexos), Rúa Covas y Rúa Pendiente (Las Cruces), camino en Loño, camino en Outeiro (Portodemouros), en el Ayuntamiento de Vila de Cruces. ']</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>0.5239411989847819</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.4542410175005595</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.5062429507573446</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.3922361930211385</v>
       </c>
     </row>
     <row r="3">
@@ -561,60 +593,72 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['service', 'instalación', 'presente', 'mantenimiento', 'suministro', 'equipos', 'edificio', 'técnicas', 'centro', 'regir', 'mantenimiento_preventivo', 'conservación', 'limpieza', 'corregir', 'ubicación']</t>
+          <t>['deportivo', 'municipal', 'instalación', 'construcción', 'polideportivo', 'cubierto', 'reparación', 'zona', 'centro', 'abierto_simplificado', 'pista', 'piscina', 'fútbol', 'sustitución', 'adecuación']</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Building Maintenance and Equipment Services</t>
+          <t>Sports Facility Development and Renovation</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>['instalación', 'suministro', 'servicio', 'sistema', 'mantenimiento', 'eléctrico', 'centro', 'obras', 'red', 'construcción', 'estación', 'proyecto', 'equipo', 'adecuación', 'montaje']</t>
+          <t>['obras', 'municipal', 'instalación', 'construcción', 'edificio', 'centro', 'proyecto', 'deportivo', 'reforma', 'ejecución', 'plan', 'adecuación', 'parque', 'fase', 'contrato']</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Electrical System Installation and Maintenance Services</t>
+          <t>Urban Infrastructure Development and Construction Plan</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[{'document_id': 13881, 'sentence': ': Obras necesarias para urbanizar uniformemente el sector I', 'score': 0.3541988432407379, 'original_document': 'ANEXO I.1 PCAP.: Obras necesarias para urbanizar uniformemente el sector I.6-1 de “La Fuensanta” definido por el Modificado nº 21 del Plan General de Ordenación Urbana de Ecija, y que fundamentalmente permitirá ordenar urbanisticamente la zona y su integración con los sistemas generales del municipio.\nAsí mismo [SIC], el presente proyecto de urbanización permitirá valorar las obras y costes de urbanización que contempla las obras de explanación de viales, pavimentación, abastecimiento de aguas, saneamiento, telefonía, suministro de energía eléctrica de Media y Baja Tensión y alumbrado público de toda la zona'}, {'document_id': 14833, 'sentence': 'Obras de reforma de áreas higiénicas para mejora de condiciones de accesibilidad y habitabilidad en varias viviendas municipales dispersas', 'score': 0.34554323554039, 'original_document': 'Obras de reforma de áreas higiénicas para mejora de condiciones de accesibilidad y habitabilidad en varias viviendas municipales dispersas'}, {'document_id': 16900, 'sentence': 'Obras de reforma de áreas higiénicas para mejora de condiciones de accesibilidad y habitabilidad en varias viviendas municipales dispersas', 'score': 0.34554323554039, 'original_document': 'Obras de reforma de áreas higiénicas para mejora de condiciones de accesibilidad y habitabilidad en varias viviendas municipales dispersas'}]</t>
+          <t>['La ejecución de las obras contempladas en el proyecto: “Renovación instalación de alumbrado en Estadio Municipal Aceró y Mini estadio anexo”.', 'Obra de emergencia por Reparación del muro de la A-44, calzada izquierda, P.K. 67+800 margen izquierda y reparación del talud del camino de servicio de la A-44 P.K. 69+750, margen izquierda. T.M. Campillo de arenas. Provincia de Jaén, subsanando la situación de grave peligro existente', 'Ejecución de las obras de “reposición de redes de abastecimiento y saneamiento e implantación de recogida de pluviales en Calle Colomers y Sant Pasqual de Xixona”. Subvención: "Programa de Fomento de la Regeneración y Renovación Urbana y Rural del Plan Estatal de Vivienda 2018-2021".']</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>['El objeto del presente Pliego de Prescripciones Técnicas es la contratación del servicio de seguridad y vigilancia presencial así como control de accesos a las instalaciones, el suministro e instalación, gestión y mantenimiento de sistemas electrónicos de seguridad y de video vigilancia, servicio de conexión a CRA, servicio de custodia de', 'El objeto del presente contrato es la concesión del servicio público para la explotación y mantenimiento de las instalaciones de las piscinas municipales de Novelda que comprenden: piscinas (adultos e infantil), vestuarios, servicios y demás instalaciones complementarias, mediante concesión administrativa, de la forma detallada en el presente', 'El presente Pliego de Prescripciones Técnicas (en adelante, Pliego de Prescripciones Técnicas) tiene por objeto definir y concretar el servicio de: Servicio de Seguridad y Vigilancia, incluyendo la Conexión a Central Receptora de Alarmas (Central Receptora de Alarmas). Servicio de mantenimiento de las instalaciones de vigilancia y seguridad']</t>
+          <t>['el objeto del contrato viene motivado por la adecuación y puesta en uso del edificio b como centro social, dependiente de la junta municipal de distrito de san blas canillejas. hasta la fecha, este edificio lleva varios años sin funcionamiento y presenta un grado de deterioro considerable, careciendo de las medidas de accesibilidad necesarias para su uso público. ante tal situación y con el fin de evitar que el espacio sea ocupado y vandalizado, el objetivo principal de la junta municipal de san blas-canillejas es volver a ponerlo en uso, reconvirtiéndolo en un centro social. para ello los servicios técnicos de la junta municipal de distrito han llevado a cabo una reforma parcial de las instalaciones interiores, no alcanzando con ellas a cubrir el total de las necesarias para la puesta en uso del edificio b.\ncon el presente contrato, la empresa municipal de la vivienda y suelo de madrid pretende llevar a cabo las obras de instalación del ascensor de tal manera que se pueda garantizar el uso del edifico en condiciones de accesibilidad universal. para ello, se prevé la instalación de un ascensor anexo a la fachada testera orientada al oeste, para lo que será necesaria la demolición parcial de esa misma fachada. la instalación no afecta a la estructura del edificio ni a su distribución funcional. para la correcta instalación del ascensor se ha redactado por el departamento de rehabilitación de la Empresa Municipal de la Vivienda y Suelo de Madrid, proyecto de ejecución para la instalación de ascensor, de acuerdo a la normativa técnica y administrativa de aplicación\n', '2º contrato basado en el acuerdo marco del lote n.º 2 "obras en equipamientos municipales, cuyo uso principal sea: deportivo (dep), que engloba: centros deportivos municipales (cdm), campos de fútbol municipales (cfm), instalaciones deportivas elementales (ide), otras instalaciones deportivas (otr), y pabellones deportivos municipales (pdm); cultural (cul); social (soc); y educativo (edu)', 'servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales']</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>['El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.', 'El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.', 'El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.']</t>
+          <t>['servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales', 'realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'servicio y suministro para el mantenimiento del alumbrado público, de edificios e instalaciones en general y para fiestas y actos culturales del ayuntamiento de santoña, con el fin de conservar las instalaciones en perfecto estado, manteniendo el nivel técnico alcanzado, minimizar los posibles riesgos a las personas, cosas o animales, incluyendo el servicio de control y funcionamiento, tanto de las instalaciones existentes, como de aquellas otras que se efectúen durante la vigencia del contrato, con arreglo a las condiciones que en su caso se señalen.\n\nel ámbito de aplicación de este contrato, se extiende a todos las instalaciones eléctricas que el ayuntamiento tiene para alumbrado público, iluminación artística además del mantenimiento de las instalaciones eléctricas de los edificios, oficinas y pabellones municipales.\n']</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>[{'document_id': 31451, 'sentence': 'Suministro, instalación y conexionado de cuadros eléctricos secundarios para la alimentación de los terminales de recarga de vehículos eléctricos, y adecuación de cuadros generales/zonales existentes en las residencias laborales de Euskotren', 'score': 0.47165948152542114, 'original_document': 'Suministro, instalación y conexionado de cuadros eléctricos secundarios para la alimentación de los terminales de recarga de vehículos eléctricos, y adecuación de cuadros generales/zonales existentes en las residencias laborales de Euskotren'}, {'document_id': 2982, 'sentence': 'Adecuacion de instalacion electrica y elaboracion documentacion para nuevo suministro en Asoc', 'score': 0.4481235146522522, 'original_document': 'Adecuacion de instalacion electrica y elaboracion documentacion para nuevo suministro en Asoc.Vecinos Casco Antiguo y Lepanto'}, {'document_id': 18428, 'sentence': 'Reinstalaciones de termos eléctricos, sustitución puertas en vestuarios y aseos, pintura, adecuación pavimento escenario, renovación baño masculino y otros en el CSC José Espronceda del Distrito', 'score': 0.4419811964035034, 'original_document': 'Reinstalaciones de termos eléctricos, sustitución puertas en vestuarios y aseos, pintura, adecuación pavimento escenario, renovación baño masculino y otros en el CSC José Espronceda del Distrito.'}]</t>
+          <t>['Servicio Mtto. Y Conservación De Edificios Y Sus Instalaciones Así Como De Accesos, Aparcam., Urbanizac. Y Área De Movimiento Del Recinto Aeroportuari', 'Obra de Mejoras Infraestructuras en Obando: c/ Alba, c/ Ronda Saliente y c/ San Jose. Plan Cohesiona 2020', 'Pavimentación varias calles de la localidad: Calle San Isidro, Calle Escuelas, Calle Corrales, Avda. Nueva Jarilla, Calle José de Espronceda, Calle Ramón Campoamor, Calle Gustavo Adolfo Bécquer y Plaza El Roble. Plan Provincial de Cooperación a las obras y servicios de competencia municipal Plan ppcos 2022-2023\n']</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>['Realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de Prodetur en Calle Leonardo Da Vinci nº 16 de Sevilla.El presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: Los equipos de ventilación proyectados serán de la marca ¿Soler &amp;Palau¿ modelo CHAT/4/560N o similar. La instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de CO y posibilitar la puesta en funcionamiento manualmente. La central de detección de CO se instalará en el cuarto de instalaciones de la planta baja. La entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. Todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. Se adjunta plano de la instalación propuesta. Se adjunta medición de la instalación propuesta para su presupuestación.', 'Instalación de un punto de recarga para abastacer hasta 2 vehículos simultáneos, de tipo 2 (hasta 22KW de potencia c/u), con conectores tipo Mennekes y equipo IP54, para uso público en general.\nLa estación de recarga se compone de el equipo de recarga propiamente dicho, las protecciones y línea de alimentación al equipo de recarga desde el cuadro eléctrico, reforma del cuadro eléctrico y la legalización de la instalación de recarga.\nSe propone la instalación de un punto de recarga (para dos vehículos) en el acceso al principal al área industrial, IP-7 – Av. Ontinyent, para dos vehículos simultáneos 22+22KW.\nPor ello, el objeto de la actuación es la ampliación de la instalación eléctrica del suministro de alumbrado público del polígono industrial, con la instalación de una estación de recarga para vehículos eléctricos, adaptada a los requisitos del Reglamento Electrotécnico de Baja Tensión (RD 842/2002), con especial interés en la instrucción técnica complementara ITC-52.\nEn general se trata de un contrato de obra, según lo establecido en el artículo 13 – anexo I, de la Ley de Contratos del Sector Público, por la instalación de edificios y obras; instalación eléctrica CPV 45310000 y siguientes.', 'Ejecución de las obras de los proyectos de ejecución de la instalación eléctrica de suministro en 25 kv para el tendido del anillo de conexión de los ct de las instalaciones ferroviarias y de protección civil de la estación de La Sagrera y su zttt,Ejecución de la instalación eléctrica interior de suministro en 25 kv para las instalaciones ferroviarias y de protección civil de la zona de tratamiento técnico de trenes de la estación de La Sagrera (Barcelona) y Ejecución de la instalación eléctrica interior de suministro en 25 kv para las instalaciones ferroviarias y de protección civil de la estación de La Sagrera (Barcelona).']</t>
+          <t>['El objeto del contrato viene motivado por la adecuación y puesta en uso del Edificio B como Centro Social, dependiente de la Junta Municipal de Distrito de San Blas Canillejas. Hasta la fecha, este edificio lleva varios años sin funcionamiento y presenta un grado de deterioro considerable, careciendo de las medidas de accesibilidad necesarias para su uso público. Ante tal situación y con el fin de evitar que el espacio sea ocupado y vandalizado, el objetivo principal de la Junta Municipal de San Blas-Canillejas es volver a ponerlo en uso, reconvirtiéndolo en un Centro Social. Para ello los Servicios Técnicos de la Junta Municipal de Distrito han llevado a cabo una reforma parcial de las instalaciones interiores, no alcanzando con ellas a cubrir el total de las necesarias para la puesta en uso del Edificio B.\nCon el presente contrato, la Empresa Municipal de la Vivienda y Suelo de Madrid pretende llevar a cabo las obras de instalación del ascensor de tal manera que se pueda garantizar el uso del edifico en condiciones de accesibilidad universal. Para ello, se prevé la instalación de un ascensor anexo a la fachada testera orientada al Oeste, para lo que será necesaria la demolición parcial de esa misma fachada. La instalación no afecta a la estructura del edificio ni a su distribución funcional. Para la correcta instalación del ascensor se ha redactado por el Departamento de Rehabilitación de la EMVS, Proyecto de Ejecución para la Instalación de Ascensor, de acuerdo a la normativa técnica y administrativa de aplicación\n', 'Ejecución de las Obras del: Proyecto de Construcción de ampliación y remodelación de la playa de vía y andenes de alta velocidad y del edificio de viajeros de la Estación de Chamartín (Madrid); Proyecto de Construcción del nuevo edificio técnico dealta velocidad en la cabecera norte de la Estación de Madrid-Chamartín; Proyecto de Construcción de conexión del vestíbulo de cercanías bajo vías con metro y futuro paso inferior de alta velocidad de la Estación de Madrid-Chamartín; Proyecto de Construcción de cimentaciones y pilas del lateral este (C/Hiedra) del cubrimiento de la Cabecera Sur de la Estación de Chamartín y Proyecto de Construcción para la demolición del Edificio 23 de la Estación de Madrid-Chamartín-Clara Campoamor y la reordenación del espacio liberado. Fase I', 'Servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. A través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de PEP: 2022/070204 “Equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales']</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>['Contrato de obra de asfaltado viarios públicos, renovación de aceras y carril bici:\n(1) Asfaltado Calle Vicente Soriano – calle Cementerio, calle Pobla de Farnals, calle San Isidro (tramo entre calle Bobalar y Diputación Provincial), calle Mártires (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Rei en Jaume (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Camí Fondo (tramo entre la avenida Sant Pere y la calle Sagunto), av. Sant Pere este (tramo parcial entre calle Camí Fondo y José Mª Llopis), av. Sant Pere este (tramo parcial entre calle José Mª Llopis y Comunidad Valenciana) y calle Castellón (tramo entre calle José Mª Llopis y Comunidad Valenciana).\n(2) Renovación de la acera oeste de la calle Mártires y la calle Vicente Soriano lado barranco y la nueva ejecución de la acera norte y oeste del polideportivo Paco Camarasa (calle Vicente Soriano y calle del Cementerio). \n(3) Carril bici en el lado barranco de la calle Vicente Soriano.', 'El objeto del contrato al que se refiere el presente pliego, es devolver las características fundamentales como son la resistencia , seguridad y comodidad de un pavimento para tráfico rodado, las cuales se van perdiendo con el envejecimiento del firme, provocando un gran número de intervenciones de bacheo, con el consiguiente aumento del coste de mantenimiento, sin que estas operaciones consigan obtener resultados positivos cuando la superficie a bachear es superior a la del pavimento primitivo. Es por todo ello por lo que se decide actuar sobre dicho pavimento con una solución de tipo preventivo y aplicable a toda la superficie de una calle, o de forma parcial. En el Anexo al Proyecto, se detallan el listado de las calles que son objeto del presente proyecto, con su medición. Calles: Calle Santa María del Pino, Calle Nueva Jarilla, Calle Madrid, Calle Plaza el Roble, Calle Manzano, Calle Covidehur, Calle Miguel de Unamuno, Calle Sepúlveda, Calle Duero, Calle Dámaso Alonso, Calle Violeta, Calle Guadalcacín-La Rosa.', 'El presente contrato tiene por objeto establecer acometer las obras  de “Pavimentación. “Carrer Saboneria” y “Carrer Botera” del municipio de Vilanova d’Alcolea / 12183, mediando Plan de Cooperación Provincial de Obras y Servicios de la Diputación Provincial para el año 2021 (Plan Castellón 135-2021), con número de expediente municipal 140/2021, de conformidad con el Proyecto de obras suscrito por el Arquitecto Vicente Pañego, colegiado COACV 08.087, conforme al artículo 13 LCSP de 2017.\nLa actuación pretendida viene motivada por la necesidad de poner el valor el Casco Antiguo de Vilanova d’Alcolea, se pretende acometer las obras de renovación y mejora del pavimento de las calles indicadas en el párrafo anterior.\n\n\tLa intervención consiste en la renovación y mejora del pavimento de las Calle Saboneria y Botera. Todo ello, se concreta adoptando la solución que se adoptó en la Calle Mayor, para ello se adopta una sección transversal tipo en las calles en las que se distinguen:\nUna franja longitudinal de 40 cm de anchura pegada a las fachadas y en ambos lados de la calle.\nUna franja central de 30 cm de anchura en el eje de la calle\nEl resto de calle se completará con adoquines de piedra granítica con ancho variable en cada punto de las calles.\n\n\tLa solución adoptada se plantea en plataforma única con pendiente de desagüe al centro de la calle.\nSe sustituirán las tapas de agua potable y de saneamiento, así como la de los pozos de registro.']</t>
-        </is>
+          <t>['Pavimentación de los siguientes caminos municipales: 1.- Acceso a Remesar 1; 2.- Acceso a Remesar 2; 3.- Camino del límite municipal a la LU-611 por Portaxe; 4.- Camino de la LU-611 la La Reina; 5.- Camino de la LU-0903 a la LU-0905; 6.- Camino de la LU-0903 a Outeiro; 7.- Camino de Lamela a Ver; 8.- Camino de la Avda. Alfonso XIII a Camino del Canal; 9.- Camino de acceso a Ver; 10.- Camino de Ribas Pequeñas a Chorente; 11.- Camino de Acceso a Guntín y 12.- Camino de Vilaboa a Xulián', 'Obras para la reparación de los siguientes caminos: Camino de los Furtivos, Camino de la Cebadilla al Porche de Alfredo, Camino Majadales, Camino de la Raña del Quinto, Camino de Portejuelo al Morrillo, Camino de las Navas 1, Camino de las Navas 2, Camino Miraflores, Camino Rubiastro, Camino las Larguillas y Camino Posada de Aguedillo.', 'Mejora de la capa de rodaje de los caminos: Lote 1: camino en Señorín (Camanzo), camino en Cirela (Gres), camino en Lareo (Salgueiros), caminos en Pastoriza (Carbia), caminos en Fondevila y Los Maestros (Bascuas) y camino en Obra (Santomé de Obra). Lote 2: camino en Oirós, camino en Castro (Besexos), Rúa Covas y Rúa Pendiente (Las Cruces), camino en Loño, camino en Outeiro (Portodemouros), en el Ayuntamiento de Vila de Cruces. ']</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>0.387961467107137</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.4217383364836375</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.4578314324220021</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.5967775781949362</v>
       </c>
     </row>
     <row r="4">
@@ -622,16 +666,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['service', 'presente', 'ayuntamiento', 'municipal', 'redacción', 'administrativo', 'dirección', 'apoyo', 'sector_público', 'ejercicio', 'organismo', 'cumplimiento', 'fase', 'público', 'técnica']</t>
+          <t>['zona', 'actuación', 'acceso', 'mejorar', 'instalación', 'consistir', 'pavimento', 'actual', 'presente', 'municipio', 'dotar', 'acondicionamiento', 'superficie', 'servicio', 'construcción']</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Public Sector Administrative Support and Compliance Services</t>
+          <t>Infrastructure Improvement Project in Municipality</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -639,43 +683,55 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>['instalación', 'plan_recuperación', 'transformación_resiliencia', 'edificio', 'financiado_unión', 'proyecto', 'municipal', 'autoconsumo', 'solar_fotovoltaico', 'obras', 'next_generation', 'actuación', 'energético', 'renovación', 'financiado']</t>
+          <t>['instalación', 'servicio', 'zona', 'actuación', 'espacio', 'él', 'suministro', 'mantenimiento', 'presente', 'elemento', 'mejorar', 'construcción', 'parque', 'actual', 'municipal']</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Building Renovation and Energy Transformation Project</t>
+          <t>Municipal Infrastructure Improvement Project</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[{'document_id': 17143, 'sentence': 'Servicio de vigilancia y seguridad de edificios de la administración de la Generalitat, su sector público instrumental y entidades adheridas', 'score': 0.44632843136787415, 'original_document': 'Servicio de vigilancia y seguridad de edificios de la administración de la Generalitat, su sector público instrumental y entidades adheridas. Contratación basada en el Acuerdo Marco de servicios de vigilancia y seguridad de edificios de la administración de la Generalitat, su sector público instrumental y entidades adheridas (AC 6/18 CC Lote 8, Valencia Consellerias)'}, {'document_id': 7769, 'sentence': 'Reforma y acondicionamiento de los aseos públicos para la creación de dos consultas médicas en el Centro de Salud de Dolores / Reforma i condicionament dels lavabos públics per a la creació de dues consultes mèdiques en el Centre de Salut de Dolores', 'score': 0.43458133935928345, 'original_document': 'Reforma y acondicionamiento de los aseos públicos para la creación de dos consultas médicas en el Centro de Salud de Dolores / Reforma i condicionament dels lavabos públics per a la creació de dues consultes mèdiques en el Centre de Salut de Dolores'}, {'document_id': 15587, 'sentence': 'Modificación del Contrato de Colaboración entre el Sector Público y el Sector Privado para la realización de una actuación global e integrada en el Hospital Universitario Marqués de Valdecilla, en relación a las condiciones específicas del Servicio de Informática', 'score': 0.4266388416290283, 'original_document': 'Modificación del Contrato de Colaboración entre el Sector Público y el Sector Privado para la realización de una actuación global e integrada en el Hospital Universitario Marqués de Valdecilla, en relación a las condiciones específicas del Servicio de Informática.'}]</t>
+          <t>['Servicio de albañilería, carpintería, revestimientos y trabajos de fontanería y saneamiento para el mantenimiento de los Ed. Administrativos Municipales', 'Contrato de obras del Proyecto de  Sustitución de Pavimentación y Redes de Abastecimiento de Aguas y Saneamiento de C/ Iglesia de Posadilla. Plan Provincial Plurianual de Cooperación a las obras y Servicios de Competencia Municipal durante el Cuatrienio 2020-2023', 'Contrato de obras del Proyecto de  Sustitución de Pavimentación y Redes de Abastecimiento de Aguas y Saneamiento de C/ Iglesia de Posadilla. Plan Provincial Plurianual de Cooperación a las obras y Servicios de Competencia Municipal durante el Cuatrienio 2020-2023']</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>['Las presentes prescripciones técnicas se aplicarán al procedimiento de contratación de los servicios de acciones de concienciación en Seguridad de la Información para todo el personal de Servicio de Empleo de Castilla y León, con arreglo a las condiciones de servicio indicadas en el mismo (en adelante el “Servicio/Servicios”).', 'La misión del Servicio de Contratación (Servicio de Contratación) de umivale es dar apoyo a las distintas Divisiones y Servicios en sus necesidades de contratación de Obras, Servicios y Suministros mediante la adjudicación de la oferta con la mejor relación calidad-precio en el entorno de calidad de umivale', 'El objeto del contrato es la prestación de los servicios de infraestructura de TI de la Agencia, que incluyen la prestación de los servicios de infraestructura de TI de la Agencia, que incluyen la prestación de los servicios de infraestructura de TI de la Agencia, que incluyen la prestación de los servicios de infraestructura']</t>
+          <t>['tal y como se especifica en el proyecto básico y de ejecución de las obras de restauración del conjunto monumental del castillo de castelló de farfanya, redactado por el equipo de la empresa ianua arquitectures, s.c.p., la obra comprende:\na) "recinto superior" del castillo. la propuesta pretende recuperar el perímetro murario del recinto, mediante la recuperación del nivel de uso interior y la consolidación de la muralla.\nmediante la consolidación, que no reconstrucción, será posible dotar al castillo de nuevo de la imagen como tal, tanto interior como exteriormente.\nb) murallas sur y este. coracha (apéndice de la muralla) hasta la torre sur. la muralla este, que cierra el recinto de la zona del cementerio, colapsó en el año 2018. esta es una zona alejada del castillo pero que requiere su reconstrucción para la seguridad de la zona de acceso peatonal y del este del foso.\nla muralla sur actualmente está sufriendo un proceso de degradación de la base, y algunas zonas se encuentra descalzada de la roca madre, muy estratificada. la zona sur se conecta con la torre sur mediante la coracha, actualmente en ruinas.\nhay material fotográfico que permite reconstruir este elemento, muy peculiar y que permitirá una explicación fácil del carácter defensivo de las estructuras.\nc) mejora del acceso peatonal desde la calle del castillo hasta la sala de caballerías. en la actuación de consolidación de murallas y recuperación de niveles, se perderá el acceso actual al recinto mediante un derribo en la zona norte; la propuesta plantea la recuperación del acceso por la cara sur de la muralla, mediante una pasarela de acceso que permita la entrada de la manera más accesible posible. el resto de esta actuación contempla una mínima actuación de mejora del acceso peatonal desde el núcleo habitado, actualmente un camino de difícil tráfico.', 'el objeto del contrato es la realización de cuatro actuaciones de mejora urbanística en determinados puntos de la localidad: \nactuación 1: c/ ronda. el tramo a intervenir de la calle ronda presenta una acera estrecha, invadida por la maleza de una franja colindante sin urbanizar donde además existe un muro en mal estado. el pavimento presenta mal estado y discontinuidades y en la calzada existe la presencia de un desagüe hundido. se pretende urbanizar esta zona y reparar los desperfectos en la calzada.\nactuación 2: rotonda cruce c/ ronda y c/ san martin. la rotonda es en la actualidad una isleta con vegetación desbordando los límites de la misma. se pretende la urbanización de esta zona.\nactuación 3: parque y punto limpio. el punto limpio se quiere reubicar junto a la pista deportiva. tanto la pista deportiva como el parque infantil requieren una renovación para la mejora de las instalaciones.\nactuación 4: c/ real. la calle real presenta tres escalones longitudinales irregulares que presentan carencias de accesibilidad. con esta actuación se mejora la accesibilidad de la zona y se crea una nueva superficie ajardinada\n\n', 'el objeto del contrato es la realización de cuatro actuaciones de mejora urbanística en\ndeterminados puntos de la localidad:\n\nactuación 1: c/ ronda. el tramo a intervenir de la calle ronda presenta una acera estrecha, invadida por la maleza de una franja colindante sin urbanizar donde además existe\nun muro en mal estado. el pavimento presenta mal estado y discontinuidades y en la calzada existe la presencia de un desagüe hundido. se pretende urbanizar esta zona y reparar los desperfectos en la calzada.\n\nactuación 2: rotonda cruce c/ ronda y c/ san martin. la rotonda es en la actualidad una isleta con vegetación desbordando los límites de la misma. se pretende la urbanización de esta zona.\n\nactuación 3: parque y punto limpio. el punto limpio se quiere reubicar junto a la pista deportiva. tanto la pista deportiva como el parque infantil requieren una renovación para la mejora de las instalaciones.\n\nactuación 4: c/ real. la calle real presenta tres escalones longitudinales irregulares que presentan carencias de accesibilidad. con esta actuación se mejora la accesibilidad de la zona y se crea una nueva superficie ajardinada']</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>['El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.', 'El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.', 'El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.']</t>
+          <t>['servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales', 'realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'servicio y suministro para el mantenimiento del alumbrado público, de edificios e instalaciones en general y para fiestas y actos culturales del ayuntamiento de santoña, con el fin de conservar las instalaciones en perfecto estado, manteniendo el nivel técnico alcanzado, minimizar los posibles riesgos a las personas, cosas o animales, incluyendo el servicio de control y funcionamiento, tanto de las instalaciones existentes, como de aquellas otras que se efectúen durante la vigencia del contrato, con arreglo a las condiciones que en su caso se señalen.\n\nel ámbito de aplicación de este contrato, se extiende a todos las instalaciones eléctricas que el ayuntamiento tiene para alumbrado público, iluminación artística además del mantenimiento de las instalaciones eléctricas de los edificios, oficinas y pabellones municipales.\n']</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>[{'document_id': 33728, 'sentence': '(Plan de Recuperación, Transformación y Resiliencia)', 'score': 0.4414082169532776, 'original_document': 'Ejecución de Obra y Coordinación de Seguridad y Salud para la Reforma en dos unidades convivenciales del C.A. Elorrio del IFAS. Financiado por la Unión Europea- Next Generation EU. (Plan de Recuperación, Transformación y Resiliencia).'}, {'document_id': 23351, 'sentence': 'Plan de recuperación, transformación y resiliencia', 'score': 0.4398255944252014, 'original_document': '52-GR-4310; 54.643/22 Proyecto de Adecuación al Real Decreto 635/2006 de los Túneles de Fuentecilla, Carchuna, Ítrabo, Cantalobos y Marchante. Provincia de Granada. Plan de recuperación, transformación y resiliencia. Financiado por la Unión Europea. NEXT GENERATION EU'}, {'document_id': 22518, 'sentence': 'Plan de Recuperación, Transformación y Resiliencia', 'score': 0.43982556462287903, 'original_document': 'Aparcamientos disuasorios junto a futuro apeadero "Casilla de los Pinos" en Venta Bermeja. Plan de Recuperación, Transformación y Resiliencia.'}]</t>
+          <t>['Servicio de albañilería, carpintería, revestimientos y trabajos de fontanería y saneamiento para el mantenimiento de los Ed. Administrativos Municipales', 'Obras necesarias para proceder a la reurbanización de Calle La Paja, entre Horquilleros y Villeta de Monda (Málaga).\n(Plan de Reactivación Económica Municipal 2020)', 'Contrato de obras para la ejecución del proyecto aconidicionamiento de les Escoletes Municipals  (PMEEN)']</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>['Realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de Prodetur en Calle Leonardo Da Vinci nº 16 de Sevilla.El presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: Los equipos de ventilación proyectados serán de la marca ¿Soler &amp;Palau¿ modelo CHAT/4/560N o similar. La instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de CO y posibilitar la puesta en funcionamiento manualmente. La central de detección de CO se instalará en el cuarto de instalaciones de la planta baja. La entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. Todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. Se adjunta plano de la instalación propuesta. Se adjunta medición de la instalación propuesta para su presupuestación.', 'El objeto del contrato viene motivado por la adecuación y puesta en uso del Edificio B como Centro Social, dependiente de la Junta Municipal de Distrito de San Blas Canillejas. Hasta la fecha, este edificio lleva varios años sin funcionamiento y presenta un grado de deterioro considerable, careciendo de las medidas de accesibilidad necesarias para su uso público. Ante tal situación y con el fin de evitar que el espacio sea ocupado y vandalizado, el objetivo principal de la Junta Municipal de San Blas-Canillejas es volver a ponerlo en uso, reconvirtiéndolo en un Centro Social. Para ello los Servicios Técnicos de la Junta Municipal de Distrito han llevado a cabo una reforma parcial de las instalaciones interiores, no alcanzando con ellas a cubrir el total de las necesarias para la puesta en uso del Edificio B.\nCon el presente contrato, la Empresa Municipal de la Vivienda y Suelo de Madrid pretende llevar a cabo las obras de instalación del ascensor de tal manera que se pueda garantizar el uso del edifico en condiciones de accesibilidad universal. Para ello, se prevé la instalación de un ascensor anexo a la fachada testera orientada al Oeste, para lo que será necesaria la demolición parcial de esa misma fachada. La instalación no afecta a la estructura del edificio ni a su distribución funcional. Para la correcta instalación del ascensor se ha redactado por el Departamento de Rehabilitación de la EMVS, Proyecto de Ejecución para la Instalación de Ascensor, de acuerdo a la normativa técnica y administrativa de aplicación\n', 'Instalación de un punto de recarga para abastacer hasta 2 vehículos simultáneos, de tipo 2 (hasta 22KW de potencia c/u), con conectores tipo Mennekes y equipo IP54, para uso público en general.\nLa estación de recarga se compone de el equipo de recarga propiamente dicho, las protecciones y línea de alimentación al equipo de recarga desde el cuadro eléctrico, reforma del cuadro eléctrico y la legalización de la instalación de recarga.\nSe propone la instalación de un punto de recarga (para dos vehículos) en el acceso al principal al área industrial, IP-7 – Av. Ontinyent, para dos vehículos simultáneos 22+22KW.\nPor ello, el objeto de la actuación es la ampliación de la instalación eléctrica del suministro de alumbrado público del polígono industrial, con la instalación de una estación de recarga para vehículos eléctricos, adaptada a los requisitos del Reglamento Electrotécnico de Baja Tensión (RD 842/2002), con especial interés en la instrucción técnica complementara ITC-52.\nEn general se trata de un contrato de obra, según lo establecido en el artículo 13 – anexo I, de la Ley de Contratos del Sector Público, por la instalación de edificios y obras; instalación eléctrica CPV 45310000 y siguientes.']</t>
+          <t>['El objeto del contrato es la ejecución de las obras para la creación de un\npunto limpio para el centro de transferencia de residuos sólidos urbanos. Los\ntrabajos que se proyectan para su ejecución son:\na) Acondicionamiento acceso al centro de transferencia, instalación de\npuerta corredera, cercado y vallado perimetral de toda la zona destinada\na la actividad gestión de residuos.\nb) Instalación de fosa séptica, decantador y separador de hidrocarburos.\nc) Instalación de sistema de videovigilancia interno.\nd) Acondicionamiento medioambiental zonas pavimentos exteriores.\ne) Instalación de báscula y caseta de control e instalación eléctrica zona de\nacceso y báscula de control.\nf) Estructura metálica muelle almacenamiento de voluminosos.\ng) Mejora de drene-desagüe en zona de muelles de carga residuos.\nh) Equipamiento para la instalación de contenedores y jaulas residuos.', 'Realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de Prodetur en Calle Leonardo Da Vinci nº 16 de Sevilla.El presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: Los equipos de ventilación proyectados serán de la marca ¿Soler &amp;Palau¿ modelo CHAT/4/560N o similar. La instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de CO y posibilitar la puesta en funcionamiento manualmente. La central de detección de CO se instalará en el cuarto de instalaciones de la planta baja. La entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. Todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. Se adjunta plano de la instalación propuesta. Se adjunta medición de la instalación propuesta para su presupuestación.', 'El objeto del contrato viene motivado por la adecuación y puesta en uso del Edificio B como Centro Social, dependiente de la Junta Municipal de Distrito de San Blas Canillejas. Hasta la fecha, este edificio lleva varios años sin funcionamiento y presenta un grado de deterioro considerable, careciendo de las medidas de accesibilidad necesarias para su uso público. Ante tal situación y con el fin de evitar que el espacio sea ocupado y vandalizado, el objetivo principal de la Junta Municipal de San Blas-Canillejas es volver a ponerlo en uso, reconvirtiéndolo en un Centro Social. Para ello los Servicios Técnicos de la Junta Municipal de Distrito han llevado a cabo una reforma parcial de las instalaciones interiores, no alcanzando con ellas a cubrir el total de las necesarias para la puesta en uso del Edificio B.\nCon el presente contrato, la Empresa Municipal de la Vivienda y Suelo de Madrid pretende llevar a cabo las obras de instalación del ascensor de tal manera que se pueda garantizar el uso del edifico en condiciones de accesibilidad universal. Para ello, se prevé la instalación de un ascensor anexo a la fachada testera orientada al Oeste, para lo que será necesaria la demolición parcial de esa misma fachada. La instalación no afecta a la estructura del edificio ni a su distribución funcional. Para la correcta instalación del ascensor se ha redactado por el Departamento de Rehabilitación de la EMVS, Proyecto de Ejecución para la Instalación de Ascensor, de acuerdo a la normativa técnica y administrativa de aplicación\n']</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>['Contrato de obra de asfaltado viarios públicos, renovación de aceras y carril bici:\n(1) Asfaltado Calle Vicente Soriano – calle Cementerio, calle Pobla de Farnals, calle San Isidro (tramo entre calle Bobalar y Diputación Provincial), calle Mártires (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Rei en Jaume (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Camí Fondo (tramo entre la avenida Sant Pere y la calle Sagunto), av. Sant Pere este (tramo parcial entre calle Camí Fondo y José Mª Llopis), av. Sant Pere este (tramo parcial entre calle José Mª Llopis y Comunidad Valenciana) y calle Castellón (tramo entre calle José Mª Llopis y Comunidad Valenciana).\n(2) Renovación de la acera oeste de la calle Mártires y la calle Vicente Soriano lado barranco y la nueva ejecución de la acera norte y oeste del polideportivo Paco Camarasa (calle Vicente Soriano y calle del Cementerio). \n(3) Carril bici en el lado barranco de la calle Vicente Soriano.', 'El objeto del contrato al que se refiere el presente pliego, es devolver las características fundamentales como son la resistencia , seguridad y comodidad de un pavimento para tráfico rodado, las cuales se van perdiendo con el envejecimiento del firme, provocando un gran número de intervenciones de bacheo, con el consiguiente aumento del coste de mantenimiento, sin que estas operaciones consigan obtener resultados positivos cuando la superficie a bachear es superior a la del pavimento primitivo. Es por todo ello por lo que se decide actuar sobre dicho pavimento con una solución de tipo preventivo y aplicable a toda la superficie de una calle, o de forma parcial. En el Anexo al Proyecto, se detallan el listado de las calles que son objeto del presente proyecto, con su medición. Calles: Calle Santa María del Pino, Calle Nueva Jarilla, Calle Madrid, Calle Plaza el Roble, Calle Manzano, Calle Covidehur, Calle Miguel de Unamuno, Calle Sepúlveda, Calle Duero, Calle Dámaso Alonso, Calle Violeta, Calle Guadalcacín-La Rosa.', 'El presente contrato tiene por objeto establecer acometer las obras  de “Pavimentación. “Carrer Saboneria” y “Carrer Botera” del municipio de Vilanova d’Alcolea / 12183, mediando Plan de Cooperación Provincial de Obras y Servicios de la Diputación Provincial para el año 2021 (Plan Castellón 135-2021), con número de expediente municipal 140/2021, de conformidad con el Proyecto de obras suscrito por el Arquitecto Vicente Pañego, colegiado COACV 08.087, conforme al artículo 13 LCSP de 2017.\nLa actuación pretendida viene motivada por la necesidad de poner el valor el Casco Antiguo de Vilanova d’Alcolea, se pretende acometer las obras de renovación y mejora del pavimento de las calles indicadas en el párrafo anterior.\n\n\tLa intervención consiste en la renovación y mejora del pavimento de las Calle Saboneria y Botera. Todo ello, se concreta adoptando la solución que se adoptó en la Calle Mayor, para ello se adopta una sección transversal tipo en las calles en las que se distinguen:\nUna franja longitudinal de 40 cm de anchura pegada a las fachadas y en ambos lados de la calle.\nUna franja central de 30 cm de anchura en el eje de la calle\nEl resto de calle se completará con adoquines de piedra granítica con ancho variable en cada punto de las calles.\n\n\tLa solución adoptada se plantea en plataforma única con pendiente de desagüe al centro de la calle.\nSe sustituirán las tapas de agua potable y de saneamiento, así como la de los pozos de registro.']</t>
-        </is>
+          <t>['Pavimentación de los siguientes caminos municipales: 1.- Acceso a Remesar 1; 2.- Acceso a Remesar 2; 3.- Camino del límite municipal a la LU-611 por Portaxe; 4.- Camino de la LU-611 la La Reina; 5.- Camino de la LU-0903 a la LU-0905; 6.- Camino de la LU-0903 a Outeiro; 7.- Camino de Lamela a Ver; 8.- Camino de la Avda. Alfonso XIII a Camino del Canal; 9.- Camino de acceso a Ver; 10.- Camino de Ribas Pequeñas a Chorente; 11.- Camino de Acceso a Guntín y 12.- Camino de Vilaboa a Xulián', 'Obras para la reparación de los siguientes caminos: Camino de los Furtivos, Camino de la Cebadilla al Porche de Alfredo, Camino Majadales, Camino de la Raña del Quinto, Camino de Portejuelo al Morrillo, Camino de las Navas 1, Camino de las Navas 2, Camino Miraflores, Camino Rubiastro, Camino las Larguillas y Camino Posada de Aguedillo.', 'Mejora de la capa de rodaje de los caminos: Lote 1: camino en Señorín (Camanzo), camino en Cirela (Gres), camino en Lareo (Salgueiros), caminos en Pastoriza (Carbia), caminos en Fondevila y Los Maestros (Bascuas) y camino en Obra (Santomé de Obra). Lote 2: camino en Oirós, camino en Castro (Besexos), Rúa Covas y Rúa Pendiente (Las Cruces), camino en Loño, camino en Outeiro (Portodemouros), en el Ayuntamiento de Vila de Cruces. ']</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>0.4432808955510457</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.4915814896424611</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.4919224381446838</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.4139114121596019</v>
       </c>
     </row>
     <row r="5">
@@ -683,60 +739,72 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['presente', 'suministro', 'adquisición', 'service', 'hospital_universitario', 'equipos', 'sanitario', 'laboratorio', 'característica', 'materiales', 'instalación', 'centro', 'universitario', 'equipamiento', 'tratamiento']</t>
+          <t>['acceso', 'avenida', 'zona', 'pavimentación', 'carretera', 'tramo', 'acondicionamiento', 'municipal', 'fase', 'construcción', 'adecuación', 'sujeto_regulación', 'asfaltado', 'urbanización', 'glorieta']</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Hospital Equipment Acquisition and Installation Analysis</t>
+          <t>Urban Infrastructure Development Project</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>['calle', 'obras', 'renovación', 'pavimentación', 'red', 'tramo', 'camino', 'plaza', 'avenida', 'proyecto', 'urbanización', 'red_abastecimiento', 'municipio', 'saneamiento', 'mejorar']</t>
+          <t>['camino', 'acceso', 'acondicionamiento', 'mejorar', 'municipal', 'reparación', 'pavimentación', 'zona', 'obras', 'firme', 'actuación', 'vial', 'tramo', 'camino_rural', 'parroquia']</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Urban Infrastructure Improvement Project</t>
+          <t>Rural Road Improvement Project</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[{'document_id': 13869, 'sentence': 'Plà – Hospital Prov', 'score': 0.45188501477241516, 'original_document': 'Reparación de patologías en la fachada del C.S. Plà – Hospital Prov. en un contexto de prácticas respetuosas con el medio ambiente'}, {'document_id': 4386, 'sentence': 'Reforma consultas externas de coloproctología y trauma Hospital Sagunto', 'score': 0.4165428578853607, 'original_document': 'Reforma consultas externas de coloproctología y trauma Hospital Sagunto.'}, {'document_id': 6398, 'sentence': 'Obra instalación climatización (preinstalación) SAIP y almacén Electromedicina del Hospital General Universitario de Elda', 'score': 0.4114189147949219, 'original_document': 'Obra instalación climatización (preinstalación) SAIP y almacén Electromedicina del Hospital General Universitario de Elda'}]</t>
+          <t>['Servicio Mtto. Y Conservación De Edificios Y Sus Instalaciones Así Como De Accesos, Aparcam., Urbanizac. Y Área De Movimiento Del Recinto Aeroportuari', 'Urbanización de cl. san Jose en el marco de la convocatoria para la ejecución de obras comprendidas entre los objetivos de desarrollo sostenbile "reactivem castelló" obres ejercicio 2021.La obra pretende integrar la pavimentación ordenada que se ha llevado a cabo\nen Forcall, mediante adoquines de Hormigón tomados con arena, sobre una base de Hormigón HN 150. La obra permite restituir las trapas particulares de alcantarillado y agua potable, sustituyéndolas por trapas de fundición de mejor durabilidad y que quedan integradas en el pavimento. La obra permitirá la sustitución de un tramo de conducto de saneamiento entre los pozos de la C/ Tomas Salvador y viviendas de la C/ Sant Josep , con el fin de adecuar la red de saneamiento.', 'Projecto Fase I del projecto de ejecución de la urbanización de un espacio libre público para equipamiento deportivo en el urbanizable 02']</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>['El alcance del suministro regulado por el presente pliego comprende las siguientes prestaciones: Suministro de material de oficina, material de imprenta y material fungible informático (consumibles) con destino a MERCASA y Oficina Municipal de Servicios al Alumnado con las características descritas en el presente pliego y anexos.', 'El alcance del suministro regulado por el presente pliego comprende las siguientes prestaciones: Suministro de material de oficina, material de imprenta y material fungible informático (consumibles) con destino a MERCASA y Oficina Municipal de Servicios al Alumnado con las características descritas en el presente pliego y anexos.', 'El objeto del presente contrato es el suministro del material de oficina, que se encuentra detallado o en el anexo | del presente pliego, así como del material escolar, que se encuentra detallado en el anexo lIl del presente pliego, con destino al uso y consumo de las diferentes Áreas y Servicios del Ayuntamiento']</t>
+          <t>['tal y como se especifica en el proyecto básico y de ejecución de las obras de restauración del conjunto monumental del castillo de castelló de farfanya, redactado por el equipo de la empresa ianua arquitectures, s.c.p., la obra comprende:\na) "recinto superior" del castillo. la propuesta pretende recuperar el perímetro murario del recinto, mediante la recuperación del nivel de uso interior y la consolidación de la muralla.\nmediante la consolidación, que no reconstrucción, será posible dotar al castillo de nuevo de la imagen como tal, tanto interior como exteriormente.\nb) murallas sur y este. coracha (apéndice de la muralla) hasta la torre sur. la muralla este, que cierra el recinto de la zona del cementerio, colapsó en el año 2018. esta es una zona alejada del castillo pero que requiere su reconstrucción para la seguridad de la zona de acceso peatonal y del este del foso.\nla muralla sur actualmente está sufriendo un proceso de degradación de la base, y algunas zonas se encuentra descalzada de la roca madre, muy estratificada. la zona sur se conecta con la torre sur mediante la coracha, actualmente en ruinas.\nhay material fotográfico que permite reconstruir este elemento, muy peculiar y que permitirá una explicación fácil del carácter defensivo de las estructuras.\nc) mejora del acceso peatonal desde la calle del castillo hasta la sala de caballerías. en la actuación de consolidación de murallas y recuperación de niveles, se perderá el acceso actual al recinto mediante un derribo en la zona norte; la propuesta plantea la recuperación del acceso por la cara sur de la muralla, mediante una pasarela de acceso que permita la entrada de la manera más accesible posible. el resto de esta actuación contempla una mínima actuación de mejora del acceso peatonal desde el núcleo habitado, actualmente un camino de difícil tráfico.', 'contratación de las obras del proyecto tecnico de regeneración  de vías municipales: acceso en santa marta de ortoá. acceso a lier desde carretera de pintín. acceso a rosende desde carretera de arxevide. acceso a abuin desde vilanova. tramos dentro del núcleo de sano saturnino. acceso a vilaesteba. acceso en la esperanza (oural).acceso al real (san fiz de reimondez).acceso en villarairo.acceso desde seteventos a toldaos y accesos en betote', 'contrato obras proyecto reformado pavimentación caminos acceso a navallos, del muro (ousende) al limite municipal ayuntamiento de bóveda, de crta de monforte a gesto (limite con bóveda), de sobreda a valdorrama, de valdorrama a lamapodre, acceso en córneas, accesos a taíz, acceso a la capilla de guadalupe, de gruñedo la llave, buxán-louredo, de vilatiñosa a corveixe, bustelo-vilaravides, de la barxa la abuime de cazapico (limite municipal), acceso a cavada, acceso a malveiros y acceso a mosiños, incluidas en el plan provincial  único de cooperación con los ayuntamientos 2018']</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>['El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.', 'El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.', 'El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.']</t>
+          <t>['servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales', 'realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'servicio y suministro para el mantenimiento del alumbrado público, de edificios e instalaciones en general y para fiestas y actos culturales del ayuntamiento de santoña, con el fin de conservar las instalaciones en perfecto estado, manteniendo el nivel técnico alcanzado, minimizar los posibles riesgos a las personas, cosas o animales, incluyendo el servicio de control y funcionamiento, tanto de las instalaciones existentes, como de aquellas otras que se efectúen durante la vigencia del contrato, con arreglo a las condiciones que en su caso se señalen.\n\nel ámbito de aplicación de este contrato, se extiende a todos las instalaciones eléctricas que el ayuntamiento tiene para alumbrado público, iluminación artística además del mantenimiento de las instalaciones eléctricas de los edificios, oficinas y pabellones municipales.\n']</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>[{'document_id': 13766, 'sentence': ', Urbanizac', 'score': 0.6113101243972778, 'original_document': 'Servicio Mtto. Y Conservación De Edificios Y Sus Instalaciones Así Como De Accesos, Aparcam., Urbanizac. Y Área De Movimiento Del Recinto Aeroportuari'}, {'document_id': 4237, 'sentence': 'Urbanización de cl', 'score': 0.5540722608566284, 'original_document': 'Urbanización de cl. san Jose en el marco de la convocatoria para la ejecución de obras comprendidas entre los objetivos de desarrollo sostenbile "reactivem castelló" obres ejercicio 2021.La obra pretende integrar la pavimentación ordenada que se ha llevado a cabo\nen Forcall, mediante adoquines de Hormigón tomados con arena, sobre una base de Hormigón HN 150. La obra permite restituir las trapas particulares de alcantarillado y agua potable, sustituyéndolas por trapas de fundición de mejor durabilidad y que quedan integradas en el pavimento. La obra permitirá la sustitución de un tramo de conducto de saneamiento entre los pozos de la C/ Tomas Salvador y viviendas de la C/ Sant Josep , con el fin de adecuar la red de saneamiento.'}, {'document_id': 9457, 'sentence': '2021/6617 urbanismo', 'score': 0.5301958322525024, 'original_document': 'Obras de demolición por emergencia- ruina física inminente y urgente demolición forzosa de la construcción sita en el lago, nº 81 y 83, turón, (mieres), referencias catastrales:8382502tn7888s0001kd y 8382503tn7888s0001rd expte. 2021/6617 urbanismo'}]</t>
+          <t>['Contrato de obra de reforma y ampliación del consultorio médico de Vélez-Blanco. Actuación financiada por la Consejería De Agricultura, Ganadería, Pesca Y Desarrollo Sostenible De La Junta De Andalucía Y Por La Unión Europea A Través Del Fondo Europeo Agrícola De Desarrollo Rural (Feader).\nRURAL (FEADER).', 'Contrato de obra de reforma y ampliación del consultorio médico de Vélez-Blanco. Actuación financiada por la Consejería De Agricultura, Ganadería, Pesca Y Desarrollo Sostenible De La Junta De Andalucía Y Por La Unión Europea A Través Del Fondo Europeo Agrícola De Desarrollo Rural (Feader).\r\nRURAL (FEADER).', 'Ejecución de la red de saneamiento en Palmés. Tramo: O Burgo-A Burata. Ourense.OH.332.823. El objeto de esta contratación se cofinanciará por la Unión Europea a través del Fondo Europeo Agrícola de Desarrollo Rural (FEADER) en un 75% del gasto elexible, en el marco del Programa de Desarrollo Rural (PDR) Galicia 2014-2020. La actuación se enmarca dentro del Programa de Desarrollo Rural en la Medida 07 Servicios básicos y renovación de poblaciones en zonas rurales , Submedida 7.2 Apoyo a las inversiones en la creación, mejora o ampliación de todo tipo de pequeñas infraestructuras, incluidos las inversiones en energías renovables y ahorro energético y Prioridad 6 de Desarrollo Rural Fomentar la inclusión social, la reducción de la pobreza y el desarrollo económico en las zonas rurales . Europa invierte en el rural. Procedimiento documentalmente simplificado. ']</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>['Contrato de obra de asfaltado viarios públicos, renovación de aceras y carril bici:\n(1) Asfaltado Calle Vicente Soriano – calle Cementerio, calle Pobla de Farnals, calle San Isidro (tramo entre calle Bobalar y Diputación Provincial), calle Mártires (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Rei en Jaume (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Camí Fondo (tramo entre la avenida Sant Pere y la calle Sagunto), av. Sant Pere este (tramo parcial entre calle Camí Fondo y José Mª Llopis), av. Sant Pere este (tramo parcial entre calle José Mª Llopis y Comunidad Valenciana) y calle Castellón (tramo entre calle José Mª Llopis y Comunidad Valenciana).\n(2) Renovación de la acera oeste de la calle Mártires y la calle Vicente Soriano lado barranco y la nueva ejecución de la acera norte y oeste del polideportivo Paco Camarasa (calle Vicente Soriano y calle del Cementerio). \n(3) Carril bici en el lado barranco de la calle Vicente Soriano.', 'El objeto del contrato al que se refiere el presente pliego, es devolver las características fundamentales como son la resistencia , seguridad y comodidad de un pavimento para tráfico rodado, las cuales se van perdiendo con el envejecimiento del firme, provocando un gran número de intervenciones de bacheo, con el consiguiente aumento del coste de mantenimiento, sin que estas operaciones consigan obtener resultados positivos cuando la superficie a bachear es superior a la del pavimento primitivo. Es por todo ello por lo que se decide actuar sobre dicho pavimento con una solución de tipo preventivo y aplicable a toda la superficie de una calle, o de forma parcial. En el Anexo al Proyecto, se detallan el listado de las calles que son objeto del presente proyecto, con su medición. Calles: Calle Santa María del Pino, Calle Nueva Jarilla, Calle Madrid, Calle Plaza el Roble, Calle Manzano, Calle Covidehur, Calle Miguel de Unamuno, Calle Sepúlveda, Calle Duero, Calle Dámaso Alonso, Calle Violeta, Calle Guadalcacín-La Rosa.', 'Reurbanización de varias calles del casco urbano de Godelleta: Calle Ramón y Cajal, Carretera de Buñol, Calle Siete Aguas, Calle Jacinto Benavente, Calle Salvador Ferrandis, Calle Maestro Serrrano, Calle Arturo Baynes, Calle Vicente Moreno, Calle Juan Ramón Jiménez, Calle Doctor Fleming, Calle Chiva, Avenida Vicente Lassala, Calle Comunidad Valenciana']</t>
+          <t>['Pavimentación de los siguientes caminos municipales: 1.- Acceso a Remesar 1; 2.- Acceso a Remesar 2; 3.- Camino del límite municipal a la LU-611 por Portaxe; 4.- Camino de la LU-611 la La Reina; 5.- Camino de la LU-0903 a la LU-0905; 6.- Camino de la LU-0903 a Outeiro; 7.- Camino de Lamela a Ver; 8.- Camino de la Avda. Alfonso XIII a Camino del Canal; 9.- Camino de acceso a Ver; 10.- Camino de Ribas Pequeñas a Chorente; 11.- Camino de Acceso a Guntín y 12.- Camino de Vilaboa a Xulián', 'Obras para la reparación de los siguientes caminos: Camino de los Furtivos, Camino de la Cebadilla al Porche de Alfredo, Camino Majadales, Camino de la Raña del Quinto, Camino de Portejuelo al Morrillo, Camino de las Navas 1, Camino de las Navas 2, Camino Miraflores, Camino Rubiastro, Camino las Larguillas y Camino Posada de Aguedillo.', 'Mejora de la capa de rodaje de los caminos: Lote 1: camino en Señorín (Camanzo), camino en Cirela (Gres), camino en Lareo (Salgueiros), caminos en Pastoriza (Carbia), caminos en Fondevila y Los Maestros (Bascuas) y camino en Obra (Santomé de Obra). Lote 2: camino en Oirós, camino en Castro (Besexos), Rúa Covas y Rúa Pendiente (Las Cruces), camino en Loño, camino en Outeiro (Portodemouros), en el Ayuntamiento de Vila de Cruces. ']</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>['Contrato de obra de asfaltado viarios públicos, renovación de aceras y carril bici:\n(1) Asfaltado Calle Vicente Soriano – calle Cementerio, calle Pobla de Farnals, calle San Isidro (tramo entre calle Bobalar y Diputación Provincial), calle Mártires (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Rei en Jaume (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Camí Fondo (tramo entre la avenida Sant Pere y la calle Sagunto), av. Sant Pere este (tramo parcial entre calle Camí Fondo y José Mª Llopis), av. Sant Pere este (tramo parcial entre calle José Mª Llopis y Comunidad Valenciana) y calle Castellón (tramo entre calle José Mª Llopis y Comunidad Valenciana).\n(2) Renovación de la acera oeste de la calle Mártires y la calle Vicente Soriano lado barranco y la nueva ejecución de la acera norte y oeste del polideportivo Paco Camarasa (calle Vicente Soriano y calle del Cementerio). \n(3) Carril bici en el lado barranco de la calle Vicente Soriano.', 'El objeto del contrato al que se refiere el presente pliego, es devolver las características fundamentales como son la resistencia , seguridad y comodidad de un pavimento para tráfico rodado, las cuales se van perdiendo con el envejecimiento del firme, provocando un gran número de intervenciones de bacheo, con el consiguiente aumento del coste de mantenimiento, sin que estas operaciones consigan obtener resultados positivos cuando la superficie a bachear es superior a la del pavimento primitivo. Es por todo ello por lo que se decide actuar sobre dicho pavimento con una solución de tipo preventivo y aplicable a toda la superficie de una calle, o de forma parcial. En el Anexo al Proyecto, se detallan el listado de las calles que son objeto del presente proyecto, con su medición. Calles: Calle Santa María del Pino, Calle Nueva Jarilla, Calle Madrid, Calle Plaza el Roble, Calle Manzano, Calle Covidehur, Calle Miguel de Unamuno, Calle Sepúlveda, Calle Duero, Calle Dámaso Alonso, Calle Violeta, Calle Guadalcacín-La Rosa.', 'El presente contrato tiene por objeto establecer acometer las obras  de “Pavimentación. “Carrer Saboneria” y “Carrer Botera” del municipio de Vilanova d’Alcolea / 12183, mediando Plan de Cooperación Provincial de Obras y Servicios de la Diputación Provincial para el año 2021 (Plan Castellón 135-2021), con número de expediente municipal 140/2021, de conformidad con el Proyecto de obras suscrito por el Arquitecto Vicente Pañego, colegiado COACV 08.087, conforme al artículo 13 LCSP de 2017.\nLa actuación pretendida viene motivada por la necesidad de poner el valor el Casco Antiguo de Vilanova d’Alcolea, se pretende acometer las obras de renovación y mejora del pavimento de las calles indicadas en el párrafo anterior.\n\n\tLa intervención consiste en la renovación y mejora del pavimento de las Calle Saboneria y Botera. Todo ello, se concreta adoptando la solución que se adoptó en la Calle Mayor, para ello se adopta una sección transversal tipo en las calles en las que se distinguen:\nUna franja longitudinal de 40 cm de anchura pegada a las fachadas y en ambos lados de la calle.\nUna franja central de 30 cm de anchura en el eje de la calle\nEl resto de calle se completará con adoquines de piedra granítica con ancho variable en cada punto de las calles.\n\n\tLa solución adoptada se plantea en plataforma única con pendiente de desagüe al centro de la calle.\nSe sustituirán las tapas de agua potable y de saneamiento, así como la de los pozos de registro.']</t>
-        </is>
+          <t>['Pavimentación de los siguientes caminos municipales: 1.- Acceso a Remesar 1; 2.- Acceso a Remesar 2; 3.- Camino del límite municipal a la LU-611 por Portaxe; 4.- Camino de la LU-611 la La Reina; 5.- Camino de la LU-0903 a la LU-0905; 6.- Camino de la LU-0903 a Outeiro; 7.- Camino de Lamela a Ver; 8.- Camino de la Avda. Alfonso XIII a Camino del Canal; 9.- Camino de acceso a Ver; 10.- Camino de Ribas Pequeñas a Chorente; 11.- Camino de Acceso a Guntín y 12.- Camino de Vilaboa a Xulián', 'Obras para la reparación de los siguientes caminos: Camino de los Furtivos, Camino de la Cebadilla al Porche de Alfredo, Camino Majadales, Camino de la Raña del Quinto, Camino de Portejuelo al Morrillo, Camino de las Navas 1, Camino de las Navas 2, Camino Miraflores, Camino Rubiastro, Camino las Larguillas y Camino Posada de Aguedillo.', 'Mejora de la capa de rodaje de los caminos: Lote 1: camino en Señorín (Camanzo), camino en Cirela (Gres), camino en Lareo (Salgueiros), caminos en Pastoriza (Carbia), caminos en Fondevila y Los Maestros (Bascuas) y camino en Obra (Santomé de Obra). Lote 2: camino en Oirós, camino en Castro (Besexos), Rúa Covas y Rúa Pendiente (Las Cruces), camino en Loño, camino en Outeiro (Portodemouros), en el Ayuntamiento de Vila de Cruces. ']</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>0.4821016788482666</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.4536506533622742</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.3187868197758992</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.3187868197758992</v>
       </c>
     </row>
     <row r="6">
@@ -744,60 +812,729 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>['protección_incendio', 'aire_acondicionado', 'instalación', 'cubierto_sustitución', 'electricidad_calefacción', 'ascensor_fachada', 'reparación_climatización', 'cambio_modificar', 'vinilo_parquet', 'termo_rótulo', 'modificar', 'termo_puerta', 'centro_arrendado', 'centro', 'reparación']</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Building Maintenance and Renovation Services</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>['instalación', 'obras', 'protección_incendio', 'aire_acondicionado', 'cubierto_sustitución', 'electricidad_calefacción', 'ascensor_fachada', 'reparación_climatización', 'obra', 'cambio_modificar', 'vinilo_parquet', 'termo_rótulo', 'regulación_armonizado', 'contratación_sujeto', 'simplificado_abierto']</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Building Renovation and Maintenance Services</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>['Obras de reforma de áreas higiénicas para mejora de condiciones de accesibilidad y habitabilidad en varias viviendas municipales dispersas', 'Obras de reforma de áreas higiénicas para mejora de condiciones de accesibilidad y habitabilidad en varias viviendas municipales dispersas', 'Obras de reforma de áreas higiénicas para mejora de condiciones de accesibilidad y habitabilidad en varias viviendas municipales dispersas']</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>['el objeto del contrato menor está conformado por las siguientes prestaciones:\n\n•  elaboración de proyecto técnico para la legalización de las instalaciones de protección contra incendios resultantes tras la realización de las obras de reforma y el suministro de componentes, sistemas y equipos de protección contra incendios. este servicio incluye los trámites administrativos necesarios ante la administración o entidad de control e inspección industrial competente.\n\n•  ejecución de las obras de reforma para la adecuación del sistema de protección contra incendios del edificio de tanatorio del cementerio jardín de alcalá de henares, a la normativa comunitaria y nacional vigente en materia de instalaciones de protección contra incendios y de industria. las obras consistirán principalmente en acciones de instalación o montaje, con los trabajos complementarios que ello requiera, de sistemas, componentes y equipos de protección contra incendios.\n\n•  suministro de los componentes, sistemas y equipos de protección contra incendios que sean precisos para adecuar las instalaciones de este tipo existentes actualmente en el edificio de tanatorio, a la normativa comunitaria y nacional vigente en materia de instalaciones de protección contra incendios y de industria. todos los productos suministrados por la empresa adjudicataria a cementerio jardín de alcalá de henares, s.a. en virtud de este contrato serán propiedad de cementerio jardín de alcalá de henares, s.a. ', 'obras de obra, reparación de climatización, aire acondicionado, electricidad, calefacción, protección contra incendios, ascensores, fachada, cubierta, etc. sustitución de termos, rótulos, vinilos, parquet. (nueva instalación, cambio o modifica', 'obras de obra, reparación de climatización, aire acondicionado, electricidad, calefacción, protección contra incendios, ascensores, fachada, cubierta, etc. sustitución de termos, rótulos, vinilos, parquet. (nueva instalación, cambio o modifica']</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>['servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales', 'realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'servicio y suministro para el mantenimiento del alumbrado público, de edificios e instalaciones en general y para fiestas y actos culturales del ayuntamiento de santoña, con el fin de conservar las instalaciones en perfecto estado, manteniendo el nivel técnico alcanzado, minimizar los posibles riesgos a las personas, cosas o animales, incluyendo el servicio de control y funcionamiento, tanto de las instalaciones existentes, como de aquellas otras que se efectúen durante la vigencia del contrato, con arreglo a las condiciones que en su caso se señalen.\n\nel ámbito de aplicación de este contrato, se extiende a todos las instalaciones eléctricas que el ayuntamiento tiene para alumbrado público, iluminación artística además del mantenimiento de las instalaciones eléctricas de los edificios, oficinas y pabellones municipales.\n']</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>['Obras de reforma de áreas higiénicas para mejora de condiciones de accesibilidad y habitabilidad en varias viviendas municipales dispersas', 'Obras de reforma de áreas higiénicas para mejora de condiciones de accesibilidad y habitabilidad en varias viviendas municipales dispersas', 'Obras de reforma de áreas higiénicas para mejora de condiciones de accesibilidad y habitabilidad en varias viviendas municipales dispersas']</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>['Obras de Obra, reparación de climatización, aire acondicionado, electricidad, calefacción, protección contra incendios, ascensores, fachada, cubierta, etc. Sustitución de termos, rótulos, vinilos, parquet. (nueva instalación, cambio o modifica', 'Obras de Obra, reparación de climatización, aire acondicionado, electricidad, calefacción, protección contra incendios, ascensores, fachada, cubierta, etc. Sustitución de termos, rótulos, vinilos, parquet. (nueva instalación, cambio o modifica', 'Obras de Obra, reparación de climatización, aire acondicionado, electricidad, calefacción, protección contra incendios, ascensores, fachada, cubierta, etc. Sustitución de termos, rótulos, vinilos, parquet. (nueva instalación, cambio o modifica']</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>['Pavimentación de los siguientes caminos municipales: 1.- Acceso a Remesar 1; 2.- Acceso a Remesar 2; 3.- Camino del límite municipal a la LU-611 por Portaxe; 4.- Camino de la LU-611 la La Reina; 5.- Camino de la LU-0903 a la LU-0905; 6.- Camino de la LU-0903 a Outeiro; 7.- Camino de Lamela a Ver; 8.- Camino de la Avda. Alfonso XIII a Camino del Canal; 9.- Camino de acceso a Ver; 10.- Camino de Ribas Pequeñas a Chorente; 11.- Camino de Acceso a Guntín y 12.- Camino de Vilaboa a Xulián', 'Obras para la reparación de los siguientes caminos: Camino de los Furtivos, Camino de la Cebadilla al Porche de Alfredo, Camino Majadales, Camino de la Raña del Quinto, Camino de Portejuelo al Morrillo, Camino de las Navas 1, Camino de las Navas 2, Camino Miraflores, Camino Rubiastro, Camino las Larguillas y Camino Posada de Aguedillo.', 'Mejora de la capa de rodaje de los caminos: Lote 1: camino en Señorín (Camanzo), camino en Cirela (Gres), camino en Lareo (Salgueiros), caminos en Pastoriza (Carbia), caminos en Fondevila y Los Maestros (Bascuas) y camino en Obra (Santomé de Obra). Lote 2: camino en Oirós, camino en Castro (Besexos), Rúa Covas y Rúa Pendiente (Las Cruces), camino en Loño, camino en Outeiro (Portodemouros), en el Ayuntamiento de Vila de Cruces. ']</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>0.4434570372104645</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.4570606350898743</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.4926644563674927</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.331246296564738</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>['instalación', 'suministro', 'eléctrico', 'centro', 'servicio', 'edificio', 'adecuación', 'sustitución', 'mantenimiento', 'estación', 'energético', 'municipal', 'autoconsumo', 'construcción', 'equipo']</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Electrical Installation and Maintenance Services</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>['instalación', 'suministro', 'sistema', 'servicio', 'red', 'eléctrico', 'obras', 'centro', 'mantenimiento', 'proyecto', 'edificio', 'autoconsumo', 'equipo', 'agua', 'municipal']</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Electrical System Installation and Maintenance Services</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>['Adecuacion de instalacion electrica y elaboracion documentacion para nuevo suministro en Asoc.Vecinos Casco Antiguo y Lepanto', 'Reforma de instalación eléctrica en B.T. de Alumbrado Exterior para Alumbrado Público en el casco antiguo de Arnedo, obras financiadas por el IDAE para el paso a una economía baja en carbono en el marco del Programa Operativo del Fondo Europeo de Desarrollo Regional (FEDER) de crecimiento sostenible 2014-2020', '116/ise/2022/gr renovación instalación electrica y carpintería en el c.p.r. monte chullo de la huertezuela, huéneja, granada - 00073/ise/2019/sc contrato basado en el acuerdo marco de obras de reforma, adaptación, ampliacion, redistribución y mejoras en centros educativos de la consejeria de educacion y deportes de la junta de andalucia sin nueva licitación.']</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>['realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'instalación de un punto de recarga para abastacer hasta 2 vehículos simultáneos, de tipo 2 (hasta 22kw de potencia c/u), con conectores tipo mennekes y equipo ip54, para uso público en general.\nla estación de recarga se compone de el equipo de recarga propiamente dicho, las protecciones y línea de alimentación al equipo de recarga desde el cuadro eléctrico, reforma del cuadro eléctrico y la legalización de la instalación de recarga.\nse propone la instalación de un punto de recarga (para dos vehículos) en el acceso al principal al área industrial, / – av. ontinyent, para dos vehículos simultáneos 22+22kw.\npor ello, el objeto de la actuación es la ampliación de la instalación eléctrica del suministro de alumbrado público del polígono industrial, con la instalación de una estación de recarga para vehículos eléctricos, adaptada a los requisitos del reglamento electrotécnico de baja tensión (rd 842/2002), con especial interés en la instrucción técnica complementara itc-52.\nen general se trata de un contrato de obra, según lo establecido en el artículo 13 – anexo i, de la ley de contratos del sector público, por la instalación de edificios y obras; instalación eléctrica Clasificación por Nomenclatura de Unidades de Contratación 45310000 y siguientes.', 'ejecución de las obras de los proyectos de ejecución de la instalación eléctrica de suministro en 25 kv para el tendido del anillo de conexión de los ct de las instalaciones ferroviarias y de protección civil de la estación de la sagrera y su zttt,ejecución de la instalación eléctrica interior de suministro en 25 kv para las instalaciones ferroviarias y de protección civil de la zona de tratamiento técnico de trenes de la estación de la sagrera (barcelona) y ejecución de la instalación eléctrica interior de suministro en 25 kv para las instalaciones ferroviarias y de protección civil de la estación de la sagrera (barcelona).']</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>['servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales', 'realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'servicio y suministro para el mantenimiento del alumbrado público, de edificios e instalaciones en general y para fiestas y actos culturales del ayuntamiento de santoña, con el fin de conservar las instalaciones en perfecto estado, manteniendo el nivel técnico alcanzado, minimizar los posibles riesgos a las personas, cosas o animales, incluyendo el servicio de control y funcionamiento, tanto de las instalaciones existentes, como de aquellas otras que se efectúen durante la vigencia del contrato, con arreglo a las condiciones que en su caso se señalen.\n\nel ámbito de aplicación de este contrato, se extiende a todos las instalaciones eléctricas que el ayuntamiento tiene para alumbrado público, iluminación artística además del mantenimiento de las instalaciones eléctricas de los edificios, oficinas y pabellones municipales.\n']</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>['Suministro, instalación y conexionado de cuadros eléctricos secundarios para la alimentación de los terminales de recarga de vehículos eléctricos, y adecuación de cuadros generales/zonales existentes en las residencias laborales de Euskotren', 'Adecuacion de instalacion electrica y elaboracion documentacion para nuevo suministro en Asoc.Vecinos Casco Antiguo y Lepanto', 'Reinstalaciones de termos eléctricos, sustitución puertas en vestuarios y aseos, pintura, adecuación pavimento escenario, renovación baño masculino y otros en el CSC José Espronceda del Distrito.']</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>['Realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de Prodetur en Calle Leonardo Da Vinci nº 16 de Sevilla.El presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: Los equipos de ventilación proyectados serán de la marca ¿Soler &amp;Palau¿ modelo CHAT/4/560N o similar. La instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de CO y posibilitar la puesta en funcionamiento manualmente. La central de detección de CO se instalará en el cuarto de instalaciones de la planta baja. La entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. Todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. Se adjunta plano de la instalación propuesta. Se adjunta medición de la instalación propuesta para su presupuestación.', 'Instalación de un punto de recarga para abastacer hasta 2 vehículos simultáneos, de tipo 2 (hasta 22KW de potencia c/u), con conectores tipo Mennekes y equipo IP54, para uso público en general.\nLa estación de recarga se compone de el equipo de recarga propiamente dicho, las protecciones y línea de alimentación al equipo de recarga desde el cuadro eléctrico, reforma del cuadro eléctrico y la legalización de la instalación de recarga.\nSe propone la instalación de un punto de recarga (para dos vehículos) en el acceso al principal al área industrial, IP-7 – Av. Ontinyent, para dos vehículos simultáneos 22+22KW.\nPor ello, el objeto de la actuación es la ampliación de la instalación eléctrica del suministro de alumbrado público del polígono industrial, con la instalación de una estación de recarga para vehículos eléctricos, adaptada a los requisitos del Reglamento Electrotécnico de Baja Tensión (RD 842/2002), con especial interés en la instrucción técnica complementara ITC-52.\nEn general se trata de un contrato de obra, según lo establecido en el artículo 13 – anexo I, de la Ley de Contratos del Sector Público, por la instalación de edificios y obras; instalación eléctrica CPV 45310000 y siguientes.', 'Ejecución de las obras de los proyectos de ejecución de la instalación eléctrica de suministro en 25 kv para el tendido del anillo de conexión de los ct de las instalaciones ferroviarias y de protección civil de la estación de La Sagrera y su zttt,Ejecución de la instalación eléctrica interior de suministro en 25 kv para las instalaciones ferroviarias y de protección civil de la zona de tratamiento técnico de trenes de la estación de La Sagrera (Barcelona) y Ejecución de la instalación eléctrica interior de suministro en 25 kv para las instalaciones ferroviarias y de protección civil de la estación de La Sagrera (Barcelona).']</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>['Pavimentación de los siguientes caminos municipales: 1.- Acceso a Remesar 1; 2.- Acceso a Remesar 2; 3.- Camino del límite municipal a la LU-611 por Portaxe; 4.- Camino de la LU-611 la La Reina; 5.- Camino de la LU-0903 a la LU-0905; 6.- Camino de la LU-0903 a Outeiro; 7.- Camino de Lamela a Ver; 8.- Camino de la Avda. Alfonso XIII a Camino del Canal; 9.- Camino de acceso a Ver; 10.- Camino de Ribas Pequeñas a Chorente; 11.- Camino de Acceso a Guntín y 12.- Camino de Vilaboa a Xulián', 'Obras para la reparación de los siguientes caminos: Camino de los Furtivos, Camino de la Cebadilla al Porche de Alfredo, Camino Majadales, Camino de la Raña del Quinto, Camino de Portejuelo al Morrillo, Camino de las Navas 1, Camino de las Navas 2, Camino Miraflores, Camino Rubiastro, Camino las Larguillas y Camino Posada de Aguedillo.', 'Mejora de la capa de rodaje de los caminos: Lote 1: camino en Señorín (Camanzo), camino en Cirela (Gres), camino en Lareo (Salgueiros), caminos en Pastoriza (Carbia), caminos en Fondevila y Los Maestros (Bascuas) y camino en Obra (Santomé de Obra). Lote 2: camino en Oirós, camino en Castro (Besexos), Rúa Covas y Rúa Pendiente (Las Cruces), camino en Loño, camino en Outeiro (Portodemouros), en el Ayuntamiento de Vila de Cruces. ']</t>
+        </is>
+      </c>
+      <c r="N7" t="n">
+        <v>0.4945149024327596</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.4386114776134491</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.4626121123631795</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.3493091364701589</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>9</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>['centro_educación', 'infantil_primaria', 'secundaria', 'instalación', 'aula', 'instituto_educación', 'centro', 'instituto_enseñanza', 'ampliación', 'colegio', 'infantil', 'infantil_primario', 'reforma', 'zona', 'patio']</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Educational Facility Expansion and Renovation</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>['edificio', 'obras', 'reforma', 'reparación', 'instalación', 'adecuación', 'madrid', 'centro', 'acondicionamiento', 'cubierto', 'planta', 'calle', 'sustitución', 'situado', 'tc']</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Building Renovation and Construction in Madrid</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>['Ejecución de las obras de “reposición de redes de abastecimiento y saneamiento e implantación de recogida de pluviales en Calle Colomers y Sant Pasqual de Xixona”. Subvención: "Programa de Fomento de la Regeneración y Renovación Urbana y Rural del Plan Estatal de Vivienda 2018-2021".', 'Ejecución de las obras de "rehabilitación de vivienda social municipal en la Calle Trinquet 6, de Xixona".  Subvención: "Programa de Fomento de la Regeneración y Renovación Urbana y Rural del Plan Estatal de Vivienda 2018-2021".', 'El objeto de esta licitación es la contratación de la obra de SUSTITUCIÓN DE CUBIERTA EN EL TALLER DE SUBBLOQUES II NAVANTIA SAN FERNANDO.\r\nLas actuaciones que realizar son:\r\n1. Trabajos previos Desmontaje de revestimientos, instalaciones y cubierta. Además de protección de los elementos existentes.\r\n2. Estructura metálica Limpieza de la estructura existente y aplicación de tratamiento intumescente.\r\n3. Cubierta Instalación completa de nueva cubierta de panel sándwich incluyendo toda la remataria necesaria y canalones.\r\n4. Revestimientos Renovación de falso techo y pintura.\r\n5. Instalaciones Renovación de instalaciones.\r\n']</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>['obras relevo de carpinterias y otras actuaciones en 10 centros de la provincia de lugo: Centro de Educación Infantil y Primaria de bretona de a pastoriza; Centro de Educación Infantil y Primaria el salvador de a pastoriza; Centro de Educación Infantil y Primaria aquilino iglesias alvarino de abadin ; Centro de Educación Infantil y Primaria de antas de ulla; Centro de Educación Infantil y Primaria rosalía de castro de bóvexpedientea ; Centro de Educación Infantil y Primaria juan rey de lourenza; Centro de Educación Infantil y Primaria de o vicexpedienteo; Centro de Educación Infantil y Primaria mato vizoso de vilalba; Escuela de Educación Infantil san roque de viveiro; Centro de Educación Infantil y Primaria de xermade. expexpedienteiente expediente 56/21-lo\n', 'obras de adecuación a normativa de sanidad de varios Centro de Educación Infantil y Primarias del distrito villa de vallecas mediante instalación de mosquieteras en ventanas de cocinas y comedores (Centro de Educación Infantil y Primaria blas de otero, calle puentelarra, 34 ; Centro de Educación Infantil y Primaria ciudad de valencia, avenida del mediterráneo km 9; Centro de Educación Infantil y Primaria francisco fatou, calle camino de la suerte, 23; Centro de Educación Infantil y Primaria josé de echegaray calle puentedey, 14; Centro de Educación Infantil y Primaria juan de herrera calle enrique garcía álvarez, 11; Centro de Educación Infantil y Primaria juan gris, calle muela de san juan, 37; Centro de Educación Infantil y Primaria loyola de palacio, embalse de navacerrada, 60) .', 'obras de relevo de carpinterías y otras actuaciones en 7 centros de la provincia de a coruña: Centro de Educación Infantil y Primaria eugenio lópez de cee; Centro de Educación Infantil y Primaria alfrexpedienteo brañas de laracha (la); Centro de Educación Infantil y Primaria cabo de la arena de laxe; Centro de Educación Infantil y Primaria plurilingüe bragade de oza-cesuras ;Centro de Educación Infantil y Primaria de oza de los los ríe de oza-cesuras : Centro de Educación Infantil y Primaria expedienteuardo pondal de ponteceso y Centro de Educación Infantil y Primaria de fonte-diaz de touro. expexpedienteiente expediente 57/21-lo']</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>['servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales', 'realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'servicio y suministro para el mantenimiento del alumbrado público, de edificios e instalaciones en general y para fiestas y actos culturales del ayuntamiento de santoña, con el fin de conservar las instalaciones en perfecto estado, manteniendo el nivel técnico alcanzado, minimizar los posibles riesgos a las personas, cosas o animales, incluyendo el servicio de control y funcionamiento, tanto de las instalaciones existentes, como de aquellas otras que se efectúen durante la vigencia del contrato, con arreglo a las condiciones que en su caso se señalen.\n\nel ámbito de aplicación de este contrato, se extiende a todos las instalaciones eléctricas que el ayuntamiento tiene para alumbrado público, iluminación artística además del mantenimiento de las instalaciones eléctricas de los edificios, oficinas y pabellones municipales.\n']</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>['Obras del proyecto de ejecución para la modificación de la instalación de fontanería y ACS (excluyendo la producción), nueva instalación solar para contribución de energía renovable para ACS y nueva instalación de fotovoltaica en la Residencia de Mayores Usera, C/ Cristo de la Victoria, nº 247. (Madrid)', 'Trabajos de reparación de la instalación de saneamiento de los Pabellones Copema y "G", en Paseo de la Infanta Isabel,1. Madrid. ', 'D.G. Madrid. Sustitución De Tarima Y Pintura Del Despacho Del Secretario General En C/ García De Paredes 65, Edificio Adscrito A La Delegación Del Gobierno En Madrid.']</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>['El objeto del contrato viene motivado por la adecuación y puesta en uso del Edificio B como Centro Social, dependiente de la Junta Municipal de Distrito de San Blas Canillejas. Hasta la fecha, este edificio lleva varios años sin funcionamiento y presenta un grado de deterioro considerable, careciendo de las medidas de accesibilidad necesarias para su uso público. Ante tal situación y con el fin de evitar que el espacio sea ocupado y vandalizado, el objetivo principal de la Junta Municipal de San Blas-Canillejas es volver a ponerlo en uso, reconvirtiéndolo en un Centro Social. Para ello los Servicios Técnicos de la Junta Municipal de Distrito han llevado a cabo una reforma parcial de las instalaciones interiores, no alcanzando con ellas a cubrir el total de las necesarias para la puesta en uso del Edificio B.\nCon el presente contrato, la Empresa Municipal de la Vivienda y Suelo de Madrid pretende llevar a cabo las obras de instalación del ascensor de tal manera que se pueda garantizar el uso del edifico en condiciones de accesibilidad universal. Para ello, se prevé la instalación de un ascensor anexo a la fachada testera orientada al Oeste, para lo que será necesaria la demolición parcial de esa misma fachada. La instalación no afecta a la estructura del edificio ni a su distribución funcional. Para la correcta instalación del ascensor se ha redactado por el Departamento de Rehabilitación de la EMVS, Proyecto de Ejecución para la Instalación de Ascensor, de acuerdo a la normativa técnica y administrativa de aplicación\n', 'El objeto del contrato son las obras de reparación de filtraciones y otros trabajos correctivos en el Centro Comercial Opción de Gijón.\nDe cara a la presente licitación, en una primera fase (FASE 0), se han localizado los siguientes ámbitos de intervención en el edificio:\n\uf0b7 Acceso de uso público por la calle General Suárez Valdés.\n\uf0b7 Acceso de uso público por el aparcamiento del centro comercial.\n\uf0b7 Interior de locales del centro comercial.\nLas intervenciones proyectadas consisten en:\n\uf0b7 Actuaciones previas de liberación de espacios de trabajo\n\uf0b7 Reparaciones en cubiertas del edificio.\n\uf0b7 Impermeabilización mediante tratamiento por el interior de forjado de hormigón\n\uf0b7 Sistema de recogida de agua y evacuación\n\uf0b7 Reposición de revestimientos a situación original\n\uf0b7 Pinturas de revestimientos repuestos.\n\uf0b7 Trabajos de corrección de deficiencias en pasos de instalaciones por sectores de incendios\n\uf0b7 Trabajos de desmontaje de falsos techos y liberación de áreas de trabajo en forjado para tercera empresa. Posterior restitución a situación original de elementos desmontados.\nEn fases posteriores a la ejecución de las reparaciones reseñadas, se requiere la ejecución de unos trabajos de control técnico de las reparaciones efectuadas y de la estanquidad de la envolvente del edificio en lo relativo a sus condiciones de protección frente a la humedad e identificación de filtraciones de agua de los cerramientos del edificio, con la visita de personal técnico y operarios para su corrección inmediata. Estos trabajos se contemplan de forma periódica o a demanda durante el periodo de duración del contrato.', 'Realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de Prodetur en Calle Leonardo Da Vinci nº 16 de Sevilla.El presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: Los equipos de ventilación proyectados serán de la marca ¿Soler &amp;Palau¿ modelo CHAT/4/560N o similar. La instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de CO y posibilitar la puesta en funcionamiento manualmente. La central de detección de CO se instalará en el cuarto de instalaciones de la planta baja. La entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. Todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. Se adjunta plano de la instalación propuesta. Se adjunta medición de la instalación propuesta para su presupuestación.']</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>['Pavimentación de los siguientes caminos municipales: 1.- Acceso a Remesar 1; 2.- Acceso a Remesar 2; 3.- Camino del límite municipal a la LU-611 por Portaxe; 4.- Camino de la LU-611 la La Reina; 5.- Camino de la LU-0903 a la LU-0905; 6.- Camino de la LU-0903 a Outeiro; 7.- Camino de Lamela a Ver; 8.- Camino de la Avda. Alfonso XIII a Camino del Canal; 9.- Camino de acceso a Ver; 10.- Camino de Ribas Pequeñas a Chorente; 11.- Camino de Acceso a Guntín y 12.- Camino de Vilaboa a Xulián', 'Obras para la reparación de los siguientes caminos: Camino de los Furtivos, Camino de la Cebadilla al Porche de Alfredo, Camino Majadales, Camino de la Raña del Quinto, Camino de Portejuelo al Morrillo, Camino de las Navas 1, Camino de las Navas 2, Camino Miraflores, Camino Rubiastro, Camino las Larguillas y Camino Posada de Aguedillo.', 'Mejora de la capa de rodaje de los caminos: Lote 1: camino en Señorín (Camanzo), camino en Cirela (Gres), camino en Lareo (Salgueiros), caminos en Pastoriza (Carbia), caminos en Fondevila y Los Maestros (Bascuas) y camino en Obra (Santomé de Obra). Lote 2: camino en Oirós, camino en Castro (Besexos), Rúa Covas y Rúa Pendiente (Las Cruces), camino en Loño, camino en Outeiro (Portodemouros), en el Ayuntamiento de Vila de Cruces. ']</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>0.3647910853226979</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.4457691013813019</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.3845249613126119</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.4437437653541565</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>['tramo', 'carretera', 'provincia', 'reparación', 'firme', 'acceso', 'construcción', 'término_municipal', 'acondicionamiento', 'drenaje', 'autovía', 'punto_kilométrico', 'rehabilitación_superficial', 'firme_carretera', 'túnel']</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Road Construction and Maintenance Project</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>['tramo', 'carretera', 'pk', 'construcción', 'reparación', 'acceso', 'obras', 'mejorar', 'vial', 'firme_carretera', 'vía', 'rehabilitación_superficial', 'túnel', 'firme', 'estación']</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Road Construction and Improvement Project</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>['Proyecto Renovación de Instalaciones de Alumbrado Público Exterior en Polígono Industrial y Casco Urbano de Manzanares dentro del Plan Provincial Ciudad Real por una Economía Baja en Carbono (Fase IIB) cofinanciado por el Fondo Europeo de Desarrollo Rural en el marco del Programa Operativo FEDER de crecimiento sostenible 2014/2020', 'Obra de Mejoras Infraestructuras en Obando: c/ Alba, c/ Ronda Saliente y c/ San Jose. Plan Cohesiona 2020', 'Ejecución de la red de saneamiento en Palmés. Tramo: O Burgo-A Burata. Ourense.OH.332.823. El objeto de esta contratación se cofinanciará por la Unión Europea a través del Fondo Europeo Agrícola de Desarrollo Rural (FEADER) en un 75% del gasto elexible, en el marco del Programa de Desarrollo Rural (PDR) Galicia 2014-2020. La actuación se enmarca dentro del Programa de Desarrollo Rural en la Medida 07 Servicios básicos y renovación de poblaciones en zonas rurales , Submedida 7.2 Apoyo a las inversiones en la creación, mejora o ampliación de todo tipo de pequeñas infraestructuras, incluidos las inversiones en energías renovables y ahorro energético y Prioridad 6 de Desarrollo Rural Fomentar la inclusión social, la reducción de la pobreza y el desarrollo económico en las zonas rurales . Europa invierte en el rural. Procedimiento documentalmente simplificado. ']</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>['el objeto la de definir la actuación proyectada para la mejora de la carretera que une el núcleo urbano de notáez con la carretera autonómica a-348, todo ello perteneciente al municipio de almegíjar. la carretera, que se pretende mejorar con la actuación y que se describe en el presente documento se encuentra en el término municipal de almegíjar. \nlas necesidades básicas a satisfacer son:\nlimpiar los arrastres existentes en las cunetas de la carretera que afectan a la circulación reduciendo la anchura efectiva de la calzada\n\nconstrucción de cunetas para desarrollen la misión de evacuación de las aguas de la carretera .en caso contrario la existencia de escorrentías en los márgenes de la carretera llevaría a la aparición de socavones laterales.\nrepaso de todos aquellos tramos de cunetas revestidas que se encuentran en mal estado, que redundara en la vida útil de la carretera, reducirá los costes de mantenimiento y roturas de vehículos en los usuarios habituales de la carretera.\n', 'contrato de obra de asfaltado viarios públicos, renovación de aceras y carril bici:\n(1) asfaltado calle vicente soriano – calle cementerio, calle pobla de farnals, calle san isidro (tramo entre calle bobalar y diputación provincial), calle mártires (tramo entre calle josé mª llopis y comunidad valenciana), calle rei en jaume (tramo entre calle josé mª llopis y comunidad valenciana), calle camí fondo (tramo entre la avenida sant pere y la calle sagunto), av. sant pere este (tramo parcial entre calle camí fondo y josé mª llopis), av. sant pere este (tramo parcial entre calle josé mª llopis y comunidad valenciana) y calle castellón (tramo entre calle josé mª llopis y comunidad valenciana).\n(2) renovación de la acera oeste de la calle mártires y la calle vicente soriano lado barranco y la nueva ejecución de la acera norte y oeste del polideportivo paco camarasa (calle vicente soriano y calle del cementerio). \n(3) carril bici en el lado barranco de la calle vicente soriano.', 'las obras consisten principalmente en el pavimentado con triple tratamiento superficial, salvo en un pequeño tramo, en el que debido a una fuerte pendiente el pavimento es de hormigón de un tramo de la pista que se encuentra muy deteriorado y que sirve de acceso a múltiples fincas y es camino habitual de ganado hacia los pastos.\nel desarrollo de la intervención pretende ser un impulso del sector primario ya que el camino es fundamental para el tránsito de numerosas cabezas de ganado que utilizan estas vías en busca de pastos en épocas estivales, así como para los propios ganaderos para actividades complementarias del sector.\nlas obras comprenden la pavimentación de una pista situada al sur de puentenansa, con una longitud aproximada de 3.000 metrosse distinguen dos tramos, con pavimentación de distintas características. partiendo del entorno de puentenansa, el primer tramo de pista se acondiciona con pavimento de hormigón, la longitud aproximada de tramo es de 200 metros, con un ancho medio de 3.50 m. en este tramo se realiza una limpieza de la traza, eliminando los restos de vegetación y residuos presentes de la misma. tras la limpieza se lleva a cabo una excavación de saneo de 15 cm de espesor, compactando con la superficie final. se extiende sobre la superficie preparada una capa de base de zahorra artificial de 5 cm, de espesor y sobre ésta una capa de 13 cm de espesor de hormgión rayado y estriado ha25, mallazo de 3 kg/ m2.']</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>['servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales', 'realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'servicio y suministro para el mantenimiento del alumbrado público, de edificios e instalaciones en general y para fiestas y actos culturales del ayuntamiento de santoña, con el fin de conservar las instalaciones en perfecto estado, manteniendo el nivel técnico alcanzado, minimizar los posibles riesgos a las personas, cosas o animales, incluyendo el servicio de control y funcionamiento, tanto de las instalaciones existentes, como de aquellas otras que se efectúen durante la vigencia del contrato, con arreglo a las condiciones que en su caso se señalen.\n\nel ámbito de aplicación de este contrato, se extiende a todos las instalaciones eléctricas que el ayuntamiento tiene para alumbrado público, iluminación artística además del mantenimiento de las instalaciones eléctricas de los edificios, oficinas y pabellones municipales.\n']</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>['Obra de Mejoras Infraestructuras en Obando: c/ Alba, c/ Ronda Saliente y c/ San Jose. Plan Cohesiona 2020', 'Proyecto Renovación de Instalaciones de Alumbrado Público Exterior en Polígono Industrial y Casco Urbano de Manzanares dentro del Plan Provincial Ciudad Real por una Economía Baja en Carbono (Fase IIB) cofinanciado por el Fondo Europeo de Desarrollo Rural en el marco del Programa Operativo FEDER de crecimiento sostenible 2014/2020', 'Plan renove en polígonos industriales-urbanización repavimentación, nuevo pintado, señalización y colocación de mobiliario en los polígonos Industrialdea y Arza']</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>['Contrato de obra de asfaltado viarios públicos, renovación de aceras y carril bici:\n(1) Asfaltado Calle Vicente Soriano – calle Cementerio, calle Pobla de Farnals, calle San Isidro (tramo entre calle Bobalar y Diputación Provincial), calle Mártires (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Rei en Jaume (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Camí Fondo (tramo entre la avenida Sant Pere y la calle Sagunto), av. Sant Pere este (tramo parcial entre calle Camí Fondo y José Mª Llopis), av. Sant Pere este (tramo parcial entre calle José Mª Llopis y Comunidad Valenciana) y calle Castellón (tramo entre calle José Mª Llopis y Comunidad Valenciana).\n(2) Renovación de la acera oeste de la calle Mártires y la calle Vicente Soriano lado barranco y la nueva ejecución de la acera norte y oeste del polideportivo Paco Camarasa (calle Vicente Soriano y calle del Cementerio). \n(3) Carril bici en el lado barranco de la calle Vicente Soriano.', 'El objeto la de definir la actuación proyectada para la mejora de la carretera que une el núcleo Urbano de Notáez con la carretera autonómica A-348, todo ello perteneciente al municipio de Almegíjar. La carretera, que se pretende mejorar con la actuación y que se describe en el presente documento se encuentra en el término municipal de Almegíjar. \nLas necesidades básicas a satisfacer son:\nLimpiar los arrastres existentes en las cunetas de la carretera que afectan a la circulación reduciendo la anchura efectiva de la calzada\n\nConstrucción de cunetas para desarrollen la misión de evacuación de las aguas de la carretera .En caso contrario la existencia de escorrentías en los márgenes de la carretera llevaría a la aparición de socavones laterales.\nRepaso de todos aquellos tramos de cunetas revestidas que se encuentran en mal estado, que redundara en la vida útil de la carretera, reducirá los costes de mantenimiento y roturas de vehículos en los usuarios habituales de la carretera.\n', 'Las obras consisten principalmente en el pavimentado con triple tratamiento superficial, salvo en un pequeño tramo, en el que debido a una fuerte pendiente el pavimento es de hormigón de un tramo de la pista que se encuentra muy deteriorado y que sirve de acceso a múltiples fincas y es camino habitual de ganado hacia los pastos.\nEl desarrollo de la intervención pretende ser un impulso del sector primario ya que el camino es fundamental para el tránsito de numerosas cabezas de ganado que utilizan estas vías en busca de pastos en épocas estivales, así como para los propios ganaderos para actividades complementarias del sector.\nLas obras comprenden la pavimentación de una pista situada al sur de Puentenansa, con una longitud aproximada de 3.000 metrosSe distinguen dos tramos, con pavimentación de distintas características. Partiendo del entorno de Puentenansa, el primer tramo de pista se acondiciona con pavimento de hormigón, la longitud aproximada de tramo es de 200 metros, con un ancho medio de 3.50 m. En este tramo se realiza una limpieza de la traza, eliminando los restos de vegetación y residuos presentes de la misma. Tras la limpieza se lleva a cabo una excavación de saneo de 15 cm de espesor, compactando con la superficie final. Se extiende sobre la superficie preparada una capa de base de zahorra artificial de 5 cm, de espesor y sobre ésta una capa de 13 cm de espesor de hormgión rayado y estriado HA25, mallazo de 3 kg/ m2.']</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>['Pavimentación de los siguientes caminos municipales: 1.- Acceso a Remesar 1; 2.- Acceso a Remesar 2; 3.- Camino del límite municipal a la LU-611 por Portaxe; 4.- Camino de la LU-611 la La Reina; 5.- Camino de la LU-0903 a la LU-0905; 6.- Camino de la LU-0903 a Outeiro; 7.- Camino de Lamela a Ver; 8.- Camino de la Avda. Alfonso XIII a Camino del Canal; 9.- Camino de acceso a Ver; 10.- Camino de Ribas Pequeñas a Chorente; 11.- Camino de Acceso a Guntín y 12.- Camino de Vilaboa a Xulián', 'Obras para la reparación de los siguientes caminos: Camino de los Furtivos, Camino de la Cebadilla al Porche de Alfredo, Camino Majadales, Camino de la Raña del Quinto, Camino de Portejuelo al Morrillo, Camino de las Navas 1, Camino de las Navas 2, Camino Miraflores, Camino Rubiastro, Camino las Larguillas y Camino Posada de Aguedillo.', 'Mejora de la capa de rodaje de los caminos: Lote 1: camino en Señorín (Camanzo), camino en Cirela (Gres), camino en Lareo (Salgueiros), caminos en Pastoriza (Carbia), caminos en Fondevila y Los Maestros (Bascuas) y camino en Obra (Santomé de Obra). Lote 2: camino en Oirós, camino en Castro (Besexos), Rúa Covas y Rúa Pendiente (Las Cruces), camino en Loño, camino en Outeiro (Portodemouros), en el Ayuntamiento de Vila de Cruces. ']</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
+        <v>0.50850710272789</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.4311296939849854</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.4898371895154317</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.4246482153733571</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>11</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>['restauración', 'actuación', 'municipal', 'construcción', 'fase', 'término_municipal', 'urbanización', 'conservación', 'edificio', 'rehabilitación', 'acondicionamiento', 'parcela', 'zona', 'adecuación', 'sito']</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Urban Development and Construction Project Management</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>6</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>['obras', 'construcción', 'proyecto', 'fase', 'calle', 'restauración', 'edificio', 'contrato', 'urbanización', 'parcela', 'rehabilitación', 'ejecución', 'zona', 'acondicionamiento', 'situado']</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Urban Development Project Management</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>['Servicio Mtto. Y Conservación De Edificios Y Sus Instalaciones Así Como De Accesos, Aparcam., Urbanizac. Y Área De Movimiento Del Recinto Aeroportuari', 'Urbanización de cl. san Jose en el marco de la convocatoria para la ejecución de obras comprendidas entre los objetivos de desarrollo sostenbile "reactivem castelló" obres ejercicio 2021.La obra pretende integrar la pavimentación ordenada que se ha llevado a cabo\nen Forcall, mediante adoquines de Hormigón tomados con arena, sobre una base de Hormigón HN 150. La obra permite restituir las trapas particulares de alcantarillado y agua potable, sustituyéndolas por trapas de fundición de mejor durabilidad y que quedan integradas en el pavimento. La obra permitirá la sustitución de un tramo de conducto de saneamiento entre los pozos de la C/ Tomas Salvador y viviendas de la C/ Sant Josep , con el fin de adecuar la red de saneamiento.', 'Servicio de albañilería, carpintería, revestimientos y trabajos de fontanería y saneamiento para el mantenimiento de los Ed. Administrativos Municipales']</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>['tal y como se especifica en el proyecto básico y de ejecución de las obras de restauración del conjunto monumental del castillo de castelló de farfanya, redactado por el equipo de la empresa ianua arquitectures, s.c.p., la obra comprende:\na) "recinto superior" del castillo. la propuesta pretende recuperar el perímetro murario del recinto, mediante la recuperación del nivel de uso interior y la consolidación de la muralla.\nmediante la consolidación, que no reconstrucción, será posible dotar al castillo de nuevo de la imagen como tal, tanto interior como exteriormente.\nb) murallas sur y este. coracha (apéndice de la muralla) hasta la torre sur. la muralla este, que cierra el recinto de la zona del cementerio, colapsó en el año 2018. esta es una zona alejada del castillo pero que requiere su reconstrucción para la seguridad de la zona de acceso peatonal y del este del foso.\nla muralla sur actualmente está sufriendo un proceso de degradación de la base, y algunas zonas se encuentra descalzada de la roca madre, muy estratificada. la zona sur se conecta con la torre sur mediante la coracha, actualmente en ruinas.\nhay material fotográfico que permite reconstruir este elemento, muy peculiar y que permitirá una explicación fácil del carácter defensivo de las estructuras.\nc) mejora del acceso peatonal desde la calle del castillo hasta la sala de caballerías. en la actuación de consolidación de murallas y recuperación de niveles, se perderá el acceso actual al recinto mediante un derribo en la zona norte; la propuesta plantea la recuperación del acceso por la cara sur de la muralla, mediante una pasarela de acceso que permita la entrada de la manera más accesible posible. el resto de esta actuación contempla una mínima actuación de mejora del acceso peatonal desde el núcleo habitado, actualmente un camino de difícil tráfico.', 'el objeto del contrato son las obras de reparación de filtraciones y otros trabajos correctivos en el centro comercial opción de gijón.\nde cara a la presente licitación, en una primera fase (fase 0), se han localizado los siguientes ámbitos de intervención en el edificio:\n\uf0b7 acceso de uso público por la calle general suárez valdés.\n\uf0b7 acceso de uso público por el aparcamiento del centro comercial.\n\uf0b7 interior de locales del centro comercial.\nlas intervenciones proyectadas consisten en:\n\uf0b7 actuaciones previas de liberación de espacios de trabajo\n\uf0b7 reparaciones en cubiertas del edificio.\n\uf0b7 impermeabilización mediante tratamiento por el interior de forjado de hormigón\n\uf0b7 sistema de recogida de agua y evacuación\n\uf0b7 reposición de revestimientos a situación original\n\uf0b7 pinturas de revestimientos repuestos.\n\uf0b7 trabajos de corrección de deficiencias en pasos de instalaciones por sectores de incendios\n\uf0b7 trabajos de desmontaje de falsos techos y liberación de áreas de trabajo en forjado para tercera empresa. posterior restitución a situación original de elementos desmontados.\nen fases posteriores a la ejecución de las reparaciones reseñadas, se requiere la ejecución de unos trabajos de control técnico de las reparaciones efectuadas y de la estanquidad de la envolvente del edificio en lo relativo a sus condiciones de protección frente a la humedad e identificación de filtraciones de agua de los cerramientos del edificio, con la visita de personal técnico y operarios para su corrección inmediata. estos trabajos se contemplan de forma periódica o a demanda durante el periodo de duración del contrato.', 'el objeto del contrato viene motivado por la adecuación y puesta en uso del edificio b como centro social, dependiente de la junta municipal de distrito de san blas canillejas. hasta la fecha, este edificio lleva varios años sin funcionamiento y presenta un grado de deterioro considerable, careciendo de las medidas de accesibilidad necesarias para su uso público. ante tal situación y con el fin de evitar que el espacio sea ocupado y vandalizado, el objetivo principal de la junta municipal de san blas-canillejas es volver a ponerlo en uso, reconvirtiéndolo en un centro social. para ello los servicios técnicos de la junta municipal de distrito han llevado a cabo una reforma parcial de las instalaciones interiores, no alcanzando con ellas a cubrir el total de las necesarias para la puesta en uso del edificio b.\ncon el presente contrato, la empresa municipal de la vivienda y suelo de madrid pretende llevar a cabo las obras de instalación del ascensor de tal manera que se pueda garantizar el uso del edifico en condiciones de accesibilidad universal. para ello, se prevé la instalación de un ascensor anexo a la fachada testera orientada al oeste, para lo que será necesaria la demolición parcial de esa misma fachada. la instalación no afecta a la estructura del edificio ni a su distribución funcional. para la correcta instalación del ascensor se ha redactado por el departamento de rehabilitación de la Empresa Municipal de la Vivienda y Suelo de Madrid, proyecto de ejecución para la instalación de ascensor, de acuerdo a la normativa técnica y administrativa de aplicación\n']</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>['servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales', 'realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'servicio y suministro para el mantenimiento del alumbrado público, de edificios e instalaciones en general y para fiestas y actos culturales del ayuntamiento de santoña, con el fin de conservar las instalaciones en perfecto estado, manteniendo el nivel técnico alcanzado, minimizar los posibles riesgos a las personas, cosas o animales, incluyendo el servicio de control y funcionamiento, tanto de las instalaciones existentes, como de aquellas otras que se efectúen durante la vigencia del contrato, con arreglo a las condiciones que en su caso se señalen.\n\nel ámbito de aplicación de este contrato, se extiende a todos las instalaciones eléctricas que el ayuntamiento tiene para alumbrado público, iluminación artística además del mantenimiento de las instalaciones eléctricas de los edificios, oficinas y pabellones municipales.\n']</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>['Servicio Mtto. Y Conservación De Edificios Y Sus Instalaciones Así Como De Accesos, Aparcam., Urbanizac. Y Área De Movimiento Del Recinto Aeroportuari', 'Urbanización de cl. san Jose en el marco de la convocatoria para la ejecución de obras comprendidas entre los objetivos de desarrollo sostenbile "reactivem castelló" obres ejercicio 2021.La obra pretende integrar la pavimentación ordenada que se ha llevado a cabo\nen Forcall, mediante adoquines de Hormigón tomados con arena, sobre una base de Hormigón HN 150. La obra permite restituir las trapas particulares de alcantarillado y agua potable, sustituyéndolas por trapas de fundición de mejor durabilidad y que quedan integradas en el pavimento. La obra permitirá la sustitución de un tramo de conducto de saneamiento entre los pozos de la C/ Tomas Salvador y viviendas de la C/ Sant Josep , con el fin de adecuar la red de saneamiento.', 'Servicio de albañilería, carpintería, revestimientos y trabajos de fontanería y saneamiento para el mantenimiento de los Ed. Administrativos Municipales']</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>['Contrato de obra de asfaltado viarios públicos, renovación de aceras y carril bici:\n(1) Asfaltado Calle Vicente Soriano – calle Cementerio, calle Pobla de Farnals, calle San Isidro (tramo entre calle Bobalar y Diputación Provincial), calle Mártires (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Rei en Jaume (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Camí Fondo (tramo entre la avenida Sant Pere y la calle Sagunto), av. Sant Pere este (tramo parcial entre calle Camí Fondo y José Mª Llopis), av. Sant Pere este (tramo parcial entre calle José Mª Llopis y Comunidad Valenciana) y calle Castellón (tramo entre calle José Mª Llopis y Comunidad Valenciana).\n(2) Renovación de la acera oeste de la calle Mártires y la calle Vicente Soriano lado barranco y la nueva ejecución de la acera norte y oeste del polideportivo Paco Camarasa (calle Vicente Soriano y calle del Cementerio). \n(3) Carril bici en el lado barranco de la calle Vicente Soriano.', 'Ejecución de las Obras del: Proyecto de Construcción de ampliación y remodelación de la playa de vía y andenes de alta velocidad y del edificio de viajeros de la Estación de Chamartín (Madrid); Proyecto de Construcción del nuevo edificio técnico dealta velocidad en la cabecera norte de la Estación de Madrid-Chamartín; Proyecto de Construcción de conexión del vestíbulo de cercanías bajo vías con metro y futuro paso inferior de alta velocidad de la Estación de Madrid-Chamartín; Proyecto de Construcción de cimentaciones y pilas del lateral este (C/Hiedra) del cubrimiento de la Cabecera Sur de la Estación de Chamartín y Proyecto de Construcción para la demolición del Edificio 23 de la Estación de Madrid-Chamartín-Clara Campoamor y la reordenación del espacio liberado. Fase I', 'El objeto del presente Contrato consiste en la ejecución de las obras de restauración de los arroyos Prado Chico y Prado Grande y construcción de tanques de laminación de aguas pluviales en el entorno del sector AH-31 (antiguo sector 6.1 Cortijo Sur) en Boadilla del Monte (Madrid), conforme a los siguientes Proyectos (conjuntamente el “Proyecto” o el “Proyecto de Ejecución”): \r\ni.\t“Proyecto de restauración de los arroyos Prado Chico y Prado Grande en el entorno del sector AH-31 (antiguo sector 6.1 Cortijo Sur) de Boadilla del Monte”, redactado por el Ingeniero de Caminos, Canales y Puertos D. Fernando González García con número de colegiado 16.867.\r\nii.\t“Proyecto de Tanques de laminación de aguas pluviales en Urbanización AH-31 (antiguo sector 6.1 Cortijo Sur) Boadilla del Monte”, redactado por el Ingeniero de Caminos, Canales y Puertos D. Alberto Lozano Carreras, con número de colegiado 6.362.\r\n\r\nEl Proyecto engloba las Obras relacionadas con las Obras de Drenaje Transversal de los Arroyos Prado Grande y Prado Chico, demoliciones, movimientos de tierras, estabilización de taludes, revegetación, tanques de laminación y puntos de vertido de aguas pluviales aprobados por la Confederación Hidrográfica del Tajo (ver Documento n.º 4 del Anexo I del Anexo Técnico), así como las obras necesarias para la consecución de la Conformidad Técnica por parte de Canal de Isabel II, S.A. (“CYII”) de los estanques de tormentas (ver Documento n.º 5 del Anexo I del Anexo Técnico).\r\n\r\n']</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>['Pavimentación de los siguientes caminos municipales: 1.- Acceso a Remesar 1; 2.- Acceso a Remesar 2; 3.- Camino del límite municipal a la LU-611 por Portaxe; 4.- Camino de la LU-611 la La Reina; 5.- Camino de la LU-0903 a la LU-0905; 6.- Camino de la LU-0903 a Outeiro; 7.- Camino de Lamela a Ver; 8.- Camino de la Avda. Alfonso XIII a Camino del Canal; 9.- Camino de acceso a Ver; 10.- Camino de Ribas Pequeñas a Chorente; 11.- Camino de Acceso a Guntín y 12.- Camino de Vilaboa a Xulián', 'Obras para la reparación de los siguientes caminos: Camino de los Furtivos, Camino de la Cebadilla al Porche de Alfredo, Camino Majadales, Camino de la Raña del Quinto, Camino de Portejuelo al Morrillo, Camino de las Navas 1, Camino de las Navas 2, Camino Miraflores, Camino Rubiastro, Camino las Larguillas y Camino Posada de Aguedillo.', 'Mejora de la capa de rodaje de los caminos: Lote 1: camino en Señorín (Camanzo), camino en Cirela (Gres), camino en Lareo (Salgueiros), caminos en Pastoriza (Carbia), caminos en Fondevila y Los Maestros (Bascuas) y camino en Obra (Santomé de Obra). Lote 2: camino en Oirós, camino en Castro (Besexos), Rúa Covas y Rúa Pendiente (Las Cruces), camino en Loño, camino en Outeiro (Portodemouros), en el Ayuntamiento de Vila de Cruces. ']</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
+        <v>0.4859902064005534</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.5028857787450155</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.5218415757020315</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.4859175682067871</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>12</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>['edificio', 'centro', 'reforma', 'adecuación', 'instalación', 'servicio', 'planta', 'local', 'acondicionamiento', 'plantar', 'oficina', 'reparación', 'rehabilitación', 'hospital_universitario', 'ampliación']</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Building Renovation and Expansion Project</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>7</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>['instalación', 'adecuación', 'obra', 'reforma', 'sala', 'obras', 'edificio', 'sustitución', 'hospital', 'hospital_universitario', 'suministro', 'centro', 'sistema', 'climatización', 'servicio']</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Building Renovation and Hospital Upgrades</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>['Obra de Mejoras Infraestructuras en Obando: c/ Alba, c/ Ronda Saliente y c/ San Jose. Plan Cohesiona 2020', 'Trabajos de acondic. vvda. Retirada de enseres existentes, i/transporte a punto de reciclaje. Tapado de hueco existente techo. Pintura general en paramentos horizontales y verticales. Limpieza general. Equipamiento mín. cocina. Revisión instalaciones.', 'Trabajos de acondicionamiento de vivienda: limpieza general. Sum. y colocación eq. mínimo cocina. Pintura param. hor. y vert. Sum. e instalac. ap. sanitarios. Arreglo carpinterías. Revisión instalaciones existentes.']</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>['el objeto del contrato viene motivado por la adecuación y puesta en uso del edificio b como centro social, dependiente de la junta municipal de distrito de san blas canillejas. hasta la fecha, este edificio lleva varios años sin funcionamiento y presenta un grado de deterioro considerable, careciendo de las medidas de accesibilidad necesarias para su uso público. ante tal situación y con el fin de evitar que el espacio sea ocupado y vandalizado, el objetivo principal de la junta municipal de san blas-canillejas es volver a ponerlo en uso, reconvirtiéndolo en un centro social. para ello los servicios técnicos de la junta municipal de distrito han llevado a cabo una reforma parcial de las instalaciones interiores, no alcanzando con ellas a cubrir el total de las necesarias para la puesta en uso del edificio b.\ncon el presente contrato, la empresa municipal de la vivienda y suelo de madrid pretende llevar a cabo las obras de instalación del ascensor de tal manera que se pueda garantizar el uso del edifico en condiciones de accesibilidad universal. para ello, se prevé la instalación de un ascensor anexo a la fachada testera orientada al oeste, para lo que será necesaria la demolición parcial de esa misma fachada. la instalación no afecta a la estructura del edificio ni a su distribución funcional. para la correcta instalación del ascensor se ha redactado por el departamento de rehabilitación de la Empresa Municipal de la Vivienda y Suelo de Madrid, proyecto de ejecución para la instalación de ascensor, de acuerdo a la normativa técnica y administrativa de aplicación\n', 'el objeto del contrato son las obras de reparación de filtraciones y otros trabajos correctivos en el centro comercial opción de gijón.\nde cara a la presente licitación, en una primera fase (fase 0), se han localizado los siguientes ámbitos de intervención en el edificio:\n\uf0b7 acceso de uso público por la calle general suárez valdés.\n\uf0b7 acceso de uso público por el aparcamiento del centro comercial.\n\uf0b7 interior de locales del centro comercial.\nlas intervenciones proyectadas consisten en:\n\uf0b7 actuaciones previas de liberación de espacios de trabajo\n\uf0b7 reparaciones en cubiertas del edificio.\n\uf0b7 impermeabilización mediante tratamiento por el interior de forjado de hormigón\n\uf0b7 sistema de recogida de agua y evacuación\n\uf0b7 reposición de revestimientos a situación original\n\uf0b7 pinturas de revestimientos repuestos.\n\uf0b7 trabajos de corrección de deficiencias en pasos de instalaciones por sectores de incendios\n\uf0b7 trabajos de desmontaje de falsos techos y liberación de áreas de trabajo en forjado para tercera empresa. posterior restitución a situación original de elementos desmontados.\nen fases posteriores a la ejecución de las reparaciones reseñadas, se requiere la ejecución de unos trabajos de control técnico de las reparaciones efectuadas y de la estanquidad de la envolvente del edificio en lo relativo a sus condiciones de protección frente a la humedad e identificación de filtraciones de agua de los cerramientos del edificio, con la visita de personal técnico y operarios para su corrección inmediata. estos trabajos se contemplan de forma periódica o a demanda durante el periodo de duración del contrato.', 'el presente contrato basado tiene por objeto la ejecución de las obras que se detallan en las edificaciones de centros educativos, edificios municipales, polideportivos e\ninstalaciones deportivas elementales así como en los espacios libres de parcela de dichas edificaciones, zonas verdes y obras en vía pública cuya competencia\ncorresponda al distrito, siempre que estén destinados al funcionamiento operativo de los servicios y/o al uso público; con el fin de satisfacer las necesidades detectadas por el servicio de medio ambiente y escena urbana del distrito centro, a través de la recopilación de observaciones realizadas por las dependencias usuarias de los centros, las inspecciones periódicas reglamentarias realizadas y como consecuencia del control de las labores de mantenimiento preventivo y correctivo de los centros. ejecución de obras de adecuación de edificio para centro social comunitario casa del cura en la infraestructura del distrito centro denominada casa del cura, en la parcela dos de mayo 1.']</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>['servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales', 'realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'servicio y suministro para el mantenimiento del alumbrado público, de edificios e instalaciones en general y para fiestas y actos culturales del ayuntamiento de santoña, con el fin de conservar las instalaciones en perfecto estado, manteniendo el nivel técnico alcanzado, minimizar los posibles riesgos a las personas, cosas o animales, incluyendo el servicio de control y funcionamiento, tanto de las instalaciones existentes, como de aquellas otras que se efectúen durante la vigencia del contrato, con arreglo a las condiciones que en su caso se señalen.\n\nel ámbito de aplicación de este contrato, se extiende a todos las instalaciones eléctricas que el ayuntamiento tiene para alumbrado público, iluminación artística además del mantenimiento de las instalaciones eléctricas de los edificios, oficinas y pabellones municipales.\n']</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>['reforma parcial en las unidades de hospitalizacion 3.2 y 3.4 por el intecambio de ubicación fisica de las especialidades medicas de digestivo y otorrino-vascular en la panta tercera. tambien se incluye una pequeña reforma de espacio en la planta baja', 'Fase IV de desarrollo del proyecto de reforma global del Colegio Mayor Santa Cruz Femenino de la Universidad de Valladolid. Reforma de 20 dormitorios', 'Fase V de desarrollo del proyecto de reforma global del Colegio Mayor Santa Cruz Femenino de la Universidad de Valladolid. Reforma de 15 dormitorios']</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>['Realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de Prodetur en Calle Leonardo Da Vinci nº 16 de Sevilla.El presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: Los equipos de ventilación proyectados serán de la marca ¿Soler &amp;Palau¿ modelo CHAT/4/560N o similar. La instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de CO y posibilitar la puesta en funcionamiento manualmente. La central de detección de CO se instalará en el cuarto de instalaciones de la planta baja. La entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. Todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. Se adjunta plano de la instalación propuesta. Se adjunta medición de la instalación propuesta para su presupuestación.', 'El objeto del contrato menor está conformado por las siguientes prestaciones:\n\n•  Elaboración de proyecto técnico para la legalización de las instalaciones de Protección Contra Incendios resultantes tras la realización de las obras de reforma y el suministro de componentes, sistemas y equipos de protección contra incendios. Este servicio incluye los trámites administrativos necesarios ante la administración o entidad de control e inspección industrial competente.\n\n•  Ejecución de las obras de reforma para la adecuación del sistema de Protección Contra Incendios del edificio de tanatorio del Cementerio Jardín de Alcalá de Henares, a la normativa comunitaria y nacional vigente en materia de instalaciones de protección contra incendios y de industria. Las obras consistirán principalmente en acciones de instalación o montaje, con los trabajos complementarios que ello requiera, de sistemas, componentes y equipos de protección contra incendios.\n\n•  Suministro de los componentes, sistemas y equipos de protección contra incendios que sean precisos para adecuar las instalaciones de este tipo existentes actualmente en el edificio de tanatorio, a la normativa comunitaria y nacional vigente en materia de instalaciones de protección contra incendios y de industria. Todos los productos suministrados por la empresa adjudicataria a CEMENTERIO JARDÍN DE ALCALÁ DE HENARES, S.A. en virtud de este contrato serán propiedad de CEMENTERIO JARDÍN DE ALCALÁ DE HENARES, S.A. ', 'El objeto del contrato viene motivado por la adecuación y puesta en uso del Edificio B como Centro Social, dependiente de la Junta Municipal de Distrito de San Blas Canillejas. Hasta la fecha, este edificio lleva varios años sin funcionamiento y presenta un grado de deterioro considerable, careciendo de las medidas de accesibilidad necesarias para su uso público. Ante tal situación y con el fin de evitar que el espacio sea ocupado y vandalizado, el objetivo principal de la Junta Municipal de San Blas-Canillejas es volver a ponerlo en uso, reconvirtiéndolo en un Centro Social. Para ello los Servicios Técnicos de la Junta Municipal de Distrito han llevado a cabo una reforma parcial de las instalaciones interiores, no alcanzando con ellas a cubrir el total de las necesarias para la puesta en uso del Edificio B.\nCon el presente contrato, la Empresa Municipal de la Vivienda y Suelo de Madrid pretende llevar a cabo las obras de instalación del ascensor de tal manera que se pueda garantizar el uso del edifico en condiciones de accesibilidad universal. Para ello, se prevé la instalación de un ascensor anexo a la fachada testera orientada al Oeste, para lo que será necesaria la demolición parcial de esa misma fachada. La instalación no afecta a la estructura del edificio ni a su distribución funcional. Para la correcta instalación del ascensor se ha redactado por el Departamento de Rehabilitación de la EMVS, Proyecto de Ejecución para la Instalación de Ascensor, de acuerdo a la normativa técnica y administrativa de aplicación\n']</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>['Pavimentación de los siguientes caminos municipales: 1.- Acceso a Remesar 1; 2.- Acceso a Remesar 2; 3.- Camino del límite municipal a la LU-611 por Portaxe; 4.- Camino de la LU-611 la La Reina; 5.- Camino de la LU-0903 a la LU-0905; 6.- Camino de la LU-0903 a Outeiro; 7.- Camino de Lamela a Ver; 8.- Camino de la Avda. Alfonso XIII a Camino del Canal; 9.- Camino de acceso a Ver; 10.- Camino de Ribas Pequeñas a Chorente; 11.- Camino de Acceso a Guntín y 12.- Camino de Vilaboa a Xulián', 'Obras para la reparación de los siguientes caminos: Camino de los Furtivos, Camino de la Cebadilla al Porche de Alfredo, Camino Majadales, Camino de la Raña del Quinto, Camino de Portejuelo al Morrillo, Camino de las Navas 1, Camino de las Navas 2, Camino Miraflores, Camino Rubiastro, Camino las Larguillas y Camino Posada de Aguedillo.', 'Mejora de la capa de rodaje de los caminos: Lote 1: camino en Señorín (Camanzo), camino en Cirela (Gres), camino en Lareo (Salgueiros), caminos en Pastoriza (Carbia), caminos en Fondevila y Los Maestros (Bascuas) y camino en Obra (Santomé de Obra). Lote 2: camino en Oirós, camino en Castro (Besexos), Rúa Covas y Rúa Pendiente (Las Cruces), camino en Loño, camino en Outeiro (Portodemouros), en el Ayuntamiento de Vila de Cruces. ']</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>0.4751849472522736</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.4444780846436818</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.4501826663812001</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.3303233981132507</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
         <v>13</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>['mantenimiento_actualización', 'canal_comunicación', 'digital_teatro', 'arriaga_publicar', 'presente', 'accidente', 'asegurar', 'suscripción', 'póliza_seguro', 'vehículo', 'cobertura', 'mínimo', 'póliza', 'consideración_cobertura', 'aseguramiento']</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Vehicle Insurance Policy Consideration and Coverage Analysis</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>['instalación', 'servicio', 'suministro', 'mantenimiento', 'centro', 'municipal', 'material', 'alquiler', 'construcción', 'desmontaje', 'montaje', 'elemento', 'equipo', 'lote', 'montaje_desmontaje']</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Construction and Maintenance Services</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>9</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>['municipal', 'proyecto', 'redactado', 'calle', 'redactado_arquitecto', 'presente', 'denominado', 'ejecución', 'término_municipal', 'conformidad', 'reparación', 'pliego_prescripciones', 'acondicionamiento', 'consistente', 'construcción']</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Municipal Construction Project Planning and Execution</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>['Reforestación y labores auxiliares de parcelas reforestadas y áreas recreativas del T.M. de Ingenio (Fondo Verde Forestal 2018)', 'Construcción de laboratorios de fabricación aditiva, “Filler Functionalization” y electrónica, en la sede de la fundación IMDEA Materiales en tecnogetafe', 'Obras de reforma de áreas higiénicas para mejora de condiciones de accesibilidad y habitabilidad en varias viviendas municipales dispersas']</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>['servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales', 'realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'servicio y suministro para el mantenimiento del alumbrado público, de edificios e instalaciones en general y para fiestas y actos culturales del ayuntamiento de santoña, con el fin de conservar las instalaciones en perfecto estado, manteniendo el nivel técnico alcanzado, minimizar los posibles riesgos a las personas, cosas o animales, incluyendo el servicio de control y funcionamiento, tanto de las instalaciones existentes, como de aquellas otras que se efectúen durante la vigencia del contrato, con arreglo a las condiciones que en su caso se señalen.\n\nel ámbito de aplicación de este contrato, se extiende a todos las instalaciones eléctricas que el ayuntamiento tiene para alumbrado público, iluminación artística además del mantenimiento de las instalaciones eléctricas de los edificios, oficinas y pabellones municipales.\n']</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>['servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales', 'realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'servicio y suministro para el mantenimiento del alumbrado público, de edificios e instalaciones en general y para fiestas y actos culturales del ayuntamiento de santoña, con el fin de conservar las instalaciones en perfecto estado, manteniendo el nivel técnico alcanzado, minimizar los posibles riesgos a las personas, cosas o animales, incluyendo el servicio de control y funcionamiento, tanto de las instalaciones existentes, como de aquellas otras que se efectúen durante la vigencia del contrato, con arreglo a las condiciones que en su caso se señalen.\n\nel ámbito de aplicación de este contrato, se extiende a todos las instalaciones eléctricas que el ayuntamiento tiene para alumbrado público, iluminación artística además del mantenimiento de las instalaciones eléctricas de los edificios, oficinas y pabellones municipales.\n']</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>['Servicio de albañilería, carpintería, revestimientos y trabajos de fontanería y saneamiento para el mantenimiento de los Ed. Administrativos Municipales', 'Sustitución de puertas y ventanas del colegio público Baladre. Incluido en el Plan Municipal de Mantenimiento de Centros Educativos. Centro Escolar Baladre.', 'Pavimentación varias calles de la localidad: Calle San Isidro, Calle Escuelas, Calle Corrales, Avda. Nueva Jarilla, Calle José de Espronceda, Calle Ramón Campoamor, Calle Gustavo Adolfo Bécquer y Plaza El Roble. Plan Provincial de Cooperación a las obras y servicios de competencia municipal Plan ppcos 2022-2023\n']</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>['Contrato de obra de asfaltado viarios públicos, renovación de aceras y carril bici:\n(1) Asfaltado Calle Vicente Soriano – calle Cementerio, calle Pobla de Farnals, calle San Isidro (tramo entre calle Bobalar y Diputación Provincial), calle Mártires (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Rei en Jaume (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Camí Fondo (tramo entre la avenida Sant Pere y la calle Sagunto), av. Sant Pere este (tramo parcial entre calle Camí Fondo y José Mª Llopis), av. Sant Pere este (tramo parcial entre calle José Mª Llopis y Comunidad Valenciana) y calle Castellón (tramo entre calle José Mª Llopis y Comunidad Valenciana).\n(2) Renovación de la acera oeste de la calle Mártires y la calle Vicente Soriano lado barranco y la nueva ejecución de la acera norte y oeste del polideportivo Paco Camarasa (calle Vicente Soriano y calle del Cementerio). \n(3) Carril bici en el lado barranco de la calle Vicente Soriano.', 'El objeto del contrato al que se refiere el presente pliego, es devolver las características fundamentales como son la resistencia , seguridad y comodidad de un pavimento para tráfico rodado, las cuales se van perdiendo con el envejecimiento del firme, provocando un gran número de intervenciones de bacheo, con el consiguiente aumento del coste de mantenimiento, sin que estas operaciones consigan obtener resultados positivos cuando la superficie a bachear es superior a la del pavimento primitivo. Es por todo ello por lo que se decide actuar sobre dicho pavimento con una solución de tipo preventivo y aplicable a toda la superficie de una calle, o de forma parcial. En el Anexo al Proyecto, se detallan el listado de las calles que son objeto del presente proyecto, con su medición. Calles: Calle Santa María del Pino, Calle Nueva Jarilla, Calle Madrid, Calle Plaza el Roble, Calle Manzano, Calle Covidehur, Calle Miguel de Unamuno, Calle Sepúlveda, Calle Duero, Calle Dámaso Alonso, Calle Violeta, Calle Guadalcacín-La Rosa.', 'El objeto del presente Contrato consiste en la ejecución de las obras de restauración de los arroyos Prado Chico y Prado Grande y construcción de tanques de laminación de aguas pluviales en el entorno del sector AH-31 (antiguo sector 6.1 Cortijo Sur) en Boadilla del Monte (Madrid), conforme a los siguientes Proyectos (conjuntamente el “Proyecto” o el “Proyecto de Ejecución”): \r\ni.\t“Proyecto de restauración de los arroyos Prado Chico y Prado Grande en el entorno del sector AH-31 (antiguo sector 6.1 Cortijo Sur) de Boadilla del Monte”, redactado por el Ingeniero de Caminos, Canales y Puertos D. Fernando González García con número de colegiado 16.867.\r\nii.\t“Proyecto de Tanques de laminación de aguas pluviales en Urbanización AH-31 (antiguo sector 6.1 Cortijo Sur) Boadilla del Monte”, redactado por el Ingeniero de Caminos, Canales y Puertos D. Alberto Lozano Carreras, con número de colegiado 6.362.\r\n\r\nEl Proyecto engloba las Obras relacionadas con las Obras de Drenaje Transversal de los Arroyos Prado Grande y Prado Chico, demoliciones, movimientos de tierras, estabilización de taludes, revegetación, tanques de laminación y puntos de vertido de aguas pluviales aprobados por la Confederación Hidrográfica del Tajo (ver Documento n.º 4 del Anexo I del Anexo Técnico), así como las obras necesarias para la consecución de la Conformidad Técnica por parte de Canal de Isabel II, S.A. (“CYII”) de los estanques de tormentas (ver Documento n.º 5 del Anexo I del Anexo Técnico).\r\n\r\n']</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>['Pavimentación de los siguientes caminos municipales: 1.- Acceso a Remesar 1; 2.- Acceso a Remesar 2; 3.- Camino del límite municipal a la LU-611 por Portaxe; 4.- Camino de la LU-611 la La Reina; 5.- Camino de la LU-0903 a la LU-0905; 6.- Camino de la LU-0903 a Outeiro; 7.- Camino de Lamela a Ver; 8.- Camino de la Avda. Alfonso XIII a Camino del Canal; 9.- Camino de acceso a Ver; 10.- Camino de Ribas Pequeñas a Chorente; 11.- Camino de Acceso a Guntín y 12.- Camino de Vilaboa a Xulián', 'Obras para la reparación de los siguientes caminos: Camino de los Furtivos, Camino de la Cebadilla al Porche de Alfredo, Camino Majadales, Camino de la Raña del Quinto, Camino de Portejuelo al Morrillo, Camino de las Navas 1, Camino de las Navas 2, Camino Miraflores, Camino Rubiastro, Camino las Larguillas y Camino Posada de Aguedillo.', 'Mejora de la capa de rodaje de los caminos: Lote 1: camino en Señorín (Camanzo), camino en Cirela (Gres), camino en Lareo (Salgueiros), caminos en Pastoriza (Carbia), caminos en Fondevila y Los Maestros (Bascuas) y camino en Obra (Santomé de Obra). Lote 2: camino en Oirós, camino en Castro (Besexos), Rúa Covas y Rúa Pendiente (Las Cruces), camino en Loño, camino en Outeiro (Portodemouros), en el Ayuntamiento de Vila de Cruces. ']</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
+        <v>0.3340534716844559</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.3340534716844559</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.3595708360274633</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.4095899065335591</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>['fondo_europeo', 'cofinanciado_europeo', 'europeo_desarrollo', 'desarrollo_regional', 'actuación', 'instalación', 'rural', 'regional_fondo', 'regional', 'crecimiento', 'europeo_regional', 'urbano_integrado', 'renovación', 'energético', 'regional_crecimiento']</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Regional Development and Growth Initiatives</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>['europeo_desarrollo', 'programa_operativo', 'cofinanciado_fondo', 'feder', 'actuación', 'regional_feder', 'desarrollo_regional', 'fondo_europeo', 'plurirregional_españa', 'obras', 'proyecto', 'españa', 'instalación', 'edusi', 'cofinanciado']</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Regional Development Projects in Spain</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>['Obras correspondientes a la actuación C.P. SE-9108, mejora de firme P.P.K.K. 0+000 al 5+730, Programa de Red Viaria Provincial (PRVP). Eje estratégico de Acción Supramunicipal. Plan Provincial de Reactivación económica y social 2020/2021. (PLAN CONTIGO)', 'Obras correspondientes a la actuación C.P. SE-9108, mejora de firme P.P.K.K. 0+000 al 5+730, Programa de Red Viaria Provincial (PRVP). Eje estratégico de Acción Supramunicipal. Plan Provincial de Reactivación económica y social 2020/2021. (PLAN CONTIGO)', 'RENOVACION DE LA ILUMINACION ORNAMENTAL DE LOS MONUMENTOS MÁS REPRESENTATIVOS DE CARRIÓN DE LOS CONDES.\nProyecto subvencionado por el Programa de subvenciones a proyectos singulares de entidades locales que favorezcan el paso a una economía baja en carbono en el marco del programa operativo Fondo Europeo de Desarrollo Regional (FEDER) de crecimiento sostenible 2014-2020."Una manera de hacer Europa"\nMedida 6. Renovación de las instalaciones de alumbrado, iluminación y señalización exterior.']</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>['el objeto del contrato se descompone en :\n\n1.- certificado previo de la actuación exigido en las actuaciones con cargo al fondo europeo de desarrollo regional, dentro del programa para el desarrollo energético sostenible de andalucía en el período 2017-2020.\n\n2.- planificación, estudios de viabilidad, ingeniería, proyecto de ingeniería y dirección de obra. \n\n3.- instalación de central de energía fotovoltaica de en captación existente para el abastecimiento de agua potable del municipio de dólar, en la provincia de granada, incluyendo equipos auxiliares, equipos de medición, seguimiento, control y gestión energética, adecuación de la zona afectada por la actuación, así como desmontaje demolición, montaje en su caso de elementos existentes que fueran necesarios para el correcto funcionamiento de la captación de agua potable.\n\n4.- pruebas y puesta en funcionamiento de la nueva instalación.\n\n5.- certificado posterior de la actuación exigido en las actuaciones con cargo al fondo europeo de desarrollo regional, dentro del programa para el desarrollo energético sostenible de andalucía en el período 2017-2020.\n\nse emitirá un certificado (certificado previo) que se pronunciará sobre la viabilidad y eficacia de las medidas energéticas solicitadas para satisfacer las necesidades identificadas. una vez finalizada, se emitirá igualmente un nuevo certificado (certificado posterior) que refrende la eficacia y adecuación de las medidas ejecutadas para la mejora energética.\n\n', 'obras de la rehabilitación del antiguo colegio séneca para fines públicos, incluida en la Fondo Europeo de Desarrollo Regionaleración  Estrategia de Desarrollo Urbano Sostenible e Integrado Fondo Europeo de Desarrollo Regional 4.2.2, 6.1.1, 6.2.2 y 6.3.2 de la Estrategia de Desarrollo Urbano Sostenible e Integrado de palma del río… la ciudad que avanza, cofinanciada por la unión eurFondo Europeo de Desarrollo Regionalea a través del fondo eurFondo Europeo de Desarrollo Regionaleo de desarrollo regional (Operación), eje 12 del programa Fondo Europeo de Desarrollo Regionalerativo plurirregional de españa 2014-2020', 'el objeto del contrato viene motivado por la adecuación y puesta en uso del edificio b como centro social, dependiente de la junta municipal de distrito de san blas canillejas. hasta la fecha, este edificio lleva varios años sin funcionamiento y presenta un grado de deterioro considerable, careciendo de las medidas de accesibilidad necesarias para su uso público. ante tal situación y con el fin de evitar que el espacio sea ocupado y vandalizado, el objetivo principal de la junta municipal de san blas-canillejas es volver a ponerlo en uso, reconvirtiéndolo en un centro social. para ello los servicios técnicos de la junta municipal de distrito han llevado a cabo una reforma parcial de las instalaciones interiores, no alcanzando con ellas a cubrir el total de las necesarias para la puesta en uso del edificio b.\ncon el presente contrato, la empresa municipal de la vivienda y suelo de madrid pretende llevar a cabo las obras de instalación del ascensor de tal manera que se pueda garantizar el uso del edifico en condiciones de accesibilidad universal. para ello, se prevé la instalación de un ascensor anexo a la fachada testera orientada al oeste, para lo que será necesaria la demolición parcial de esa misma fachada. la instalación no afecta a la estructura del edificio ni a su distribución funcional. para la correcta instalación del ascensor se ha redactado por el departamento de rehabilitación de la Empresa Municipal de la Vivienda y Suelo de Madrid, proyecto de ejecución para la instalación de ascensor, de acuerdo a la normativa técnica y administrativa de aplicación\n']</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>['servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales', 'realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'servicio y suministro para el mantenimiento del alumbrado público, de edificios e instalaciones en general y para fiestas y actos culturales del ayuntamiento de santoña, con el fin de conservar las instalaciones en perfecto estado, manteniendo el nivel técnico alcanzado, minimizar los posibles riesgos a las personas, cosas o animales, incluyendo el servicio de control y funcionamiento, tanto de las instalaciones existentes, como de aquellas otras que se efectúen durante la vigencia del contrato, con arreglo a las condiciones que en su caso se señalen.\n\nel ámbito de aplicación de este contrato, se extiende a todos las instalaciones eléctricas que el ayuntamiento tiene para alumbrado público, iluminación artística además del mantenimiento de las instalaciones eléctricas de los edificios, oficinas y pabellones municipales.\n']</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>['Peatonalización blanda de la calle Miguel de Cervantes de Torre Pacheco para desarrollar la línea 2 de su EDUSI. cofinanciado por el Fondo Europeo de Desarrollo Regional en el marco del programa operativo FEDER 2014-2020 pluriregional de España.\r\n', 'Dentro de las inversiones en locales previstas en el C.C. Los Cipreses en Salamanca, se debe adaptar los locales para su comercialización, para que cumplan las necesidades del arrendatario. Los trabajos a realizar para ejecutar la nueva fachada son los siguientes:\n- Desmontaje de dos cierres metálicos existentes.\n- Instalación de carpinterías fijas de aluminio I/vidrio\n- Instalación de cierre enrollable de lamas de chapa de acero galvanizado con equipo de motorización\n- Trabajos de reparación y pintura en tabique de pladur existente e instalación de nueva puerta de paso de chapa lacada.', 'Alumbrado Inteligente en el Parque del Príncipe, Proyecto Red URBANSOL. Programa de Cooperación Interreg V A España-Portugal, (POCTEP 2014-2020).']</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>['Obras de mejora de movilidad y accesibilidad de la Travesía Postas de Soria.\nEsta Obra está destinada a la Estrategia DUSI Soria Intramuros, en los\nObjetivos Específicos 4.5.1 "Fomento de estrategias de reducción del carbono para\ntodo tipo de territorio, especialmente las zonas urbanas, incluido el fomento de la\nmovilidad urbana multimodal sostenible y las medidas de adaptación con efecto\nmitigación" y OE 6.5.2 “Acciones integradas de revitalización de ciudades, de\nmejora del entorno urbano y su medio ambiente”; dentro de las Líneas de Actuación\nLA 5 "Promoción de la Movilidad Urbana Sostenible, ciudad habitable y peatonal",\nLA 10 “Plan Conecta en Verde Soria Intramuros” y LA11 “Programa Recupera Soria:\nRehabilitación de espacios degradados e infrautilizados”; está cofinanciado al 50%\npor el Fondo Europeo de Desarrollo Regional (FEDER) de la Unión Europea, en el\nPrograma Operativo Plurirregional de España del periodo de programación 2014-\n2020, incluido en el Eje 12: Desarrollo Urbano.', 'Obras consistentes en la Mejora de\nmovilidad y accesibilidad Esta Obra está destinada a la Estrategia DUSI Soria Intramuros, en los\nObjetivos Específicos 4.5.1 "Fomento de estrategias de reducción del carbono para\ntodo tipo de territorio, especialmente las zonas urbanas, incluido el fomento de la\nmovilidad urbana multimodal sostenible y las medidas de adaptación con efecto\nmitigación" y OE 6.5.2 “Acciones integradas de revitalización de ciudades, de\nmejora del entorno urbano y su medio ambiente”; dentro de las Líneas de Actuación\nLA 5 "Promoción de la Movilidad Urbana Sostenible, ciudad habitable y peatonal",\nLA 10 “Plan Conecta en Verde Soria Intramuros” y LA11 “Programa Recupera Soria:\nRehabilitación de espacios degradados e infrautilizados”; está cofinanciado al 50%\npor el Fondo Europeo de Desarrollo Regional (FEDER) de la Unión Europea, en el\nPrograma Operativo Plurirregional de España del periodo de programación 2014-\n2020, incluido en el Eje 12: Desarrollo Urbano.de las calles Sorovega Y POSTAS DE Soria - FASE 1', 'Contrato de Obras consistente en la REDACCIÓN DE PROYECTO Y EJECUCIÓN DE OBRAS DE LA ESTRATEGIA INTEGRADA DE DESARROLLO SOSTENIBLE “AYAMONTE MIRA AL RÍO” (comprendiendo redacción de Proyecto Básico y de Ejecución, Estudio de Seguridad y Salud, Ensayos, Dirección de Obra, Dirección de Ejecución de Obra y Coordinación de Seguridad y Salud  y ejecución de las obras) correspondientes a las líneas de actuación (la3) Ayamonte se mueve, (la4) Desarrollo y conexión del carril bici para una movilidad más sostenible, (la5) Optimización de la eficiencia energética en las infraestructuras, equipamiento y servicios públicos, y (la6) Programa de Rehabilitación de espacios públicos degradados y recuperación de áreas para zonas verdes. Muelle de Portugal, desarrolladas cada una ellas en el Pliego de Prescripciones Técnicas, enmarcadas en la Estrategia de Desarrollo Urbano Sostenible Integrado (EDUSI), cofinanciadas por el Fondo Europeo de Desarrollo Regional en un 80%, en el marco del Programa Operativo de Crecimiento Sostenible FEDER 2014-2020, actual Programa Operativo Pluriregional de España.']</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>['Pavimentación de los siguientes caminos municipales: 1.- Acceso a Remesar 1; 2.- Acceso a Remesar 2; 3.- Camino del límite municipal a la LU-611 por Portaxe; 4.- Camino de la LU-611 la La Reina; 5.- Camino de la LU-0903 a la LU-0905; 6.- Camino de la LU-0903 a Outeiro; 7.- Camino de Lamela a Ver; 8.- Camino de la Avda. Alfonso XIII a Camino del Canal; 9.- Camino de acceso a Ver; 10.- Camino de Ribas Pequeñas a Chorente; 11.- Camino de Acceso a Guntín y 12.- Camino de Vilaboa a Xulián', 'Obras para la reparación de los siguientes caminos: Camino de los Furtivos, Camino de la Cebadilla al Porche de Alfredo, Camino Majadales, Camino de la Raña del Quinto, Camino de Portejuelo al Morrillo, Camino de las Navas 1, Camino de las Navas 2, Camino Miraflores, Camino Rubiastro, Camino las Larguillas y Camino Posada de Aguedillo.', 'Mejora de la capa de rodaje de los caminos: Lote 1: camino en Señorín (Camanzo), camino en Cirela (Gres), camino en Lareo (Salgueiros), caminos en Pastoriza (Carbia), caminos en Fondevila y Los Maestros (Bascuas) y camino en Obra (Santomé de Obra). Lote 2: camino en Oirós, camino en Castro (Besexos), Rúa Covas y Rúa Pendiente (Las Cruces), camino en Loño, camino en Outeiro (Portodemouros), en el Ayuntamiento de Vila de Cruces. ']</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>0.4812789559364319</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.4034287730852763</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.4607601463794708</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.4743659496307373</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>8</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>['renovación', 'pavimentación', 'saneamiento', 'red_abastecimiento', 'municipal', 'tramo', 'red_saneamiento', 'servicio', 'municipio', 'sustitución', 'pluvial', 'fase', 'canalización', 'colector', 'redactado']</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Municipal Infrastructure Improvement Project</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>3</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>['calle', 'obras', 'renovación', 'pavimentación', 'tramo', 'red', 'plaza', 'avenida', 'urbanización', 'saneamiento', 'zona', 'municipio', 'proyecto', 'red_abastecimiento', 'mejorar']</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Urban Infrastructure Improvement Project</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>['Servicio de albañilería, carpintería, revestimientos y trabajos de fontanería y saneamiento para el mantenimiento de los Ed. Administrativos Municipales', 'Obras necesarias para proceder a la reurbanización de Calle La Paja, entre Horquilleros y Villeta de Monda (Málaga).\n(Plan de Reactivación Económica Municipal 2020)', 'Contrato de obras para la ejecución del proyecto aconidicionamiento de les Escoletes Municipals  (PMEEN)']</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>['es objeto del presente contrato, por procedimiento abierto simplificado, tramitación ordinaria,\na través de varios criterios, la ejecución de las obras de renovación del pavimento e\ninstalaciones de varias viales públicas en suelo urbano consolidado del casco antiguo del\nnúcleo urbano de ibeas de juarros (burgos) dado el mal estado actual de las mismas por falta\nde mantenimiento y las adversas condiciones climatológicas de la zona.\nla actuación propuesta consistirá en un acabado uniforme de la pavimentación y de la\nurbanización de la red viaria del casco antiguo, en concreto para las calles la iglesia y san\nmiguel, zona del edificio de emiliano aguirre, incremento isleta n-120, dentro de la sobriedad\nde las soluciones empleadas, fijando las pautas globales a seguir en posteriores actuaciones\nde sustitución, conservación y reparación de la urbanización; así como en la renovación de las\nredes de abastecimiento de agua potable y saneamiento existentes, en concreto:\n\uf0b7 sustitución total de la pavimentación con nueva disposición de calzadas y aceras en\nlas calles indicadas.\n\uf0b7 sustitución, ampliación y refuerzo de las conducciones de distribución y evacuación\nanticuadas en los tramos de sustitución de pavimentación con ejecución de acometidas\ndomiciliarias y en los tramos de recuperación de firme de calzada con la conexión de\nlas acometidas existentes, además de reforma saneamiento c/soto y rejilla sumidero\nen la c/yacimientos arqueológicos.\n\uf0b7 colocación de canalizaciones para cableado de electricidad y alumbrado y\ntelecomunicaciones para sustitución de tendidos aéreos en las zonas de sustitución\ntotal de la pavimentación', 'el presente proyecto tiene por objeto la descripción de las actuaciones y obras a realizar para la urbanización de una\nparte de los viales que se hallan en el ámbito del plan especial, ubicada en el norte de la localidad de albocàsser.\ndicho vial complementara los ya realizados con anterioridad.\ndicho vial contará con una capa de rodadura y una zona peatonal. las instalaciones contará con los servicios de\nalumbrado realizado con luminarias solares, red de agua potable para completar un anillo y así minimizar el deterioro\nde la red existente, red de saneamiento y telecomunicaciones. estas obras son necesarias para la futura construcción\nde los equipamientos previstos en el área.\nse redacta el presente proyecto en aplicación de la ordenanza reguladora del plan provincial de obras y servicios\n(inversiones) castelló avança. es de especial relevancia la aplicación de criterior relacionados con los ods. en\nconcreto con los siguientes:\nobjetivo 6. agua limpia y saneamiento:\n1. renovación o nueva implantación de redes de distribución y abastecimiento de agua potable:\na) sustitución de canalizaciones existentes con el objeto de reducir pérdidas en la red, eliminar materiales obsoletos o corregir deficiencias\n2. renovación o nueva implantación de redes de saneamiento o recogida de aguas pluviales:\ng) en general, cualquier actuación destinada a la optimización y mejora de la eficiencia en el funcionamiento de las redes de saneamiento o recogida\nde aguas pluviales municipales.\nobjetivo 7. energía asequible y no contaminante\n1. mejora de la eficiencia energética en alumbrado público:\nb) instalación de luminarias que se abastezcan de energía solar.', 'renovación de redes de saneamiento y abastecimiento y posterior pavimentación con adoquín de hormigón prefabricado de color y envejecido en la c/ jesús.\npavimentación con aglomerado asfáltico de la calle camino viejo de las huelgas, así como renovación de la acera existente, al inicio de la calle, con baldosa.\nrenovación parcial de un tramo del saneamiento de la c/ palazuelos en la urb. parque jardín..pavimentación con aglomerado asfáltico de las calles san lázaro y atanzón.pavimentación con aglomerado asfáltico del aparcamiento situado junto a la biblioteca municipal y pavimentación parcial de un tramo de la calle superior barranquillo. pavimentación de un aparcamiento de caravanas con aglomerado asfáltico en la calle camino de la isla 51, y canalizaciones previstas para su servicio. instalación de mobiliario urbano de diferentes tipos similar al existente en varias zonas del municipio en el municipio de siguenza']</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>['servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales', 'realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'servicio y suministro para el mantenimiento del alumbrado público, de edificios e instalaciones en general y para fiestas y actos culturales del ayuntamiento de santoña, con el fin de conservar las instalaciones en perfecto estado, manteniendo el nivel técnico alcanzado, minimizar los posibles riesgos a las personas, cosas o animales, incluyendo el servicio de control y funcionamiento, tanto de las instalaciones existentes, como de aquellas otras que se efectúen durante la vigencia del contrato, con arreglo a las condiciones que en su caso se señalen.\n\nel ámbito de aplicación de este contrato, se extiende a todos las instalaciones eléctricas que el ayuntamiento tiene para alumbrado público, iluminación artística además del mantenimiento de las instalaciones eléctricas de los edificios, oficinas y pabellones municipales.\n']</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>['Servicio Mtto. Y Conservación De Edificios Y Sus Instalaciones Así Como De Accesos, Aparcam., Urbanizac. Y Área De Movimiento Del Recinto Aeroportuari', 'Urbanización de cl. san Jose en el marco de la convocatoria para la ejecución de obras comprendidas entre los objetivos de desarrollo sostenbile "reactivem castelló" obres ejercicio 2021.La obra pretende integrar la pavimentación ordenada que se ha llevado a cabo\nen Forcall, mediante adoquines de Hormigón tomados con arena, sobre una base de Hormigón HN 150. La obra permite restituir las trapas particulares de alcantarillado y agua potable, sustituyéndolas por trapas de fundición de mejor durabilidad y que quedan integradas en el pavimento. La obra permitirá la sustitución de un tramo de conducto de saneamiento entre los pozos de la C/ Tomas Salvador y viviendas de la C/ Sant Josep , con el fin de adecuar la red de saneamiento.', 'Obras de demolición por emergencia- ruina física inminente y urgente demolición forzosa de la construcción sita en el lago, nº 81 y 83, turón, (mieres), referencias catastrales:8382502tn7888s0001kd y 8382503tn7888s0001rd expte. 2021/6617 urbanismo']</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>['Contrato de obra de asfaltado viarios públicos, renovación de aceras y carril bici:\n(1) Asfaltado Calle Vicente Soriano – calle Cementerio, calle Pobla de Farnals, calle San Isidro (tramo entre calle Bobalar y Diputación Provincial), calle Mártires (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Rei en Jaume (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Camí Fondo (tramo entre la avenida Sant Pere y la calle Sagunto), av. Sant Pere este (tramo parcial entre calle Camí Fondo y José Mª Llopis), av. Sant Pere este (tramo parcial entre calle José Mª Llopis y Comunidad Valenciana) y calle Castellón (tramo entre calle José Mª Llopis y Comunidad Valenciana).\n(2) Renovación de la acera oeste de la calle Mártires y la calle Vicente Soriano lado barranco y la nueva ejecución de la acera norte y oeste del polideportivo Paco Camarasa (calle Vicente Soriano y calle del Cementerio). \n(3) Carril bici en el lado barranco de la calle Vicente Soriano.', 'El objeto del contrato al que se refiere el presente pliego, es devolver las características fundamentales como son la resistencia , seguridad y comodidad de un pavimento para tráfico rodado, las cuales se van perdiendo con el envejecimiento del firme, provocando un gran número de intervenciones de bacheo, con el consiguiente aumento del coste de mantenimiento, sin que estas operaciones consigan obtener resultados positivos cuando la superficie a bachear es superior a la del pavimento primitivo. Es por todo ello por lo que se decide actuar sobre dicho pavimento con una solución de tipo preventivo y aplicable a toda la superficie de una calle, o de forma parcial. En el Anexo al Proyecto, se detallan el listado de las calles que son objeto del presente proyecto, con su medición. Calles: Calle Santa María del Pino, Calle Nueva Jarilla, Calle Madrid, Calle Plaza el Roble, Calle Manzano, Calle Covidehur, Calle Miguel de Unamuno, Calle Sepúlveda, Calle Duero, Calle Dámaso Alonso, Calle Violeta, Calle Guadalcacín-La Rosa.', 'Reurbanización de varias calles del casco urbano de Godelleta: Calle Ramón y Cajal, Carretera de Buñol, Calle Siete Aguas, Calle Jacinto Benavente, Calle Salvador Ferrandis, Calle Maestro Serrrano, Calle Arturo Baynes, Calle Vicente Moreno, Calle Juan Ramón Jiménez, Calle Doctor Fleming, Calle Chiva, Avenida Vicente Lassala, Calle Comunidad Valenciana']</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>['Pavimentación de los siguientes caminos municipales: 1.- Acceso a Remesar 1; 2.- Acceso a Remesar 2; 3.- Camino del límite municipal a la LU-611 por Portaxe; 4.- Camino de la LU-611 la La Reina; 5.- Camino de la LU-0903 a la LU-0905; 6.- Camino de la LU-0903 a Outeiro; 7.- Camino de Lamela a Ver; 8.- Camino de la Avda. Alfonso XIII a Camino del Canal; 9.- Camino de acceso a Ver; 10.- Camino de Ribas Pequeñas a Chorente; 11.- Camino de Acceso a Guntín y 12.- Camino de Vilaboa a Xulián', 'Obras para la reparación de los siguientes caminos: Camino de los Furtivos, Camino de la Cebadilla al Porche de Alfredo, Camino Majadales, Camino de la Raña del Quinto, Camino de Portejuelo al Morrillo, Camino de las Navas 1, Camino de las Navas 2, Camino Miraflores, Camino Rubiastro, Camino las Larguillas y Camino Posada de Aguedillo.', 'Mejora de la capa de rodaje de los caminos: Lote 1: camino en Señorín (Camanzo), camino en Cirela (Gres), camino en Lareo (Salgueiros), caminos en Pastoriza (Carbia), caminos en Fondevila y Los Maestros (Bascuas) y camino en Obra (Santomé de Obra). Lote 2: camino en Oirós, camino en Castro (Besexos), Rúa Covas y Rúa Pendiente (Las Cruces), camino en Loño, camino en Outeiro (Portodemouros), en el Ayuntamiento de Vila de Cruces. ']</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>0.4820087750752767</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.4267442524433136</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.4732866783936818</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.4248956839243571</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>['calle', 'obras', 'edificio', 'municipal', 'construcción', 'contrato', 'sito', 'urbanización', 'rehabilitación', 'situado', 'parcela', 'acondicionamiento', 'proyecto', 'centro', 'fase']</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Urban Development Project Analysis</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>[{'document_id': 8452, 'sentence': 'Plan Cohesiona 2023', 'score': 0.3572709262371063, 'original_document': 'Contrato de Obra de mejoras viarias c/ Gabriel y Galán, Luís Chamizo y aledañas. Plan Cohesiona 2023'}, {'document_id': 2889, 'sentence': 'Plan Cohesiona 2020', 'score': 0.3512280285358429, 'original_document': 'Obra de Mejoras Infraestructuras en Obando: c/ Alba, c/ Ronda Saliente y c/ San Jose. Plan Cohesiona 2020'}, {'document_id': 1540, 'sentence': 'Insp', 'score': 0.34550508856773376, 'original_document': 'Insp. Periodica Baja tension ETAP'}]</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>['El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.', 'El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.', 'El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.']</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>['El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.', 'El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.', 'El objeto del contrato es el mantenimiento y actualización de los contenidos digitales que el teatro arriaga publica en cada uno de sus canales de comunicación.']</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>[{'document_id': 13766, 'sentence': ', Urbanizac', 'score': 0.5680121779441833, 'original_document': 'Servicio Mtto. Y Conservación De Edificios Y Sus Instalaciones Así Como De Accesos, Aparcam., Urbanizac. Y Área De Movimiento Del Recinto Aeroportuari'}, {'document_id': 9457, 'sentence': '2021/6617 urbanismo', 'score': 0.4923281967639923, 'original_document': 'Obras de demolición por emergencia- ruina física inminente y urgente demolición forzosa de la construcción sita en el lago, nº 81 y 83, turón, (mieres), referencias catastrales:8382502tn7888s0001kd y 8382503tn7888s0001rd expte. 2021/6617 urbanismo'}, {'document_id': 4237, 'sentence': 'Urbanización de cl', 'score': 0.48859721422195435, 'original_document': 'Urbanización de cl. san Jose en el marco de la convocatoria para la ejecución de obras comprendidas entre los objetivos de desarrollo sostenbile "reactivem castelló" obres ejercicio 2021.La obra pretende integrar la pavimentación ordenada que se ha llevado a cabo\nen Forcall, mediante adoquines de Hormigón tomados con arena, sobre una base de Hormigón HN 150. La obra permite restituir las trapas particulares de alcantarillado y agua potable, sustituyéndolas por trapas de fundición de mejor durabilidad y que quedan integradas en el pavimento. La obra permitirá la sustitución de un tramo de conducto de saneamiento entre los pozos de la C/ Tomas Salvador y viviendas de la C/ Sant Josep , con el fin de adecuar la red de saneamiento.'}]</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>['Contrato de obra de asfaltado viarios públicos, renovación de aceras y carril bici:\n(1) Asfaltado Calle Vicente Soriano – calle Cementerio, calle Pobla de Farnals, calle San Isidro (tramo entre calle Bobalar y Diputación Provincial), calle Mártires (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Rei en Jaume (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Camí Fondo (tramo entre la avenida Sant Pere y la calle Sagunto), av. Sant Pere este (tramo parcial entre calle Camí Fondo y José Mª Llopis), av. Sant Pere este (tramo parcial entre calle José Mª Llopis y Comunidad Valenciana) y calle Castellón (tramo entre calle José Mª Llopis y Comunidad Valenciana).\n(2) Renovación de la acera oeste de la calle Mártires y la calle Vicente Soriano lado barranco y la nueva ejecución de la acera norte y oeste del polideportivo Paco Camarasa (calle Vicente Soriano y calle del Cementerio). \n(3) Carril bici en el lado barranco de la calle Vicente Soriano.', 'El objeto del contrato al que se refiere el presente pliego, es devolver las características fundamentales como son la resistencia , seguridad y comodidad de un pavimento para tráfico rodado, las cuales se van perdiendo con el envejecimiento del firme, provocando un gran número de intervenciones de bacheo, con el consiguiente aumento del coste de mantenimiento, sin que estas operaciones consigan obtener resultados positivos cuando la superficie a bachear es superior a la del pavimento primitivo. Es por todo ello por lo que se decide actuar sobre dicho pavimento con una solución de tipo preventivo y aplicable a toda la superficie de una calle, o de forma parcial. En el Anexo al Proyecto, se detallan el listado de las calles que son objeto del presente proyecto, con su medición. Calles: Calle Santa María del Pino, Calle Nueva Jarilla, Calle Madrid, Calle Plaza el Roble, Calle Manzano, Calle Covidehur, Calle Miguel de Unamuno, Calle Sepúlveda, Calle Duero, Calle Dámaso Alonso, Calle Violeta, Calle Guadalcacín-La Rosa.', 'El presente contrato tiene por objeto establecer acometer las obras  de “Pavimentación. “Carrer Saboneria” y “Carrer Botera” del municipio de Vilanova d’Alcolea / 12183, mediando Plan de Cooperación Provincial de Obras y Servicios de la Diputación Provincial para el año 2021 (Plan Castellón 135-2021), con número de expediente municipal 140/2021, de conformidad con el Proyecto de obras suscrito por el Arquitecto Vicente Pañego, colegiado COACV 08.087, conforme al artículo 13 LCSP de 2017.\nLa actuación pretendida viene motivada por la necesidad de poner el valor el Casco Antiguo de Vilanova d’Alcolea, se pretende acometer las obras de renovación y mejora del pavimento de las calles indicadas en el párrafo anterior.\n\n\tLa intervención consiste en la renovación y mejora del pavimento de las Calle Saboneria y Botera. Todo ello, se concreta adoptando la solución que se adoptó en la Calle Mayor, para ello se adopta una sección transversal tipo en las calles en las que se distinguen:\nUna franja longitudinal de 40 cm de anchura pegada a las fachadas y en ambos lados de la calle.\nUna franja central de 30 cm de anchura en el eje de la calle\nEl resto de calle se completará con adoquines de piedra granítica con ancho variable en cada punto de las calles.\n\n\tLa solución adoptada se plantea en plataforma única con pendiente de desagüe al centro de la calle.\nSe sustituirán las tapas de agua potable y de saneamiento, así como la de los pozos de registro.']</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>['Contrato de obra de asfaltado viarios públicos, renovación de aceras y carril bici:\n(1) Asfaltado Calle Vicente Soriano – calle Cementerio, calle Pobla de Farnals, calle San Isidro (tramo entre calle Bobalar y Diputación Provincial), calle Mártires (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Rei en Jaume (tramo entre calle José Mª Llopis y Comunidad Valenciana), calle Camí Fondo (tramo entre la avenida Sant Pere y la calle Sagunto), av. Sant Pere este (tramo parcial entre calle Camí Fondo y José Mª Llopis), av. Sant Pere este (tramo parcial entre calle José Mª Llopis y Comunidad Valenciana) y calle Castellón (tramo entre calle José Mª Llopis y Comunidad Valenciana).\n(2) Renovación de la acera oeste de la calle Mártires y la calle Vicente Soriano lado barranco y la nueva ejecución de la acera norte y oeste del polideportivo Paco Camarasa (calle Vicente Soriano y calle del Cementerio). \n(3) Carril bici en el lado barranco de la calle Vicente Soriano.', 'El objeto del contrato al que se refiere el presente pliego, es devolver las características fundamentales como son la resistencia , seguridad y comodidad de un pavimento para tráfico rodado, las cuales se van perdiendo con el envejecimiento del firme, provocando un gran número de intervenciones de bacheo, con el consiguiente aumento del coste de mantenimiento, sin que estas operaciones consigan obtener resultados positivos cuando la superficie a bachear es superior a la del pavimento primitivo. Es por todo ello por lo que se decide actuar sobre dicho pavimento con una solución de tipo preventivo y aplicable a toda la superficie de una calle, o de forma parcial. En el Anexo al Proyecto, se detallan el listado de las calles que son objeto del presente proyecto, con su medición. Calles: Calle Santa María del Pino, Calle Nueva Jarilla, Calle Madrid, Calle Plaza el Roble, Calle Manzano, Calle Covidehur, Calle Miguel de Unamuno, Calle Sepúlveda, Calle Duero, Calle Dámaso Alonso, Calle Violeta, Calle Guadalcacín-La Rosa.', 'El presente contrato tiene por objeto establecer acometer las obras  de “Pavimentación. “Carrer Saboneria” y “Carrer Botera” del municipio de Vilanova d’Alcolea / 12183, mediando Plan de Cooperación Provincial de Obras y Servicios de la Diputación Provincial para el año 2021 (Plan Castellón 135-2021), con número de expediente municipal 140/2021, de conformidad con el Proyecto de obras suscrito por el Arquitecto Vicente Pañego, colegiado COACV 08.087, conforme al artículo 13 LCSP de 2017.\nLa actuación pretendida viene motivada por la necesidad de poner el valor el Casco Antiguo de Vilanova d’Alcolea, se pretende acometer las obras de renovación y mejora del pavimento de las calles indicadas en el párrafo anterior.\n\n\tLa intervención consiste en la renovación y mejora del pavimento de las Calle Saboneria y Botera. Todo ello, se concreta adoptando la solución que se adoptó en la Calle Mayor, para ello se adopta una sección transversal tipo en las calles en las que se distinguen:\nUna franja longitudinal de 40 cm de anchura pegada a las fachadas y en ambos lados de la calle.\nUna franja central de 30 cm de anchura en el eje de la calle\nEl resto de calle se completará con adoquines de piedra granítica con ancho variable en cada punto de las calles.\n\n\tLa solución adoptada se plantea en plataforma única con pendiente de desagüe al centro de la calle.\nSe sustituirán las tapas de agua potable y de saneamiento, así como la de los pozos de registro.']</t>
-        </is>
+      <c r="B15" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>['plan_recuperación', 'municipal', 'resiliencia_financiado', 'plan_provincial', 'financiado', 'next_generation', 'resiliencia', 'incluido_plan', 'actuación', 'provincial', 'instalación', 'municipio', 'energío_fotovoltaico', 'generation_eu', 'zona']</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Financial Resilience and Energy Infrastructure Development Plan</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>8</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>['plan_recuperación', 'transformación_resiliencia', 'financiado_unión', 'desarrollo_rural', 'next_generation', 'eu', 'unión_europea', 'generation_eu', 'zona', 'actuación', 'proyecto', 'financiado', 'programa', 'incluido', 'recuperación_transformación']</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>European Union Recovery and Transformation Program</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>['Obras de urbanización de la nueva zona de bajas emisiones (zbe) la villa de Parla.\nPlan de recuperación, transformación y resiliencia de la economía.\nPrograma de ayudas a municipios para la implantación de zonas de bajas emisiones y la transformación digital y sostenible del transporte urbano.\nComponente 1, inversión 1 (c1.i1), medida: zonas de bajas emisiones y transformación digital y sostenible del transporte urbano y metropolitano, según anexo revisado de la decisión de ejecución del consejo, relativa a la aprobación de la evaluación del plan de recuperación y resiliencia de España.', 'Obras de proyecto de construcción de aparcamiento disuasorio sur estación de ADIF. Fase I del Proyecto conexión intermodal y aparcamientos disuasorios para el intercambiador Parla Norte (Estación ferroviaria cercanías, tranvía y autobús urbano e interurbano). Plan de recuperación, transformación y resiliencia de la economía. Programa de ayudas a municipios para la implantación de zonas de bajas emisiones y la transformación digital y sostenible del transporte urbano.\n', 'Obras necesarias para proceder a la reurbanización de Calle La Paja, entre Horquilleros y Villeta de Monda (Málaga).\n(Plan de Reactivación Económica Municipal 2020)']</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>['el objeto del contrato es la ejecución de las obras definidas en el proyecto de “reforma del inmueble situado al c/ garcia, 3 para destinarlo a oficinas municipales” del municipio de la figuera. este proyecto ha sido redactado por el equipo técnico de la unidad de arquitectura municipal del servicio de asistencia en el municipio (sam) de la diputación de tarragona. el autor del proyecto es jaume mutlló pàmies, jefe de la unidad de arquitectura municipal de la diputación de tarragona. este proyecto se redactó el noviembre del año 2022.\n\nel contrato que se licita deriva del citado proyecto, fue aprobado por el mitma (ministerio de transportes, movilidad y agenda urbana), en el marco de los fondos procedentes del plan de recuperación, transformación y resiliencia, se financiará con cargo a fondo del mecanismo de recuperación y resiliencia de la unión europea – next generation eu, en el marco del programa de impulso a la rehabilitación de los edificios públicos (pirep).\n\ncon este contrato se da cumplimiento a los objetivos generales de la política palanca 1 «agenda urbana y rural, lucha contra la despoblación y desarrollo de la agricultura» y, concretamente del componente 2 “plan de rehabilitación de vivienda y regeneración urbana”, la inversión 5, “programa de impulso a la rehabilitación de edificios públicos”, en el marco del plan de recuperación, transformación y resiliencia de la unión europea – next generation ue.\n', 'el objeto del contrato viene motivado por la adecuación y puesta en uso del edificio b como centro social, dependiente de la junta municipal de distrito de san blas canillejas. hasta la fecha, este edificio lleva varios años sin funcionamiento y presenta un grado de deterioro considerable, careciendo de las medidas de accesibilidad necesarias para su uso público. ante tal situación y con el fin de evitar que el espacio sea ocupado y vandalizado, el objetivo principal de la junta municipal de san blas-canillejas es volver a ponerlo en uso, reconvirtiéndolo en un centro social. para ello los servicios técnicos de la junta municipal de distrito han llevado a cabo una reforma parcial de las instalaciones interiores, no alcanzando con ellas a cubrir el total de las necesarias para la puesta en uso del edificio b.\ncon el presente contrato, la empresa municipal de la vivienda y suelo de madrid pretende llevar a cabo las obras de instalación del ascensor de tal manera que se pueda garantizar el uso del edifico en condiciones de accesibilidad universal. para ello, se prevé la instalación de un ascensor anexo a la fachada testera orientada al oeste, para lo que será necesaria la demolición parcial de esa misma fachada. la instalación no afecta a la estructura del edificio ni a su distribución funcional. para la correcta instalación del ascensor se ha redactado por el departamento de rehabilitación de la Empresa Municipal de la Vivienda y Suelo de Madrid, proyecto de ejecución para la instalación de ascensor, de acuerdo a la normativa técnica y administrativa de aplicación\n', '“reforma del complejo de escuelas y guarderia de\nalcazarén”en el marco del «plan de recuperación, transformación y resiliencia -\nfinanciado por la unión europea " next generation eu", c2.i5.\n\nen singular, el complejo educativo cuenta con cinco edificaciones\naisladas, siendo las de objeto de actuación el edificio destinado actualmente a guardería,\nlos bloques denominados b y c según proyecto que están destinados a aulas y el\nbloque a destinado en la actualidad a gimnasio y sala de profesores. todas las\nedificaciones son construcciones de los años 1950, que se encuentran en estado\naceptable pero bastante obsoleto siendo necesario acometer: mejora de envolvente\ntérmica (actuación tipo a), sostenibilidad ambiental (actuación tipo b),\naccesibilidad (actuación tipo c), habitabilidad (actuación tipo d),\nconservación de los edificios (actuación tipo d).']</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>['servicio de instalación de equipos básicos y opcionales de monitorización energética\nen instalaciones fotovoltaicas de diversos edificios e instalaciones municipales, así\ncomo el servicio de inversión sin cargo a ahorros para el suministro e instalación de\npantallas de visualización de datos de la producción fotovoltaica de diversos edificios e\ninstalaciones municipales. a través del presente contrato se procede a ejecutar el\nproyecto de inversión, con número de Plan Estratégico de Inversión: 2022/070204 “equipos de monitorización\npara instalaciones fotovoltaicas en dependencias municipales', 'realización de las obras necesarias para el suministro e instalación de un sistema de ventilación en el sótano del edificio sede de prodetur en calle leonardo da vinci nº 16 de sevilla.el presupuesto a aportar en este procedimiento de contratación deberá reunir las siguientes características técnicas: los equipos de ventilación proyectados serán de la marca ¿soler &amp;palau¿ modelo chat/4/560n o similar. la instalación de ventilación deberá estar controlada o automatizada mediante la instalación de detección de co y posibilitar la puesta en funcionamiento manualmente. la central de detección de co se instalará en el cuarto de instalaciones de la planta baja. la entrada y salida de aire a planta sótano se realizará a través de dos monolitos proyectados en planta baja en el exterior del edificio con rejillas de ventilación. todas aquellas actuaciones que sean necesarias realizar en las instalaciones o revestimientos existentes en el edificio correrán a cargo de la empresa contratista y, una vez finalizada la instalación de ventilación, deberán ser retornados a su estado original de partida por la empresa contratista, comprobando el correcto funcionamiento de todas ellas. se adjunta plano de la instalación propuesta. se adjunta medición de la instalación propuesta para su presupuestación.', 'servicio y suministro para el mantenimiento del alumbrado público, de edificios e instalaciones en general y para fiestas y actos culturales del ayuntamiento de santoña, con el fin de conservar las instalaciones en perfecto estado, manteniendo el nivel técnico alcanzado, minimizar los posibles riesgos a las personas, cosas o animales, incluyendo el servicio de control y funcionamiento, tanto de las instalaciones existentes, como de aquellas otras que se efectúen durante la vigencia del contrato, con arreglo a las condiciones que en su caso se señalen.\n\nel ámbito de aplicación de este contrato, se extiende a todos las instalaciones eléctricas que el ayuntamiento tiene para alumbrado público, iluminación artística además del mantenimiento de las instalaciones eléctricas de los edificios, oficinas y pabellones municipales.\n']</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>['39-O-6260 54.833/21. Actuaciones contra el ruido en la Autovía AI-81, de acceso a Avilés. Provincia: Asturias. Plan de Recuperación, Transformación y Resiliencia Financiado por la Unión Europea Next Generation EU', '52-MA-4980 Proyecto de Adecuación Túneles Churriana y San Pedro. Provincia de Malaga. Plan de recuperación, transformación y resiliencia financiado por la Unión Europea Next Generation EU.', '39-B-50195; 54.634/22 Medidas correctoras acústicas a implantar en la salida Este de los Túneles de Vallirana. Autovía B-24. T. M. de Vallirana. Provincia de Barcelona.  Plan de Recuperación, Transformación y Resiliencia financiado por la Unión Europea NEXT GENERATION EU']</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>['El objeto del contrato es la ejecución de las obras definidas en el proyecto de “Reforma del inmueble situado al c/ Garcia, 3 para destinarlo a oficinas municipales” del municipio de la Figuera. Este proyecto ha sido redactado por el equipo técnico de la Unidad de Arquitectura Municipal del Servicio de Asistencia en el Municipio (SAM) de la Diputación de Tarragona. El autor del proyecto es Jaume Mutlló Pàmies, jefe de la Unidad de Arquitectura Municipal de la Diputación de Tarragona. Este proyecto se redactó el noviembre del año 2022.\n\nEl contrato que se licita deriva del citado proyecto, fue aprobado por el MITMA (Ministerio de Transportes, Movilidad y Agenda Urbana), en el marco de los fondos procedentes del Plan de Recuperación, Transformación y Resiliencia, se financiará con cargo a fondo del Mecanismo de Recuperación y Resiliencia de la Unión Europea – Next Generation EU, en el marco del programa de impulso a la rehabilitación de los edificios públicos (PIREP).\n\nCon este contrato se da cumplimiento a los objetivos generales de la Política Palanca 1 «Agenda urbana y rural, lucha contra la despoblación y desarrollo de la agricultura» y, concretamente del Componente 2 “Plan de Rehabilitación de vivienda y Regeneración Urbana”, la Inversión 5, “Programa de Impulso a la Rehabilitación de Edificios Públicos”, en el marco del Plan de Recuperación, Transformación y Resiliencia de la Unión Europea – Next Generation UE.\n', 'Ejecución de las obras consistes en “PACIFICACIÓN DE LOS TRAMOS DE LAS CALLES ALFONSO VIII, AVENIDA DE NAVARRA Y LINAJES, ALEDAÑAS A LA ZONA DE BAJAS EMISIONES (ZBE) DE LA CIUDAD DE SORIA”\nEl presente contrato está financiado por el Plan de Recuperación, Transformación y Resiliencia – Financiado por la Unión Europea – NextGenerationEU, con cargo al Programa de ayudas a municipios para la implantación de zonas de bajas emisiones y la transformación digital y sostenible del Transporte Urbano, convocado por el Ministerio de Transportes Movilidad y Agenda Urbana, Orden TMA/892/2021. Inversión 1 de la componente 1 del Plan de Recuperación, Transformación y Resiliencia.', 'Ejecución de las obras consistes en\n“Ampliación del aparcamiento disuasorio/ pacificación de la calle Doctrina”.El presente contrato está financiado por el Plan de\nRecuperación, Transformación y Resiliencia – Financiado por la Unión Europea –\nNextGenerationEU, con cargo al Programa de ayudas a municipios para la\nimplantación de zonas de bajas emisiones y la transformación digital y sostenible del\nTransporte Urbano, convocado por el Ministerio de Transportes Movilidad y Agenda\nUrbana, Orden TMA/892/2021. Inversión 1 de la componente 1 del Plan de\nRecuperación, Transformación y Resiliencia.\n\n']</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>['Pavimentación de los siguientes caminos municipales: 1.- Acceso a Remesar 1; 2.- Acceso a Remesar 2; 3.- Camino del límite municipal a la LU-611 por Portaxe; 4.- Camino de la LU-611 la La Reina; 5.- Camino de la LU-0903 a la LU-0905; 6.- Camino de la LU-0903 a Outeiro; 7.- Camino de Lamela a Ver; 8.- Camino de la Avda. Alfonso XIII a Camino del Canal; 9.- Camino de acceso a Ver; 10.- Camino de Ribas Pequeñas a Chorente; 11.- Camino de Acceso a Guntín y 12.- Camino de Vilaboa a Xulián', 'Obras para la reparación de los siguientes caminos: Camino de los Furtivos, Camino de la Cebadilla al Porche de Alfredo, Camino Majadales, Camino de la Raña del Quinto, Camino de Portejuelo al Morrillo, Camino de las Navas 1, Camino de las Navas 2, Camino Miraflores, Camino Rubiastro, Camino las Larguillas y Camino Posada de Aguedillo.', 'Mejora de la capa de rodaje de los caminos: Lote 1: camino en Señorín (Camanzo), camino en Cirela (Gres), camino en Lareo (Salgueiros), caminos en Pastoriza (Carbia), caminos en Fondevila y Los Maestros (Bascuas) y camino en Obra (Santomé de Obra). Lote 2: camino en Oirós, camino en Castro (Besexos), Rúa Covas y Rúa Pendiente (Las Cruces), camino en Loño, camino en Outeiro (Portodemouros), en el Ayuntamiento de Vila de Cruces. ']</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
+        <v>0.4398381312688192</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.4535448749860128</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.4800822635491689</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.3893087108929952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>